<commit_message>
update results of using trust-region method
to solve continuous relaxation with tv regularizer
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92BEF278-45EB-2143-A2E6-5DDBC54AD371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B53CD59-EC4C-414B-8153-9BC15775082D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -184,27 +184,18 @@
     <t>Switching time+Minup</t>
   </si>
   <si>
-    <t>GRAPE+TR</t>
-  </si>
-  <si>
     <t>GRAPE+TR+Minup</t>
   </si>
   <si>
     <t>GRAPE+TR+Maxswitch</t>
   </si>
   <si>
-    <t>ADMM+TR</t>
-  </si>
-  <si>
     <t>ADMM+TR+Minup</t>
   </si>
   <si>
     <t>ADMM+TR+Maxswitch</t>
   </si>
   <si>
-    <t>Switching+TR</t>
-  </si>
-  <si>
     <t>Switching+Minup</t>
   </si>
   <si>
@@ -212,6 +203,44 @@
   </si>
   <si>
     <t>time (s)</t>
+  </si>
+  <si>
+    <t>GRAPE+TR (binary)</t>
+  </si>
+  <si>
+    <t>ADMM+TR (binary)</t>
+  </si>
+  <si>
+    <t>Switching+TR (binary)</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>GRAPE+TR (continuous)</t>
+  </si>
+  <si>
+    <t>ADMM+TR (continuous)</t>
+  </si>
+  <si>
+    <t>solve continuous relaxation
+with TV norm starting from GRAPE</t>
+  </si>
+  <si>
+    <t>solve continuous relaxation
+with TV norm starting from ADMM</t>
+  </si>
+  <si>
+    <t>SNOPT</t>
+  </si>
+  <si>
+    <t>continuous results</t>
+  </si>
+  <si>
+    <t>IPOPT</t>
   </si>
 </sst>
 </file>
@@ -219,7 +248,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -252,7 +281,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -576,19 +605,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="120.5" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -605,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -659,413 +688,488 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D4">
         <v>-0.999</v>
       </c>
       <c r="E4">
-        <v>54</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="F4" s="1">
         <f>D4+E4*0.01</f>
-        <v>-0.45899999999999996</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
+        <v>-0.99333000000000005</v>
+      </c>
+      <c r="G4">
+        <v>1.77</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D5">
-        <v>-0.84099999999999997</v>
+        <v>-0.999</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="F5" s="1">
         <f>D5+E5*0.01</f>
-        <v>-0.80099999999999993</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
+        <v>-0.99377000000000004</v>
+      </c>
+      <c r="G5">
+        <v>0.09</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>-0.97099999999999997</v>
+        <v>-0.999</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1">
-        <f>D6+E6*0.01</f>
-        <v>-0.871</v>
+        <f t="shared" ref="F6:F15" si="0">D6+E6*0.01</f>
+        <v>-0.45899999999999996</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7">
-        <v>-0.999</v>
+        <v>-0.84099999999999997</v>
       </c>
       <c r="E7">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
-        <f>D7+E7*0.01</f>
-        <v>-0.51900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>-0.80099999999999993</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>-0.84599999999999997</v>
+        <v>-0.97099999999999997</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1">
-        <f>D8+E8*0.01</f>
-        <v>-0.78600000000000003</v>
+        <f t="shared" si="0"/>
+        <v>-0.871</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9">
-        <v>-0.97199999999999998</v>
+        <v>-0.999</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1">
-        <f>D9+E9*0.01</f>
-        <v>-0.872</v>
-      </c>
-      <c r="G9">
-        <v>0.01</v>
-      </c>
-      <c r="H9" s="3"/>
+        <f t="shared" si="0"/>
+        <v>-0.51900000000000002</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>-0.84599999999999997</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1">
-        <f>D10+E10*0.01</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.01</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>-0.78600000000000003</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11">
+        <v>-0.97199999999999998</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.872</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <f>D11+E11*0.01</f>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12">
-        <v>-0.997</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1">
-        <f>D12+E12*0.01</f>
-        <v>-0.89700000000000002</v>
-      </c>
       <c r="G12">
-        <v>3.41</v>
+        <v>0.01</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
       </c>
       <c r="D13">
-        <v>-0.996</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f>D13+E13*0.01</f>
-        <v>-0.91600000000000004</v>
-      </c>
-      <c r="G13">
-        <v>3.15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D14">
-        <v>-0.99399999999999999</v>
+        <v>-0.997</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" ref="F14:F20" si="0">D14+E14*0.01</f>
-        <v>-0.89400000000000002</v>
+        <f t="shared" si="0"/>
+        <v>-0.89700000000000002</v>
       </c>
       <c r="G14">
-        <v>4.84</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>28</v>
+        <v>3.41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>-0.997</v>
+        <v>-0.996</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.95699999999999996</v>
+        <v>-0.91600000000000004</v>
       </c>
       <c r="G15">
-        <v>2.2599999999999998</v>
+        <v>3.15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>-0.95899999999999996</v>
+        <v>-0.99399999999999999</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.89900000000000002</v>
+        <f t="shared" ref="F16:F22" si="1">D16+E16*0.01</f>
+        <v>-0.89400000000000002</v>
       </c>
       <c r="G16">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>4.84</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D17">
-        <v>-0.90900000000000003</v>
+        <v>-0.997</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.86899999999999999</v>
+        <f t="shared" si="1"/>
+        <v>-0.95699999999999996</v>
       </c>
       <c r="G17">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18">
-        <v>-0.97099999999999997</v>
+        <v>-0.95899999999999996</v>
       </c>
       <c r="E18">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.871</v>
+        <f t="shared" si="1"/>
+        <v>-0.89900000000000002</v>
       </c>
       <c r="G18">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19">
-        <v>-0.97199999999999998</v>
+        <v>-0.90900000000000003</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.872</v>
+        <f t="shared" si="1"/>
+        <v>-0.86899999999999999</v>
       </c>
       <c r="G19">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>-0.97099999999999997</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.871</v>
+      </c>
+      <c r="G20">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>-0.97199999999999998</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.872</v>
+      </c>
+      <c r="G21">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20">
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22">
         <v>-0.90900000000000003</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>4</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="0"/>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
         <v>-0.86899999999999999</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25">
+        <v>-0.91600000000000004</v>
+      </c>
+      <c r="H25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26">
+        <v>-0.91600000000000004</v>
+      </c>
+      <c r="G26">
+        <v>0.02</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="A2:A20"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="A2:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update results obtained from ampl
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B53CD59-EC4C-414B-8153-9BC15775082D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC251CC-1407-EB46-B124-09D81BC11028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>IPOPT</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_snopt</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_Ipopt</t>
   </si>
 </sst>
 </file>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,35 +1147,57 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C25" s="2" t="s">
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D25">
+      <c r="D23">
         <v>-0.91600000000000004</v>
       </c>
-      <c r="H25" t="s">
+      <c r="E23">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:F24" si="2">D23+E23*0.01</f>
+        <v>-0.90672000000000008</v>
+      </c>
+      <c r="H23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="C26" s="2" t="s">
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D26">
+      <c r="D24">
         <v>-0.91600000000000004</v>
       </c>
-      <c r="G26">
-        <v>0.02</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="E24">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.90672000000000008</v>
+      </c>
+      <c r="G24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H24" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H9:H11"/>
-    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="A2:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add cnot example without sos1 constriant
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC251CC-1407-EB46-B124-09D81BC11028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59044877-6E6D-2541-ACF9-C90668BAEDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1. update rounding function 2. update results for energy examples
3. update results for CNOT example without SOS1 property
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08122A2F-4CDD-FE46-B3AE-4C39DAA14B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79ABC5B-D762-BD48-9F2E-E9F88F91AA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -95,19 +95,6 @@
     <t>rounding results of ADMM</t>
   </si>
   <si>
-    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.0</t>
-  </si>
-  <si>
-    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.5</t>
-  </si>
-  <si>
-    <t>swithing time optimization results</t>
-  </si>
-  <si>
-    <t>swithing time optimization results
- with 10 minimum up time steps</t>
-  </si>
-  <si>
     <t>start from SUR results of GRAPE</t>
   </si>
   <si>
@@ -178,12 +165,6 @@
     <t>ADMM+Maxswitch</t>
   </si>
   <si>
-    <t>Switching time</t>
-  </si>
-  <si>
-    <t>Switching time+Minup</t>
-  </si>
-  <si>
     <t>GRAPE+TR+Minup</t>
   </si>
   <si>
@@ -217,23 +198,13 @@
     <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
   </si>
   <si>
-    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
-  </si>
-  <si>
     <t>GRAPE+TR (continuous)</t>
-  </si>
-  <si>
-    <t>ADMM+TR (continuous)</t>
   </si>
   <si>
     <t>solve continuous relaxation
 with TV norm starting from GRAPE</t>
   </si>
   <si>
-    <t>solve continuous relaxation
-with TV norm starting from ADMM</t>
-  </si>
-  <si>
     <t>SNOPT</t>
   </si>
   <si>
@@ -247,6 +218,36 @@
   </si>
   <si>
     <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_Ipopt</t>
+  </si>
+  <si>
+    <t>binary results</t>
+  </si>
+  <si>
+    <t>MINLP</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minlp</t>
+  </si>
+  <si>
+    <t>MUCOD_II</t>
+  </si>
+  <si>
+    <t>continuous results based on ODE</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_mucod2</t>
+  </si>
+  <si>
+    <t>GRAPE+TR+SUR</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc__maxswitch5</t>
   </si>
 </sst>
 </file>
@@ -291,13 +292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -649,13 +648,13 @@
     </row>
     <row r="2" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>-0.999</v>
@@ -677,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>-0.999</v>
@@ -698,10 +697,10 @@
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>-0.999</v>
@@ -717,237 +716,233 @@
         <v>1.77</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
       </c>
       <c r="D5">
         <v>-0.999</v>
       </c>
       <c r="E5">
-        <v>0.52300000000000002</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1">
-        <f>D5+E5*0.01</f>
-        <v>-0.99377000000000004</v>
-      </c>
-      <c r="G5">
-        <v>0.09</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F5:F15" si="0">D5+E5*0.01</f>
+        <v>-0.45899999999999996</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>-0.999</v>
+        <v>-0.84099999999999997</v>
       </c>
       <c r="E6">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F15" si="0">D6+E6*0.01</f>
-        <v>-0.45899999999999996</v>
+        <f t="shared" si="0"/>
+        <v>-0.80099999999999993</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
-        <v>8</v>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>-0.84099999999999997</v>
+        <v>-0.97099999999999997</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>-0.80099999999999993</v>
+        <v>-0.871</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>-0.97099999999999997</v>
+        <v>-0.999</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>-0.871</v>
+        <v>-0.51900000000000002</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>11</v>
+      <c r="H8" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9">
-        <v>-0.999</v>
+        <v>-0.84599999999999997</v>
       </c>
       <c r="E9">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.51900000000000002</v>
+        <v>-0.78600000000000003</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10">
-        <v>-0.84599999999999997</v>
+        <v>-0.97199999999999998</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.78600000000000003</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <f>D10+E10*0.01</f>
+        <v>-0.872</v>
+      </c>
+      <c r="G10">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D11">
-        <v>-0.97199999999999998</v>
+        <v>-0.995</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.872</v>
-      </c>
-      <c r="G11">
-        <v>0.01</v>
-      </c>
-      <c r="H11" s="3"/>
+        <f>D11+E11*0.01</f>
+        <v>-0.45499999999999996</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-0.84</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0.01</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F12:F13" si="1">D12+E12*0.01</f>
+        <v>-0.79999999999999993</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-0.96</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>22</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>-0.86</v>
+      </c>
+      <c r="G13">
+        <v>0.01</v>
+      </c>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>-0.997</v>
@@ -963,16 +958,16 @@
         <v>3.41</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>-0.996</v>
@@ -988,16 +983,16 @@
         <v>3.15</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>-0.99399999999999999</v>
@@ -1006,23 +1001,23 @@
         <v>10</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ref="F16:F22" si="1">D16+E16*0.01</f>
+        <f t="shared" ref="F16:F22" si="2">D16+E16*0.01</f>
         <v>-0.89400000000000002</v>
       </c>
       <c r="G16">
         <v>4.84</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>-0.997</v>
@@ -1031,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.95699999999999996</v>
       </c>
       <c r="G17">
@@ -1041,10 +1036,10 @@
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D18">
         <v>-0.95899999999999996</v>
@@ -1053,7 +1048,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.89900000000000002</v>
       </c>
       <c r="G18">
@@ -1063,10 +1058,10 @@
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>-0.90900000000000003</v>
@@ -1075,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.86899999999999999</v>
       </c>
       <c r="G19">
@@ -1085,10 +1080,10 @@
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20">
         <v>-0.97099999999999997</v>
@@ -1097,7 +1092,7 @@
         <v>10</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.871</v>
       </c>
       <c r="G20">
@@ -1107,10 +1102,10 @@
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>-0.97199999999999998</v>
@@ -1119,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.872</v>
       </c>
       <c r="G21">
@@ -1129,10 +1124,10 @@
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>-0.90900000000000003</v>
@@ -1141,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.86899999999999999</v>
       </c>
       <c r="G22">
@@ -1151,10 +1146,10 @@
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D23">
         <v>-0.91600000000000004</v>
@@ -1163,23 +1158,23 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" ref="F23:F24" si="2">D23+E23*0.01</f>
+        <f t="shared" ref="F23:F26" si="3">D23+E23*0.01</f>
         <v>-0.90672000000000008</v>
       </c>
       <c r="G23">
         <v>0.18</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>-0.91600000000000004</v>
@@ -1188,21 +1183,66 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.90672000000000008</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="3">
         <v>0.1</v>
       </c>
       <c r="H24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25">
+        <v>-0.85199999999999998</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.73199999999999998</v>
+      </c>
+      <c r="G25">
+        <v>13628.4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>63</v>
       </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>-0.999</v>
+      </c>
+      <c r="E26">
+        <v>8.6370000000000005</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.91263000000000005</v>
+      </c>
+      <c r="G26">
+        <v>1.67</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="A2:A24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. update results for energy example with n=4, 6
2. update results for energy example with n=2, n_ts=20 3. update results for CNOT example without SOS-1 constraint with n_ts=200
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79ABC5B-D762-BD48-9F2E-E9F88F91AA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD59D000-040C-F746-9114-94CABA063C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -248,6 +248,37 @@
   </si>
   <si>
     <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc__maxswitch5</t>
+  </si>
+  <si>
+    <t>Switching time+Minup</t>
+  </si>
+  <si>
+    <t>Switching time</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_2.0_n_ts40_n_switch1_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_2.0_n_ts40_n_switch1_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>GRAPE+TR+Switching time</t>
+  </si>
+  <si>
+    <t>GRAPE+TR+Switching time
++Minup</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100</t>
+  </si>
+  <si>
+    <t>alpha=0.1</t>
   </si>
 </sst>
 </file>
@@ -266,12 +297,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -297,6 +334,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +773,7 @@
         <v>54</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F15" si="0">D5+E5*0.01</f>
+        <f t="shared" ref="F5:F19" si="0">D5+E5*0.01</f>
         <v>-0.45899999999999996</v>
       </c>
       <c r="G5" t="s">
@@ -905,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ref="F12:F13" si="1">D12+E12*0.01</f>
+        <f t="shared" ref="F12:F17" si="1">D12+E12*0.01</f>
         <v>-0.79999999999999993</v>
       </c>
       <c r="G12" t="s">
@@ -936,310 +975,931 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14">
-        <v>-0.997</v>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.89700000000000002</v>
-      </c>
-      <c r="G14">
-        <v>3.41</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>-0.996</v>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.91600000000000004</v>
-      </c>
-      <c r="G15">
-        <v>3.15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16">
-        <v>-0.99399999999999999</v>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ref="F16:F22" si="2">D16+E16*0.01</f>
-        <v>-0.89400000000000002</v>
-      </c>
-      <c r="G16">
-        <v>4.84</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
+      <c r="B17" t="s">
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17">
-        <v>-0.997</v>
+        <v>75</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.95699999999999996</v>
-      </c>
-      <c r="G17">
-        <v>2.2599999999999998</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D18">
-        <v>-0.95899999999999996</v>
+        <v>-0.997</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.89900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>-0.89700000000000002</v>
       </c>
       <c r="G18">
-        <v>1.59</v>
+        <v>3.41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19">
-        <v>-0.90900000000000003</v>
+        <v>-0.996</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.86899999999999999</v>
+        <f t="shared" si="0"/>
+        <v>-0.91600000000000004</v>
       </c>
       <c r="G19">
-        <v>1.1499999999999999</v>
+        <v>3.15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D20">
-        <v>-0.97099999999999997</v>
+        <v>-0.99399999999999999</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.871</v>
+        <f t="shared" ref="F20:F26" si="2">D20+E20*0.01</f>
+        <v>-0.89400000000000002</v>
       </c>
       <c r="G20">
-        <v>0.46</v>
+        <v>4.84</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D21">
-        <v>-0.97199999999999998</v>
+        <v>-0.997</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="2"/>
-        <v>-0.872</v>
+        <v>-0.95699999999999996</v>
       </c>
       <c r="G21">
-        <v>0.37</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22">
-        <v>-0.90900000000000003</v>
+        <v>-0.95899999999999996</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="2"/>
+        <v>-0.89900000000000002</v>
+      </c>
+      <c r="G22">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>-0.90900000000000003</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="2"/>
         <v>-0.86899999999999999</v>
       </c>
-      <c r="G22">
+      <c r="G23">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>-0.97099999999999997</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.871</v>
+      </c>
+      <c r="G24">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>-0.97199999999999998</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.872</v>
+      </c>
+      <c r="G25">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>-0.90900000000000003</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.86899999999999999</v>
+      </c>
+      <c r="G26">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" t="s">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D23">
+      <c r="D27">
         <v>-0.91600000000000004</v>
       </c>
-      <c r="E23">
+      <c r="E27">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F23" s="1">
-        <f t="shared" ref="F23:F26" si="3">D23+E23*0.01</f>
+      <c r="F27" s="1">
+        <f t="shared" ref="F27:F30" si="3">D27+E27*0.01</f>
         <v>-0.90672000000000008</v>
       </c>
-      <c r="G23">
+      <c r="G27">
         <v>0.18</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" t="s">
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <v>-0.91600000000000004</v>
       </c>
-      <c r="E24">
+      <c r="E28">
         <v>0.92800000000000005</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F28" s="1">
         <f t="shared" si="3"/>
         <v>-0.90672000000000008</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G28" s="3">
         <v>0.1</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" t="s">
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <v>-0.85199999999999998</v>
       </c>
-      <c r="E25">
+      <c r="E29">
         <v>12</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F29" s="1">
         <f t="shared" si="3"/>
         <v>-0.73199999999999998</v>
       </c>
-      <c r="G25">
+      <c r="G29">
         <v>13628.4</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>-0.999</v>
       </c>
-      <c r="E26">
+      <c r="E30">
         <v>8.6370000000000005</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F30" s="1">
         <f t="shared" si="3"/>
         <v>-0.91263000000000005</v>
       </c>
-      <c r="G26">
+      <c r="G30">
         <v>1.67</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H30" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>D33+E33*0.1</f>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G33">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>-0.79600000000000004</v>
+      </c>
+      <c r="E34">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F52" si="4">D34+E34*0.1</f>
+        <v>-0.7198</v>
+      </c>
+      <c r="G34">
+        <v>14.82</v>
+      </c>
+      <c r="H34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35">
+        <v>-0.90700000000000003</v>
+      </c>
+      <c r="E35">
+        <v>1.355</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.77150000000000007</v>
+      </c>
+      <c r="G35">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <v>-0.80600000000000005</v>
+      </c>
+      <c r="E39">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1">
+        <f>D42+E42*0.1</f>
+        <v>0.4880000000000001</v>
+      </c>
+      <c r="G39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <v>-0.76500000000000001</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <f>D43+E43*0.1</f>
+        <v>-0.73100000000000009</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <v>-0.71399999999999997</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1">
+        <f>D44+E44*0.1</f>
+        <v>7.8999999999999959E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42">
+        <v>-0.91200000000000003</v>
+      </c>
+      <c r="E42">
+        <v>14</v>
+      </c>
+      <c r="F42" s="1">
+        <f>D42+E42*0.1</f>
+        <v>0.4880000000000001</v>
+      </c>
+      <c r="G42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43">
+        <v>-0.93100000000000005</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1">
+        <f>D43+E43*0.1</f>
+        <v>-0.73100000000000009</v>
+      </c>
+      <c r="G43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <v>-0.92100000000000004</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1">
+        <f>D44+E44*0.1</f>
+        <v>7.8999999999999959E-2</v>
+      </c>
+      <c r="G44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="1">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-0.76500000000000001</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.56499999999999995</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="1">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="1">
+        <v>-0.76500000000000001</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.56499999999999995</v>
+      </c>
+      <c r="G48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G49">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G51">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G52">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" ref="F43:F57" si="5">D53+E53*0.01</f>
+        <v>-0.92899999999999994</v>
+      </c>
+      <c r="G53">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.92899999999999994</v>
+      </c>
+      <c r="G54">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.92899999999999994</v>
+      </c>
+      <c r="G55">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.92899999999999994</v>
+      </c>
+      <c r="G56">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.92899999999999994</v>
+      </c>
+      <c r="G57">
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add results of CNOT example without SOS1 constraint with n_ts=400
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD59D000-040C-F746-9114-94CABA063C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3537E3F-2364-314F-A52C-950FB1FF0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -116,24 +117,6 @@
 optimization results</t>
   </si>
   <si>
-    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR_sigma0.25_eta0.001
-_threshold30_iter100_typeminup_time10</t>
-  </si>
-  <si>
-    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
-  </si>
-  <si>
-    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.0_sigma0.25_eta0.001
-_threshold30_iter100_typeminup_time10</t>
-  </si>
-  <si>
-    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch5</t>
-  </si>
-  <si>
-    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR_sigma0.25_eta0.001
-_threshold30_iter100_typemaxswitch_switch5</t>
-  </si>
-  <si>
     <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.0_sigma0.25_eta0.001
 _threshold30_iter100_typemaxswitch_switch5</t>
   </si>
@@ -247,9 +230,6 @@
     <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
   </si>
   <si>
-    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc__maxswitch5</t>
-  </si>
-  <si>
     <t>Switching time+Minup</t>
   </si>
   <si>
@@ -275,10 +255,395 @@
 +Minup</t>
   </si>
   <si>
-    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100</t>
-  </si>
-  <si>
     <t>alpha=0.1</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_alpha0.1_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_SUR</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_minup10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_SUR_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100_SUR_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_1.0_n_ts20_n_switch1_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_1.0_n_ts20_n_switch1_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_1.0_n_ts20_n_switch1_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>100 iterations, beta=0.25, alpha=0.001</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minup10</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_1.0_n_ts20_n_switch1_initwarm_minuptime0.5_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotim_e1.0_n_ts20_n_switch1_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch5_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch5_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch5</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT</t>
+  </si>
+  <si>
+    <t>rounding of GRAPE with 
+20 maximum switches</t>
+  </si>
+  <si>
+    <t>rounding results of Trust-region for tv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_SUR</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_minup10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime10.0_n_ts200_ptypeWARM_offset0.5_objUNIT_penalty0.001_ADMM_0.25_iter100_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minup10</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch5_initwarm_minuptime0.0</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch5_initwarm_minuptime0.5</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_SUR_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_SUR_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.0_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyST4_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.5_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyST6_evotime_2.0_n_ts40_n_switch3_initwarm_minuptime0.5_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyST2_evotime_2.0_n_ts40_n_switch0_initwarm_minuptime0.5_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minup10_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minup10_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_minup10_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_minup10_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch5</t>
+  </si>
+  <si>
+    <t>Energy2_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_maxswitch5_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM2_evotime1.0_n_ts20_ptypeWARM_offset0.5_penalty0.1_ADMM_10.0_iter100_maxswitch5_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>Energy2_evotime1.0_n_ts20_ptypeCONSTANT_offset0.5_maxswitch5_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>Energy6_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_maxswitch5_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM6_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>EnergyADMM4_evotime2.0_n_ts40_ptypeWARM_offset0.5_penalty0.01_ADMM_10.0_iter100_maxswitch5_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>Energy4_evotime2.0_n_ts40_ptypeCONSTANT_offset0.5_maxswitch5_alpha0.01_sigma0.25_eta0.001
+_threshold30_iter100_typemaxswitch_switch5</t>
+  </si>
+  <si>
+    <t>&lt;0.02</t>
+  </si>
+  <si>
+    <t>&lt;0.03</t>
+  </si>
+  <si>
+    <t>alpha=0.01</t>
+  </si>
+  <si>
+    <t>alpha=0.0001</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime10.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_SUR</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_minup10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime20.0_n_ts400_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
   </si>
 </sst>
 </file>
@@ -288,10 +653,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -336,6 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A110" zoomScale="109" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -687,13 +1059,13 @@
     </row>
     <row r="2" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>-0.999</v>
@@ -715,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>-0.999</v>
@@ -736,10 +1108,10 @@
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>-0.999</v>
@@ -755,7 +1127,7 @@
         <v>1.77</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -764,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>-0.999</v>
@@ -789,7 +1161,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>-0.84099999999999997</v>
@@ -814,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>-0.97099999999999997</v>
@@ -839,7 +1211,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>-0.999</v>
@@ -864,7 +1236,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>-0.84599999999999997</v>
@@ -887,7 +1259,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>-0.97199999999999998</v>
@@ -907,10 +1279,10 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>-0.995</v>
@@ -926,16 +1298,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>-0.84</v>
@@ -955,10 +1327,10 @@
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1">
         <v>-0.96</v>
@@ -978,10 +1350,10 @@
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -1001,10 +1373,10 @@
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -1024,10 +1396,10 @@
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -1047,10 +1419,10 @@
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -1073,7 +1445,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D18">
         <v>-0.997</v>
@@ -1095,10 +1467,10 @@
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>-0.996</v>
@@ -1120,23 +1492,23 @@
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>161</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D20">
-        <v>-0.99399999999999999</v>
+        <v>-0.999</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ref="F20:F26" si="2">D20+E20*0.01</f>
-        <v>-0.89400000000000002</v>
+        <v>-0.89900000000000002</v>
       </c>
       <c r="G20">
-        <v>4.84</v>
+        <v>1.27</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
@@ -1145,10 +1517,10 @@
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>-0.997</v>
@@ -1167,10 +1539,10 @@
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>-0.95899999999999996</v>
@@ -1189,32 +1561,32 @@
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D23">
-        <v>-0.90900000000000003</v>
+        <v>-0.998</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="2"/>
-        <v>-0.86899999999999999</v>
+        <v>-0.91800000000000004</v>
       </c>
       <c r="G23">
-        <v>1.1499999999999999</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D24">
         <v>-0.97099999999999997</v>
@@ -1233,10 +1605,10 @@
     <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>151</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>-0.97199999999999998</v>
@@ -1255,32 +1627,32 @@
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D26">
-        <v>-0.90900000000000003</v>
+        <v>-0.997</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="2"/>
-        <v>-0.86899999999999999</v>
+        <v>-0.91700000000000004</v>
       </c>
       <c r="G26">
-        <v>1.1599999999999999</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>-0.91600000000000004</v>
@@ -1296,16 +1668,16 @@
         <v>0.18</v>
       </c>
       <c r="H27" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>-0.91600000000000004</v>
@@ -1321,16 +1693,16 @@
         <v>0.1</v>
       </c>
       <c r="H28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D29">
         <v>-0.85199999999999998</v>
@@ -1346,15 +1718,15 @@
         <v>13628.4</v>
       </c>
       <c r="H29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>-0.999</v>
@@ -1370,16 +1742,16 @@
         <v>1.67</v>
       </c>
       <c r="H30" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D33">
         <v>-0.94899999999999995</v>
@@ -1397,10 +1769,10 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>-0.79600000000000004</v>
@@ -1409,22 +1781,22 @@
         <v>0.76200000000000001</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F52" si="4">D34+E34*0.1</f>
+        <f t="shared" ref="F34:F57" si="4">D34+E34*0.1</f>
         <v>-0.7198</v>
       </c>
       <c r="G34">
         <v>14.82</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D35">
         <v>-0.90700000000000003</v>
@@ -1442,10 +1814,10 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D36">
         <v>-0.94899999999999995</v>
@@ -1463,10 +1835,10 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>-0.94899999999999995</v>
@@ -1484,10 +1856,10 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D38">
         <v>-0.94899999999999995</v>
@@ -1505,10 +1877,10 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D39">
         <v>-0.80600000000000005</v>
@@ -1526,10 +1898,10 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D40">
         <v>-0.76500000000000001</v>
@@ -1547,10 +1919,10 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D41">
         <v>-0.71399999999999997</v>
@@ -1568,10 +1940,10 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>-0.91200000000000003</v>
@@ -1589,10 +1961,10 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D43">
         <v>-0.93100000000000005</v>
@@ -1610,10 +1982,10 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D44">
         <v>-0.92100000000000004</v>
@@ -1631,10 +2003,10 @@
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D45" s="1">
         <v>-0.94899999999999995</v>
@@ -1652,10 +2024,10 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D46" s="1">
         <v>-0.76500000000000001</v>
@@ -1673,10 +2045,10 @@
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D47" s="1">
         <v>-0.94899999999999995</v>
@@ -1694,10 +2066,10 @@
     </row>
     <row r="48" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D48" s="1">
         <v>-0.76500000000000001</v>
@@ -1715,10 +2087,10 @@
     </row>
     <row r="49" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D49">
         <v>-0.94899999999999995</v>
@@ -1736,10 +2108,10 @@
     </row>
     <row r="50" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D50">
         <v>-0.94899999999999995</v>
@@ -1757,10 +2129,10 @@
     </row>
     <row r="51" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D51">
         <v>-0.94899999999999995</v>
@@ -1773,15 +2145,15 @@
         <v>-0.74899999999999989</v>
       </c>
       <c r="G51">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D52">
         <v>-0.94899999999999995</v>
@@ -1799,10 +2171,10 @@
     </row>
     <row r="53" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D53">
         <v>-0.94899999999999995</v>
@@ -1811,8 +2183,8 @@
         <v>2</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" ref="F43:F57" si="5">D53+E53*0.01</f>
-        <v>-0.92899999999999994</v>
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
       </c>
       <c r="G53">
         <v>0.6</v>
@@ -1820,10 +2192,10 @@
     </row>
     <row r="54" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D54">
         <v>-0.94899999999999995</v>
@@ -1832,19 +2204,19 @@
         <v>2</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.92899999999999994</v>
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
       </c>
       <c r="G54">
-        <v>0.61</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D55">
         <v>-0.94899999999999995</v>
@@ -1853,8 +2225,8 @@
         <v>2</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.92899999999999994</v>
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
       </c>
       <c r="G55">
         <v>0.26</v>
@@ -1862,10 +2234,10 @@
     </row>
     <row r="56" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D56">
         <v>-0.94899999999999995</v>
@@ -1874,8 +2246,8 @@
         <v>2</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.92899999999999994</v>
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
       </c>
       <c r="G56">
         <v>0.69</v>
@@ -1883,10 +2255,10 @@
     </row>
     <row r="57" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D57">
         <v>-0.94899999999999995</v>
@@ -1895,13 +2267,1905 @@
         <v>2</v>
       </c>
       <c r="F57" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.74899999999999989</v>
+      </c>
+      <c r="G57">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60">
+        <v>-4.7359999999999998</v>
+      </c>
+      <c r="E60">
+        <v>9.8680000000000003</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" ref="F60:F84" si="5">D60+E60*0.01</f>
+        <v>-4.6373199999999999</v>
+      </c>
+      <c r="G60">
+        <v>40.481000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61">
+        <v>-4.6550000000000002</v>
+      </c>
+      <c r="E61">
+        <v>2.5179999999999998</v>
+      </c>
+      <c r="F61" s="1">
         <f t="shared" si="5"/>
-        <v>-0.92899999999999994</v>
-      </c>
-      <c r="G57">
-        <v>0.21</v>
-      </c>
-    </row>
+        <v>-4.6298200000000005</v>
+      </c>
+      <c r="G61">
+        <v>1143.44</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62">
+        <v>-4.734</v>
+      </c>
+      <c r="E62">
+        <v>7.0789999999999997</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.6632100000000003</v>
+      </c>
+      <c r="G62">
+        <v>151.85</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="1">
+        <v>-4.67</v>
+      </c>
+      <c r="E63">
+        <v>30</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.37</v>
+      </c>
+      <c r="G63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="G64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="1">
+        <v>-4.62</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.5200000000000005</v>
+      </c>
+      <c r="G65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66">
+        <v>-4.6440000000000001</v>
+      </c>
+      <c r="E66">
+        <v>56</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.0839999999999996</v>
+      </c>
+      <c r="G66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="1">
+        <v>-0.28199999999999997</v>
+      </c>
+      <c r="E67">
+        <v>6</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.22199999999999998</v>
+      </c>
+      <c r="G67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68">
+        <v>-4.1040000000000001</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.0040000000000004</v>
+      </c>
+      <c r="G68">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" s="1">
+        <v>-4.7220000000000004</v>
+      </c>
+      <c r="E69">
+        <v>38</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.3420000000000005</v>
+      </c>
+      <c r="G69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="E70">
+        <v>4</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="G70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" s="1">
+        <v>-4.5810000000000004</v>
+      </c>
+      <c r="E71">
+        <v>10</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.4810000000000008</v>
+      </c>
+      <c r="G71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72">
+        <v>-2.8780000000000001</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.8380000000000001</v>
+      </c>
+      <c r="G72">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="1">
+        <v>-1.272</v>
+      </c>
+      <c r="E73">
+        <v>6</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.212</v>
+      </c>
+      <c r="G73">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>104</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="1">
+        <v>-0.156</v>
+      </c>
+      <c r="E75">
+        <v>6</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="5"/>
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="G75">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76">
+        <v>-4.6859999999999999</v>
+      </c>
+      <c r="E76">
+        <v>22</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.4660000000000002</v>
+      </c>
+      <c r="G76">
+        <v>19.510000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B77" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" s="1">
+        <v>-1.1319999999999999</v>
+      </c>
+      <c r="E77">
+        <v>6</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.0719999999999998</v>
+      </c>
+      <c r="G77">
+        <v>20.02</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B78" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78">
+        <v>-4.6660000000000004</v>
+      </c>
+      <c r="E78">
+        <v>10</v>
+      </c>
+      <c r="F78" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.5660000000000007</v>
+      </c>
+      <c r="G78">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B79" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79" s="1">
+        <v>-4.6440000000000001</v>
+      </c>
+      <c r="E79">
+        <v>56</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.0839999999999996</v>
+      </c>
+      <c r="G79">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B80" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80">
+        <v>-1.1319999999999999</v>
+      </c>
+      <c r="E80">
+        <v>4</v>
+      </c>
+      <c r="F80" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.0919999999999999</v>
+      </c>
+      <c r="G80">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B81" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" s="1">
+        <v>-4.681</v>
+      </c>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="F81" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.5810000000000004</v>
+      </c>
+      <c r="G81">
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B82" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82">
+        <v>-4.5179999999999998</v>
+      </c>
+      <c r="E82">
+        <v>20</v>
+      </c>
+      <c r="F82" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.3179999999999996</v>
+      </c>
+      <c r="G82">
+        <v>79.12</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B83" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="1">
+        <v>-1.548</v>
+      </c>
+      <c r="E83">
+        <v>6</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.488</v>
+      </c>
+      <c r="G83">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B84" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84">
+        <v>-4.681</v>
+      </c>
+      <c r="E84">
+        <v>10</v>
+      </c>
+      <c r="F84" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.5810000000000004</v>
+      </c>
+      <c r="G84">
+        <v>88.38</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87">
+        <v>-3.9990000000000001</v>
+      </c>
+      <c r="E87">
+        <v>4.5519999999999996</v>
+      </c>
+      <c r="F87" s="1">
+        <f t="shared" ref="F87:F111" si="6">D87+E87*0.01</f>
+        <v>-3.9534800000000003</v>
+      </c>
+      <c r="G87">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88">
+        <v>-3.9929999999999999</v>
+      </c>
+      <c r="E88">
+        <v>3.4289999999999998</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.95871</v>
+      </c>
+      <c r="G88">
+        <v>133.13999999999999</v>
+      </c>
+      <c r="H88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89">
+        <v>-3.9990000000000001</v>
+      </c>
+      <c r="E89">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.96217</v>
+      </c>
+      <c r="G89">
+        <v>43.35</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90">
+        <v>-3.9980000000000002</v>
+      </c>
+      <c r="E90">
+        <v>42</v>
+      </c>
+      <c r="F90" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.5780000000000003</v>
+      </c>
+      <c r="G90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E91">
+        <v>6</v>
+      </c>
+      <c r="F91" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>134</v>
+      </c>
+      <c r="C92" t="s">
+        <v>31</v>
+      </c>
+      <c r="D92">
+        <v>-3.92</v>
+      </c>
+      <c r="E92">
+        <v>10</v>
+      </c>
+      <c r="F92" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.82</v>
+      </c>
+      <c r="G92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93">
+        <v>-3.9940000000000002</v>
+      </c>
+      <c r="E93">
+        <v>46</v>
+      </c>
+      <c r="F93" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.5340000000000003</v>
+      </c>
+      <c r="G93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>136</v>
+      </c>
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E94">
+        <v>6</v>
+      </c>
+      <c r="F94" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95">
+        <v>-3.9279999999999999</v>
+      </c>
+      <c r="E95">
+        <v>10</v>
+      </c>
+      <c r="F95" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8279999999999998</v>
+      </c>
+      <c r="G95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" t="s">
+        <v>59</v>
+      </c>
+      <c r="D96">
+        <v>-3.9990000000000001</v>
+      </c>
+      <c r="E96">
+        <v>38</v>
+      </c>
+      <c r="F96" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.6190000000000002</v>
+      </c>
+      <c r="G96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E97">
+        <v>6</v>
+      </c>
+      <c r="F97" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G97" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>140</v>
+      </c>
+      <c r="C98" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98">
+        <v>-3.9260000000000002</v>
+      </c>
+      <c r="E98">
+        <v>10</v>
+      </c>
+      <c r="F98" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8260000000000001</v>
+      </c>
+      <c r="G98" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>141</v>
+      </c>
+      <c r="C99" t="s">
+        <v>63</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99" s="1">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+      <c r="G99">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>142</v>
+      </c>
+      <c r="C100" t="s">
+        <v>62</v>
+      </c>
+      <c r="D100">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E100">
+        <v>6</v>
+      </c>
+      <c r="F100" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G100">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>143</v>
+      </c>
+      <c r="C101" t="s">
+        <v>68</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101" s="1">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+      <c r="G101">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>144</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D102">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E102">
+        <v>6</v>
+      </c>
+      <c r="F102" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G102">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B103" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103">
+        <v>-3.9980000000000002</v>
+      </c>
+      <c r="E103">
+        <v>42</v>
+      </c>
+      <c r="F103" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.5780000000000003</v>
+      </c>
+      <c r="G103">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B104" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E104">
+        <v>6</v>
+      </c>
+      <c r="F104" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G104">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B105" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D105">
+        <v>-3.9620000000000002</v>
+      </c>
+      <c r="E105">
+        <v>10</v>
+      </c>
+      <c r="F105" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8620000000000001</v>
+      </c>
+      <c r="G105">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B106" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D106">
+        <v>-3.9940000000000002</v>
+      </c>
+      <c r="E106">
+        <v>46</v>
+      </c>
+      <c r="F106" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.5340000000000003</v>
+      </c>
+      <c r="G106">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B107" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E107">
+        <v>6</v>
+      </c>
+      <c r="F107" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G107">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B108" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D108">
+        <v>-3.9710000000000001</v>
+      </c>
+      <c r="E108">
+        <v>10</v>
+      </c>
+      <c r="F108" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.871</v>
+      </c>
+      <c r="G108">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B109" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D109">
+        <v>-3.9889999999999999</v>
+      </c>
+      <c r="E109">
+        <v>14</v>
+      </c>
+      <c r="F109" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8489999999999998</v>
+      </c>
+      <c r="G109">
+        <v>22.66</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B110" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E110">
+        <v>6</v>
+      </c>
+      <c r="F110" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G110">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B111" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D111">
+        <v>-3.992</v>
+      </c>
+      <c r="E111">
+        <v>10</v>
+      </c>
+      <c r="F111" s="1">
+        <f t="shared" si="6"/>
+        <v>-3.8919999999999999</v>
+      </c>
+      <c r="G111">
+        <v>13.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
+  <dimension ref="B1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="119.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="8" max="8" width="57.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.159E-9</v>
+      </c>
+      <c r="E2">
+        <v>20.978999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <f>D2+E2*0.001</f>
+        <v>2.0979001159000001E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3.2079999999999999E-4</v>
+      </c>
+      <c r="E3">
+        <v>11.055999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <f>D3+E3*0.001</f>
+        <v>1.1376799999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>70.209999999999994</v>
+      </c>
+      <c r="H3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2.654E-4</v>
+      </c>
+      <c r="E4">
+        <v>15.194000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>D4+E4*0.01</f>
+        <v>0.15220540000000002</v>
+      </c>
+      <c r="G4">
+        <v>192.78</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="8">
+        <v>6.0090000000000002E-4</v>
+      </c>
+      <c r="E5">
+        <v>116</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F19" si="0">D5+E5*0.01</f>
+        <v>1.1606008999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>0.158</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.378</v>
+      </c>
+      <c r="G6">
+        <v>19.29</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="G7">
+        <v>61.83</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
+        <v>86</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23399999999999999</v>
+      </c>
+      <c r="G9">
+        <v>6.49</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1">
+        <f>D10+E10*0.01</f>
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="G10">
+        <v>61.83</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>1E-3</v>
+      </c>
+      <c r="E11">
+        <v>116</v>
+      </c>
+      <c r="F11" s="1">
+        <f>D11+E11*0.01</f>
+        <v>1.1609999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" ref="F12:F13" si="1">D12+E12*0.01</f>
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G12">
+        <v>13.5</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E13">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="G13">
+        <v>61.83</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>1E-3</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="G14">
+        <v>70.36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E15">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G15">
+        <v>74.83</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>1E-3</v>
+      </c>
+      <c r="E16">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G16">
+        <v>19.89</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>1E-3</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="G17">
+        <v>56.9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.156</v>
+      </c>
+      <c r="G18">
+        <v>51.37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>1E-3</v>
+      </c>
+      <c r="E19">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="G19">
+        <v>16.649999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5.9270000000000003E-10</v>
+      </c>
+      <c r="E22">
+        <v>26.161999999999999</v>
+      </c>
+      <c r="F22" s="1">
+        <f>D22+E22*0.0001</f>
+        <v>2.6162005927000001E-3</v>
+      </c>
+      <c r="G22">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8">
+        <v>8.0709999999999997E-7</v>
+      </c>
+      <c r="E23">
+        <v>15.099</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:F39" si="2">D23+E23*0.0001</f>
+        <v>1.5107071000000001E-3</v>
+      </c>
+      <c r="G23">
+        <v>150.25</v>
+      </c>
+      <c r="H23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="8">
+        <v>4.0629999999999999E-6</v>
+      </c>
+      <c r="E24">
+        <v>23.481000000000002</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="2"/>
+        <v>2.352163E-3</v>
+      </c>
+      <c r="G24">
+        <v>432.73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>1E-3</v>
+      </c>
+      <c r="E25">
+        <v>491</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0100000000000006E-2</v>
+      </c>
+      <c r="G25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="E26">
+        <v>53</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.7873</v>
+      </c>
+      <c r="G26">
+        <v>28.46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.65790000000000004</v>
+      </c>
+      <c r="G27">
+        <v>67.41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>1E-3</v>
+      </c>
+      <c r="E28">
+        <v>467</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7700000000000006E-2</v>
+      </c>
+      <c r="G28">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="E29">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="2"/>
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="G29">
+        <v>38.42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="E30">
+        <v>39</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="2"/>
+        <v>0.62290000000000001</v>
+      </c>
+      <c r="G30">
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>1E-3</v>
+      </c>
+      <c r="E31">
+        <v>480</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="2"/>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="G31">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32">
+        <v>0.314</v>
+      </c>
+      <c r="E32">
+        <v>51</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="2"/>
+        <v>0.31909999999999999</v>
+      </c>
+      <c r="G32">
+        <v>22.86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="E33">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.70089999999999997</v>
+      </c>
+      <c r="G33">
+        <v>67.22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="8">
+        <v>4.5560000000000002E-4</v>
+      </c>
+      <c r="E34">
+        <v>479</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="2"/>
+        <v>4.8355600000000006E-2</v>
+      </c>
+      <c r="G34">
+        <v>27.82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35">
+        <v>1E-3</v>
+      </c>
+      <c r="E35">
+        <v>38</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="G35">
+        <v>208.79</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="8">
+        <v>9.4689999999999998E-4</v>
+      </c>
+      <c r="E36">
+        <v>40</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="2"/>
+        <v>4.9468999999999997E-3</v>
+      </c>
+      <c r="G36">
+        <v>153.63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="8">
+        <v>5.0730000000000003E-4</v>
+      </c>
+      <c r="E37">
+        <v>441</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4607300000000003E-2</v>
+      </c>
+      <c r="G37">
+        <v>33.770000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>1E-3</v>
+      </c>
+      <c r="E38">
+        <v>48</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8000000000000005E-3</v>
+      </c>
+      <c r="G38">
+        <v>157.57</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="8">
+        <v>7.4489999999999995E-4</v>
+      </c>
+      <c r="E39">
+        <v>40</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7448999999999998E-3</v>
+      </c>
+      <c r="G39">
+        <v>157.87</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add results of CNOT example without SOS1 constraint with n_ts=300
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3537E3F-2364-314F-A52C-950FB1FF0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D606DD17-B188-B54F-9531-40D30F189B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="520" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -644,6 +644,114 @@
   </si>
   <si>
     <t>CNOTADMM_evotime20.0_n_ts400_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_SUR_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_SUR</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_minup10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_penalty0.01_ADMM_0.25_iter100_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime5.0_n_ts100_ptypeCONSTANT_offset0.5_objUNIT_SUR_alpha0.01_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_SUR</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_minup10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch20</t>
+  </si>
+  <si>
+    <t>CNOT_evotime15.0_n_ts300_ptypeCONSTANT_offset0.5_objUNIT_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv</t>
+  </si>
+  <si>
+    <t>CNOTADMM_evotime15.0_n_ts300_ptypeWARM_offset0.5_objUNIT_penalty0.0001_ADMM_0.25_iter100_maxswitch20_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch20</t>
   </si>
 </sst>
 </file>
@@ -694,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -708,6 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A98" zoomScale="109" workbookViewId="0">
       <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
@@ -3337,10 +3446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3430,8 +3539,8 @@
         <v>15.194000000000001</v>
       </c>
       <c r="F4" s="1">
-        <f>D4+E4*0.01</f>
-        <v>0.15220540000000002</v>
+        <f>D4+E4*0.001</f>
+        <v>1.5459400000000002E-2</v>
       </c>
       <c r="G4">
         <v>192.78</v>
@@ -3454,8 +3563,8 @@
         <v>116</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F19" si="0">D5+E5*0.01</f>
-        <v>1.1606008999999999</v>
+        <f t="shared" ref="F5:F18" si="0">D5+E5*0.001</f>
+        <v>0.11660090000000001</v>
       </c>
       <c r="G5">
         <v>0.01</v>
@@ -3479,7 +3588,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.378</v>
+        <v>0.18</v>
       </c>
       <c r="G6">
         <v>19.29</v>
@@ -3503,7 +3612,7 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0.40100000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="G7">
         <v>61.83</v>
@@ -3527,7 +3636,7 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>0.86099999999999999</v>
+        <v>8.7000000000000008E-2</v>
       </c>
       <c r="G8">
         <v>0.01</v>
@@ -3551,7 +3660,7 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>0.23399999999999999</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="G9">
         <v>6.49</v>
@@ -3572,8 +3681,8 @@
         <v>32</v>
       </c>
       <c r="F10" s="1">
-        <f>D10+E10*0.01</f>
-        <v>0.32600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G10">
         <v>61.83</v>
@@ -3594,8 +3703,8 @@
         <v>116</v>
       </c>
       <c r="F11" s="1">
-        <f>D11+E11*0.01</f>
-        <v>1.1609999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.11700000000000001</v>
       </c>
       <c r="G11">
         <v>0.01</v>
@@ -3618,8 +3727,8 @@
         <v>21</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ref="F12:F13" si="1">D12+E12*0.01</f>
-        <v>0.53300000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.34400000000000003</v>
       </c>
       <c r="G12">
         <v>13.5</v>
@@ -3640,8 +3749,8 @@
         <v>38</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.39900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>5.6999999999999995E-2</v>
       </c>
       <c r="G13">
         <v>61.83</v>
@@ -3663,7 +3772,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>0.30099999999999999</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G14">
         <v>70.36</v>
@@ -3687,7 +3796,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>0.23400000000000001</v>
+        <v>2.7E-2</v>
       </c>
       <c r="G15">
         <v>74.83</v>
@@ -3711,7 +3820,7 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>0.39100000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="G16">
         <v>19.89</v>
@@ -3735,7 +3844,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>0.20100000000000001</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G17">
         <v>56.9</v>
@@ -3756,7 +3865,7 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>0.156</v>
+        <v>2.0999999999999998E-2</v>
       </c>
       <c r="G18">
         <v>51.37</v>
@@ -3776,8 +3885,8 @@
         <v>36</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.36099999999999999</v>
+        <f>D19+E19*0.001</f>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="G19">
         <v>16.649999999999999</v>
@@ -3819,7 +3928,7 @@
         <v>15.099</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" ref="F23:F39" si="2">D23+E23*0.0001</f>
+        <f>D23+E23*0.0001</f>
         <v>1.5107071000000001E-3</v>
       </c>
       <c r="G23">
@@ -3843,7 +3952,7 @@
         <v>23.481000000000002</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F23:F39" si="1">D24+E24*0.0001</f>
         <v>2.352163E-3</v>
       </c>
       <c r="G24">
@@ -3864,7 +3973,7 @@
         <v>491</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.0100000000000006E-2</v>
       </c>
       <c r="G25">
@@ -3885,7 +3994,7 @@
         <v>53</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.7873</v>
       </c>
       <c r="G26">
@@ -3906,7 +4015,7 @@
         <v>39</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.65790000000000004</v>
       </c>
       <c r="G27">
@@ -3927,7 +4036,7 @@
         <v>467</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.7700000000000006E-2</v>
       </c>
       <c r="G28">
@@ -3948,7 +4057,7 @@
         <v>47</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.52170000000000005</v>
       </c>
       <c r="G29">
@@ -3969,7 +4078,7 @@
         <v>39</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.62290000000000001</v>
       </c>
       <c r="G30">
@@ -3990,7 +4099,7 @@
         <v>480</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="G31">
@@ -4011,14 +4120,14 @@
         <v>51</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.31909999999999999</v>
       </c>
       <c r="G32">
         <v>22.86</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>187</v>
       </c>
@@ -4032,14 +4141,14 @@
         <v>39</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.70089999999999997</v>
       </c>
       <c r="G33">
         <v>67.22</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>181</v>
       </c>
@@ -4053,14 +4162,14 @@
         <v>479</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.8355600000000006E-2</v>
       </c>
       <c r="G34">
         <v>27.82</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>188</v>
       </c>
@@ -4074,14 +4183,14 @@
         <v>38</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.8000000000000004E-3</v>
       </c>
       <c r="G35">
         <v>208.79</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>189</v>
       </c>
@@ -4095,14 +4204,14 @@
         <v>40</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.9468999999999997E-3</v>
       </c>
       <c r="G36">
         <v>153.63</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>190</v>
       </c>
@@ -4116,14 +4225,14 @@
         <v>441</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.4607300000000003E-2</v>
       </c>
       <c r="G37">
         <v>33.770000000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>191</v>
       </c>
@@ -4137,14 +4246,14 @@
         <v>48</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.8000000000000005E-3</v>
       </c>
       <c r="G38">
         <v>157.57</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>192</v>
       </c>
@@ -4158,14 +4267,777 @@
         <v>40</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.7448999999999998E-3</v>
       </c>
       <c r="G39">
         <v>157.87</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="E42">
+        <v>16</v>
+      </c>
+      <c r="F42" s="1">
+        <f>D42+E42*0.01</f>
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="G42">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43">
+        <v>0.191</v>
+      </c>
+      <c r="E43">
+        <v>6.0940000000000003</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" ref="F43:F59" si="2">D43+E43*0.01</f>
+        <v>0.25194</v>
+      </c>
+      <c r="G43">
+        <v>21.75</v>
+      </c>
+      <c r="H43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44">
+        <v>0.124</v>
+      </c>
+      <c r="E44">
+        <v>9.4190000000000005</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21819</v>
+      </c>
+      <c r="G44">
+        <v>79.55</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45">
+        <v>0.17</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33</v>
+      </c>
+      <c r="G45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="2"/>
+        <v>0.34299999999999997</v>
+      </c>
+      <c r="G46">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47">
+        <v>0.17</v>
+      </c>
+      <c r="E47">
+        <v>16</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33</v>
+      </c>
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>204</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48">
+        <v>0.19</v>
+      </c>
+      <c r="E48">
+        <v>41</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E49">
+        <v>7</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="2"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="G49">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50">
+        <v>0.191</v>
+      </c>
+      <c r="E50">
+        <v>32</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="2"/>
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="G50">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="E51">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="2"/>
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="2"/>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="G52">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="2"/>
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="G53">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>210</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E54">
+        <v>9</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G54">
+        <v>12.69</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E55">
+        <v>9</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="G55">
+        <v>19.670000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56">
+        <v>0.17</v>
+      </c>
+      <c r="E56">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33</v>
+      </c>
+      <c r="G56">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E57">
+        <v>9</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G57">
+        <v>30.09</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="G58">
+        <v>21.46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="E59">
+        <v>16</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33199999999999996</v>
+      </c>
+      <c r="G59">
+        <v>12.58</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>213</v>
+      </c>
+      <c r="C62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="8">
+        <v>1.004E-10</v>
+      </c>
+      <c r="E62">
+        <v>29.846</v>
+      </c>
+      <c r="F62" s="1">
+        <f>D62+E62*0.0001</f>
+        <v>2.9846001004E-3</v>
+      </c>
+      <c r="G62">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" s="8">
+        <v>3.653E-6</v>
+      </c>
+      <c r="E63">
+        <v>16.795000000000002</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" ref="F63:F79" si="3">D63+E63*0.0001</f>
+        <v>1.6831530000000002E-3</v>
+      </c>
+      <c r="G63">
+        <v>100.59</v>
+      </c>
+      <c r="H63" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="8">
+        <v>8.4270000000000008E-6</v>
+      </c>
+      <c r="E64">
+        <v>24.347999999999999</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4432270000000001E-3</v>
+      </c>
+      <c r="G64">
+        <v>348.96</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>214</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E65">
+        <v>266</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7600000000000003E-2</v>
+      </c>
+      <c r="G65">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="E66">
+        <v>37</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="3"/>
+        <v>0.54270000000000007</v>
+      </c>
+      <c r="G66">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E67">
+        <v>38</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="3"/>
+        <v>0.32880000000000004</v>
+      </c>
+      <c r="G67">
+        <v>64.36</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>219</v>
+      </c>
+      <c r="C68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E68">
+        <v>279</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="3"/>
+        <v>3.09E-2</v>
+      </c>
+      <c r="G68">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E69">
+        <v>27</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="3"/>
+        <v>0.1787</v>
+      </c>
+      <c r="G69">
+        <v>25.79</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0.214</v>
+      </c>
+      <c r="E70">
+        <v>39</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="3"/>
+        <v>0.21789999999999998</v>
+      </c>
+      <c r="G70">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="E71">
+        <v>276</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="3"/>
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="G71">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>223</v>
+      </c>
+      <c r="C72" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E72">
+        <v>36</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="3"/>
+        <v>0.29359999999999997</v>
+      </c>
+      <c r="G72">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E73">
+        <v>40</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="3"/>
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G73">
+        <v>64.62</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="8">
+        <v>5.5900000000000004E-4</v>
+      </c>
+      <c r="E74">
+        <v>262</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6759000000000002E-2</v>
+      </c>
+      <c r="G74">
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B75" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E75">
+        <v>33</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="3"/>
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="G75">
+        <v>150.25</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D76" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E76">
+        <v>39</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="3"/>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="G76">
+        <v>113.02</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B77" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" s="8">
+        <v>8.5079999999999997E-4</v>
+      </c>
+      <c r="E77">
+        <v>263</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7150799999999999E-2</v>
+      </c>
+      <c r="G77">
+        <v>25.57</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B78" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E78">
+        <v>30</v>
+      </c>
+      <c r="F78" s="1">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G78">
+        <v>107.17</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B79" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="E79">
+        <v>40</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" si="3"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G79">
+        <v>82.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update results of Hadamard example with n=2
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADE12B4-C7BB-1545-86DE-196C8BE3139F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7576038-8115-4F47-9843-06802E3F2266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -3825,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
   <dimension ref="B1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4392,7 +4392,7 @@
         <v>23.481000000000002</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" ref="F27:F42" si="1">D27+E27*0.0001</f>
+        <f t="shared" ref="F27:F45" si="1">D27+E27*0.0001</f>
         <v>2.352163E-3</v>
       </c>
       <c r="G27">
@@ -4721,8 +4721,19 @@
       <c r="C43" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="F43" s="1"/>
+      <c r="D43" s="8">
+        <v>6.1320000000000005E-4</v>
+      </c>
+      <c r="E43">
+        <v>471</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7713200000000004E-2</v>
+      </c>
+      <c r="G43">
+        <v>26.22</v>
+      </c>
     </row>
     <row r="44" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
@@ -4731,8 +4742,19 @@
       <c r="C44" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="F44" s="1"/>
+      <c r="D44" s="8">
+        <v>8.2229999999999998E-4</v>
+      </c>
+      <c r="E44">
+        <v>49</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7222999999999996E-3</v>
+      </c>
+      <c r="G44">
+        <v>139.69</v>
+      </c>
     </row>
     <row r="45" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
@@ -4741,8 +4763,19 @@
       <c r="C45" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="F45" s="1"/>
+      <c r="D45" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E45">
+        <v>40</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G45">
+        <v>155.07</v>
+      </c>
     </row>
     <row r="47" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
1. modify rounding function to add time limit.
2. update results of LiH example
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F510B2-499D-384D-BEB3-AEA7F364F6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC55121-B04C-0649-8F9C-EC99D4E9AAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="271">
   <si>
     <t>Name</t>
   </si>
@@ -876,6 +877,9 @@
   </si>
   <si>
     <t>t_f=15</t>
+  </si>
+  <si>
+    <t>l2 norm</t>
   </si>
 </sst>
 </file>
@@ -3867,7 +3871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
@@ -5814,19 +5818,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0842C86B-7D36-B04D-B09B-8D3C95D38C2E}">
-  <dimension ref="B1:H26"/>
+  <dimension ref="B1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="8" max="8" width="45.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="9" max="9" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -5840,89 +5845,120 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E2">
+        <v>15.271000000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <f>D2+E2*0.0001</f>
+        <v>1.75271E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>91.605999999999995</v>
+      </c>
+      <c r="H2">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>229</v>
       </c>
-      <c r="H3" t="s">
+      <c r="D3" s="8">
+        <v>1.5590000000000001E-9</v>
+      </c>
+      <c r="E3">
+        <v>18.867999999999999</v>
+      </c>
+      <c r="G3" s="8">
+        <v>6.9650000000000002E-7</v>
+      </c>
+      <c r="H3">
+        <v>0.39</v>
+      </c>
+      <c r="I3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>35</v>
       </c>
@@ -5974,6 +6010,149 @@
     </row>
     <row r="26" spans="3:3" ht="17" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
+  <dimension ref="B2:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update results of Hadamard transform example with n=3
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC55121-B04C-0649-8F9C-EC99D4E9AAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4E3E79-6B83-9A47-9BB1-3B3DE9288FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="346">
   <si>
     <t>Name</t>
   </si>
@@ -880,6 +880,252 @@
   </si>
   <si>
     <t>l2 norm</t>
+  </si>
+  <si>
+    <t>sum_penalty=1.0</t>
+  </si>
+  <si>
+    <t>alpha=0.0001, beta=0.5, iterations=100</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_
+eta0.001_threshold30_iter100_typetvc.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_minup10.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.25
+_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10_sigma0.25_eta0.001
+_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8_sigma0.25_
+eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR_alpha0.0001_sigma0.25_
+eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+TR</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+Minup</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+Maxswitch</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8_sigma0.25_eta0.001_
+threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10_sigma0.25_eta0.001_
+threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
+maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>instance of molecule example with H2</t>
+  </si>
+  <si>
+    <t>ADMM+ST</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+ST</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+ST+Minup</t>
+  </si>
+  <si>
+    <t>ADMM+ST+Minup</t>
+  </si>
+  <si>
+    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_minup10.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8_sigma0.25_
+eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR_alpha0.0001_sigma0.25_
+eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_
+eta0.001_threshold30_iter100_typetvc.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch2_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch2_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch10_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch10_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_SUR.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.00_threshold30_iter100_typetvc_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.2_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>instance of molecule example with LiH</t>
+  </si>
+  <si>
+    <t>sum_penalty=0.1</t>
+  </si>
+  <si>
+    <t>Molecule2_LiH_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
   </si>
 </sst>
 </file>
@@ -3872,7 +4118,7 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+      <selection activeCell="C89" sqref="C89:C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5821,7 +6067,7 @@
   <dimension ref="B1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D1" sqref="D1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6020,140 +6266,1593 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
-  <dimension ref="B2:B26"/>
+  <dimension ref="B1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D2" s="8">
+        <v>4.3679999999999999E-7</v>
+      </c>
+      <c r="E2">
+        <v>25.515999999999998</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2+E2*0.0001</f>
+        <v>2.5520368E-3</v>
+      </c>
+      <c r="G2">
+        <v>167.48099999999999</v>
+      </c>
+      <c r="H2">
+        <v>1.42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D3" s="8">
+        <v>2.4830000000000002E-7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>18.72</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F23" si="0">D3+E3*0.0001</f>
+        <v>1.8722483000000001E-3</v>
+      </c>
+      <c r="G3" s="8">
+        <v>5.553E-7</v>
+      </c>
+      <c r="H3">
+        <v>3.01</v>
+      </c>
+      <c r="I3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" s="8">
+        <v>5.3229999999999997E-7</v>
+      </c>
+      <c r="E4">
+        <v>2.0510000000000002</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0563230000000002E-4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>2.1660000000000002E-9</v>
+      </c>
+      <c r="H4">
+        <v>54.19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D5" s="8">
+        <v>2.8770000000000001E-5</v>
+      </c>
+      <c r="E5">
+        <v>15.753</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6040700000000002E-3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>6.8670000000000005E-4</v>
+      </c>
+      <c r="H5" s="3">
+        <v>167.13499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D6" s="9">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="E6">
+        <v>102</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.92920000000000003</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D7" s="9">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>29.77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D8" s="9">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D9" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4200000000000003E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D10" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.6008</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="D11" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="D12" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2400000000000001E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D13" s="9">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2954</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="D14" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E14">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>60.76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="D15" s="9">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="D16" s="9">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.57979999999999998</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E17">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" s="9">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E18">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D19" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D21" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.72E-2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D22" s="9">
+        <v>0.245</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1">
+        <f>D22+E22*0.0001</f>
+        <v>0.2462</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D23" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D24" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E24">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1">
+        <f>D24+E24*0.0001</f>
+        <v>1.2400000000000001E-2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="D25" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>D25+E25*0.0001</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="D26" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1">
+        <f>D26+E26*0.0001</f>
+        <v>6.8000000000000005E-3</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="F27" s="1">
+        <f>D27+E27*0.0001</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D28" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <f>D28+E28*0.0001</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E29">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1">
+        <f>D29+E29*0.0001</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>303</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D30" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>D30+E30*0.0001</f>
+        <v>4.82E-2</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>304</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.246</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>D31+E31*0.0001</f>
+        <v>0.2462</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>305</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D32" s="8">
+        <v>2.5309999999999998E-10</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <f>D32+E32*0.0001</f>
+        <v>2.0000002531000002E-3</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.749</v>
+      </c>
+      <c r="E33">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1">
+        <f>D33+E33*0.0001</f>
+        <v>0.75039999999999996</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>345</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E38">
+        <v>339.31900000000002</v>
+      </c>
+      <c r="F38" s="8">
+        <f>D38+E38*0.0001</f>
+        <v>7.99319E-2</v>
+      </c>
+      <c r="G38">
+        <v>7090.22</v>
+      </c>
+      <c r="H38">
+        <v>327.06</v>
+      </c>
+      <c r="I38" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C39" t="s">
+        <v>229</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0.126</v>
+      </c>
+      <c r="E39" s="1">
+        <v>32.523000000000003</v>
+      </c>
+      <c r="F39" s="8">
+        <f>D39+E39*0.0001</f>
+        <v>0.12925230000000001</v>
+      </c>
+      <c r="G39" s="8">
+        <v>6.7670000000000002E-4</v>
+      </c>
+      <c r="H39">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="I39" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>308</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="8">
+        <v>5.3229999999999997E-7</v>
+      </c>
+      <c r="E40">
+        <v>2.0510000000000002</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" ref="F39:F57" si="1">D40+E40*0.0001</f>
+        <v>2.0563230000000002E-4</v>
+      </c>
+      <c r="G40" s="8">
+        <v>2.1660000000000002E-9</v>
+      </c>
+      <c r="H40">
+        <v>54.19</v>
+      </c>
+      <c r="I40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" s="8">
+        <v>2.8770000000000001E-5</v>
+      </c>
+      <c r="E41">
+        <v>15.753</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="1"/>
+        <v>1.6040700000000002E-3</v>
+      </c>
+      <c r="G41" s="8">
+        <v>6.8670000000000005E-4</v>
+      </c>
+      <c r="H41" s="3">
+        <v>167.13499999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>323</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="E42">
+        <v>102</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.92920000000000003</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>324</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" si="1"/>
+        <v>0.71</v>
+      </c>
+      <c r="G43" s="9">
+        <v>0</v>
+      </c>
+      <c r="H43" s="9">
+        <v>29.77</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>320</v>
+      </c>
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E44">
+        <v>30</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" t="s">
+        <v>231</v>
+      </c>
+      <c r="D45" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E45">
+        <v>32</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4200000000000003E-2</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>313</v>
+      </c>
+      <c r="C46" t="s">
+        <v>232</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.6008</v>
+      </c>
+      <c r="G46" s="9">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>314</v>
+      </c>
+      <c r="C47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E47">
+        <v>22</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G47" s="9">
+        <v>0</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E48">
+        <v>64</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2400000000000001E-2</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2954</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0</v>
+      </c>
+      <c r="H49" s="9">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E50">
+        <v>26</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="G50" s="9">
+        <v>0</v>
+      </c>
+      <c r="H50" s="9">
+        <v>60.76</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="9">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E51">
+        <v>34</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0</v>
+      </c>
+      <c r="H51" s="9">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57979999999999998</v>
+      </c>
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E53">
+        <v>22</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0</v>
+      </c>
+      <c r="H53" s="9">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="9">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E54">
+        <v>22</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="G54" s="9">
+        <v>0</v>
+      </c>
+      <c r="H54" s="9">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="G55" s="9">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E56">
+        <v>18</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="G56" s="9">
+        <v>0</v>
+      </c>
+      <c r="H56" s="9">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D57" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E57">
+        <v>32</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="1"/>
+        <v>1.72E-2</v>
+      </c>
+      <c r="G57" s="9">
+        <v>0</v>
+      </c>
+      <c r="H57" s="9">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0.245</v>
+      </c>
+      <c r="E58">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1">
+        <f>D58+E58*0.0001</f>
+        <v>0.2462</v>
+      </c>
+      <c r="G58" s="9">
+        <v>0</v>
+      </c>
+      <c r="H58" s="9">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E59">
+        <v>18</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" ref="F59" si="2">D59+E59*0.0001</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0</v>
+      </c>
+      <c r="H59" s="9">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E60">
+        <v>64</v>
+      </c>
+      <c r="F60" s="1">
+        <f>D60+E60*0.0001</f>
+        <v>1.2400000000000001E-2</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1">
+        <f>D61+E61*0.0001</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="G61" s="9">
+        <v>0</v>
+      </c>
+      <c r="H61" s="9">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E62">
+        <v>18</v>
+      </c>
+      <c r="F62" s="1">
+        <f>D62+E62*0.0001</f>
+        <v>6.8000000000000005E-3</v>
+      </c>
+      <c r="G62" s="9">
+        <v>0</v>
+      </c>
+      <c r="H62" s="9">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D63" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E63">
+        <v>30</v>
+      </c>
+      <c r="F63" s="1">
+        <f>D63+E63*0.0001</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="G63" s="9">
+        <v>0</v>
+      </c>
+      <c r="H63" s="9">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D64" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E64">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1">
+        <f>D64+E64*0.0001</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0</v>
+      </c>
+      <c r="H64" s="9">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E65">
+        <v>18</v>
+      </c>
+      <c r="F65" s="1">
+        <f>D65+E65*0.0001</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G65" s="9">
+        <v>0</v>
+      </c>
+      <c r="H65" s="9">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>325</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D66" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66" s="1">
+        <f>D66+E66*0.0001</f>
+        <v>4.82E-2</v>
+      </c>
+      <c r="G66" s="9">
+        <v>0</v>
+      </c>
+      <c r="H66" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>326</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0.246</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1">
+        <f>D67+E67*0.0001</f>
+        <v>0.2462</v>
+      </c>
+      <c r="G67" s="9">
+        <v>0</v>
+      </c>
+      <c r="H67" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>327</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D68" s="8">
+        <v>2.5309999999999998E-10</v>
+      </c>
+      <c r="E68">
+        <v>20</v>
+      </c>
+      <c r="F68" s="1">
+        <f>D68+E68*0.0001</f>
+        <v>2.0000002531000002E-3</v>
+      </c>
+      <c r="G68" s="9">
+        <v>0</v>
+      </c>
+      <c r="H68" s="9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>328</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0.749</v>
+      </c>
+      <c r="E69">
+        <v>14</v>
+      </c>
+      <c r="F69" s="1">
+        <f>D69+E69*0.0001</f>
+        <v>0.75039999999999996</v>
+      </c>
+      <c r="G69" s="9">
+        <v>0</v>
+      </c>
+      <c r="H69" s="9">
+        <v>4.5599999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. modify switching time optimization to add target matrix
2. update results of LiH example
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4E3E79-6B83-9A47-9BB1-3B3DE9288FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583855BD-C793-2241-8B62-2D29A00FD9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="413">
   <si>
     <t>Name</t>
   </si>
@@ -885,247 +885,431 @@
     <t>sum_penalty=1.0</t>
   </si>
   <si>
-    <t>alpha=0.0001, beta=0.5, iterations=100</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_minup10.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+TR</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+Minup</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+Maxswitch</t>
+  </si>
+  <si>
+    <t>ADMM+ST</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+ST</t>
+  </si>
+  <si>
+    <t>GRAPE+L2+TRC+ST+Minup</t>
+  </si>
+  <si>
+    <t>ADMM+ST+Minup</t>
+  </si>
+  <si>
+    <t>sum_penalty=0.1</t>
+  </si>
+  <si>
+    <t>alpha=0.001, beta=0.5, iterations=100</t>
+  </si>
+  <si>
+    <t>instance of MoleculeNew example with H2</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8_sigma0.25_
+eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10_sigma0.25_eta0.001_
+threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>instance of MoleculeNew example with LiH</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_
 eta0.001_threshold30_iter100_typetvc.log</t>
   </si>
   <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-minup10.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-SUR.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
-_threshold30_iter100_typetvc_minup10.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
-_threshold30_iter100_typetvc_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.25
-_eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10_sigma0.25_eta0.001
-_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8_sigma0.25_
-eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR_alpha0.0001_sigma0.25_
-eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
-_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>GRAPE+L2+TRC+TR</t>
-  </si>
-  <si>
-    <t>GRAPE+L2+TRC+Minup</t>
-  </si>
-  <si>
-    <t>GRAPE+L2+TRC+Maxswitch</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
-_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8_sigma0.25_eta0.001_
-threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10_sigma0.25_eta0.001_
-threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_
-maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>instance of molecule example with H2</t>
-  </si>
-  <si>
-    <t>ADMM+ST</t>
-  </si>
-  <si>
-    <t>GRAPE+L2+TRC+ST</t>
-  </si>
-  <si>
-    <t>GRAPE+L2+TRC+ST+Minup</t>
-  </si>
-  <si>
-    <t>ADMM+ST+Minup</t>
-  </si>
-  <si>
-    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.0.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.5.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.0.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.5.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime5.0_n_ts100_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001
-_threshold30_iter100_typetvc_minup10.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8_sigma0.25_
-eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR_alpha0.0001_sigma0.25_
-eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_
-eta0.001_threshold30_iter100_typetvc.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch2_initwarm_minuptime0.0.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch2_initwarm_minuptime0.5.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch10_initwarm_minuptime0.0.log</t>
-  </si>
-  <si>
-    <t>MoleculeST_LiH_evotime_15.0_n_ts150_n_switch10_initwarm_minuptime0.5.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_minup10.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_SUR.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.00_threshold30_iter100_typetvc_maxswitch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.2_eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>MoleculeADMM_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.0001_ADMM_0.5_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>Molecule_LiH_evotime15.0_n_ts150_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
-  </si>
-  <si>
-    <t>instance of molecule example with LiH</t>
-  </si>
-  <si>
-    <t>sum_penalty=0.1</t>
-  </si>
-  <si>
-    <t>Molecule2_LiH_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_sum_penalty1.0_penalty0.001_ADMM_0.5_iter100_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>MoleculeSTNew_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeSTNew_H2_evotime_4.0_n_ts80_n_switch2_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeSTNew_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeSTNew_H2_evotime_4.0_n_ts80_n_switch10_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty1.0_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_minup10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_SUR.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_minup10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime8.0_n_ts80_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>HadamardST2_evotime_8.0_n_ts80_n_switch7_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST2_evotime_8.0_n_ts80_n_switch7_initwarm_minuptime1.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST2_evotime_8.0_n_ts80_n_switch14_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST2_evotime_8.0_n_ts80_n_switch14_initwarm_minuptime1.0.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_minup10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup10_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc_maxswitch8_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM2_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_alpha0.0001_sigma0.25_eta0.001_threshold30_iter100_typetvc.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_minup10.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_minup10.log</t>
+  </si>
+  <si>
+    <t>HadamardADMM3_evotime12.0_n_ts120_ptypeWARM_offset0.5_sum_penalty0.01_penalty0.0001_ADMM_0.5_iter100_SUR.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.log</t>
+  </si>
+  <si>
+    <t>Hadamard2_evotime8.0_n_ts80_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_maxswitch8.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0_maxswitch12.log</t>
+  </si>
+  <si>
+    <t>Hadamard3_evotime12.0_n_ts120_ptypeWARM_offset0.5_objUNIT_sum_penalty0.01_maxswitch12.log</t>
+  </si>
+  <si>
+    <t>HadamardST3_evotime_12.0_n_ts120_n_switch17_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST3_evotime_12.0_n_ts120_n_switch17_initwarm_minuptime1.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST3_evotime_8.0_n_ts80_n_switch49_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>HadamardST3_evotime_8.0_n_ts80_n_switch49_initwarm_minuptime1.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew_H2_evotime4.0_n_ts80_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1</t>
+  </si>
+  <si>
+    <t>min-up-time steps: 10</t>
+  </si>
+  <si>
+    <t>min-up time steps: 5</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_H2_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_minup5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_maxswitch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_minup5.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_maxswitch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.001
+_threshold30_iter100_typetvc_minup5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.00_threshold30_iter100_typetvc_maxswitch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_SUR_alpha0.001_sigma0.2_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_minup5_sigma0.25_eta0.001_threshold30_iter100_typeminup_time5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.0_maxswitch40_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_minup5_sigma0.25_eta0.001_threshold30_iter100_typeminup_time10.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_maxswitch40_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_minup5_sigma0.25_eta0.001_threshold30_iter100_typeminup_time5.log</t>
+  </si>
+  <si>
+    <t>MoleculeADMMNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_sum_penalty0.1_penalty0.001_ADMM_0.5_iter100_maxswitch40_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeCONSTANT_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_SUR_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetv.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.001_threshold30_iter100_typetvc_minup5_sigma0.25_eta0.001_threshold30_iter100_typeminup_time5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNew3_LiH_evotime20.0_n_ts200_ptypeWARM_offset0.5_objUNIT_sum_penalty0.1_alpha0.001_sigma0.25_eta0.00_threshold30_iter100_typetvc_maxswitch40_sigma0.25_eta0.001_threshold30_iter100_typemaxswitch_switch40.log</t>
+  </si>
+  <si>
+    <t>MoleculeNewST_LiH_evotime_20.0_n_ts200_n_switch8_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeNewST_LiH_evotime_20.0_n_ts200_n_switch8_initwarm_minuptime0.5.log</t>
+  </si>
+  <si>
+    <t>MoleculeNewST_LiH_evotime_20.0_n_ts200_n_switch38_initwarm_minuptime0.0.log</t>
+  </si>
+  <si>
+    <t>MoleculeNewST_LiH_evotime_20.0_n_ts200_n_switch38_initwarm_minuptime0.5.log</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1231,6 +1415,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1547,7 +1734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" workbookViewId="0">
       <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
@@ -4117,7 +4304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C89" sqref="C89:C91"/>
     </sheetView>
   </sheetViews>
@@ -6064,14 +6251,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0842C86B-7D36-B04D-B09B-8D3C95D38C2E}">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I1"/>
+    <sheetView zoomScale="67" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="89.6640625" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="9" max="9" width="45.1640625" customWidth="1"/>
@@ -6101,6 +6289,9 @@
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>317</v>
+      </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
@@ -6122,6 +6313,9 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>318</v>
+      </c>
       <c r="C3" t="s">
         <v>229</v>
       </c>
@@ -6131,6 +6325,10 @@
       <c r="E3">
         <v>18.867999999999999</v>
       </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F33" si="0">D3+E3*0.0001</f>
+        <v>1.886801559E-3</v>
+      </c>
       <c r="G3" s="8">
         <v>6.9650000000000002E-7</v>
       </c>
@@ -6141,122 +6339,1501 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>319</v>
+      </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
+      <c r="D4" s="8">
+        <v>1.2480000000000001E-7</v>
+      </c>
+      <c r="E4">
+        <v>3.698</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>3.6992479999999999E-4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.156E-4</v>
+      </c>
+      <c r="H4">
+        <v>36.82</v>
+      </c>
       <c r="I4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>320</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="D5" s="8">
+        <v>1.011E-5</v>
+      </c>
+      <c r="E5">
+        <v>17.265000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7366100000000002E-3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.2279999999999998E-4</v>
+      </c>
+      <c r="H5">
+        <v>153.77000000000001</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>272</v>
+      </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
+      <c r="D6" s="9">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E6">
+        <v>126</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.81859999999999999</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>273</v>
+      </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
+      <c r="D7" s="9">
+        <v>0.876</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.877</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>15.72</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
+      <c r="D8" s="9">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>19.07</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>321</v>
+      </c>
       <c r="C9" t="s">
         <v>231</v>
       </c>
+      <c r="D9" s="9">
+        <v>0.193</v>
+      </c>
+      <c r="E9">
+        <v>136</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.94</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>322</v>
+      </c>
       <c r="C10" t="s">
         <v>232</v>
       </c>
+      <c r="D10" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.95119999999999993</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1.19</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>371</v>
+      </c>
       <c r="C11" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="9">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67220000000000002</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>18.78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="9">
+        <v>0.224</v>
+      </c>
+      <c r="E12">
+        <v>154</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2394</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="9">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90580000000000005</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>325</v>
+      </c>
       <c r="C14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="9">
+        <v>0.747</v>
+      </c>
+      <c r="E14">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75019999999999998</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="C15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="9">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E15">
+        <v>136</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="C16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="9">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60439999999999994</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>328</v>
+      </c>
       <c r="C17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" s="9">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="E17">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.62119999999999997</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>60.62</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" s="9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E18">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>330</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D19" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.62719999999999998</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>17.420000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>331</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" s="9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9000000000000004E-2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D21" s="9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E21">
+        <v>128</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>333</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D22" s="9">
+        <v>0.216</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21809999999999999</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>13.87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>334</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D23" s="9">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E23">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10579999999999999</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D24" s="9">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E24">
+        <v>154</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8399999999999997E-2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="3:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D25" s="9">
+        <v>0.193</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1938</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>337</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.126</v>
+      </c>
+      <c r="E26">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E27">
+        <v>134</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3448</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D29" s="9">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>4.02E-2</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>20.18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D30" s="9">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.95439999999999992</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D32" s="8">
+        <v>5.3090000000000002E-5</v>
+      </c>
+      <c r="E32">
+        <v>22</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2530900000000001E-3</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="E33">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91039999999999999</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>370</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E39">
+        <v>50.935000000000002</v>
+      </c>
+      <c r="F39" s="1">
+        <f>D39+E39*0.0001</f>
+        <v>0.1030935</v>
+      </c>
+      <c r="G39" s="1">
+        <v>555.36699999999996</v>
+      </c>
+      <c r="H39">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>362</v>
+      </c>
+      <c r="C40" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="8">
+        <v>3.5870000000000003E-8</v>
+      </c>
+      <c r="E40">
+        <v>75.215999999999994</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" ref="F40:F70" si="1">D40+E40*0.0001</f>
+        <v>7.5216358699999996E-3</v>
+      </c>
+      <c r="G40" s="8">
+        <v>5.9340000000000003E-6</v>
+      </c>
+      <c r="H40">
+        <v>24.83</v>
+      </c>
+      <c r="I40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.8770000000000002E-5</v>
+      </c>
+      <c r="E41">
+        <v>15.026999999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="1"/>
+        <v>1.52147E-3</v>
+      </c>
+      <c r="G41" s="8">
+        <v>1.156E-4</v>
+      </c>
+      <c r="H41">
+        <v>110.19</v>
+      </c>
+      <c r="I41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1.1070000000000001E-5</v>
+      </c>
+      <c r="E42">
+        <v>74.037999999999997</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4148700000000005E-3</v>
+      </c>
+      <c r="G42" s="8">
+        <v>8.5979999999999997E-4</v>
+      </c>
+      <c r="H42">
+        <v>390.11</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="20">
+        <v>0.749</v>
+      </c>
+      <c r="E43" s="19">
+        <v>168</v>
+      </c>
+      <c r="F43" s="21">
+        <f t="shared" si="1"/>
+        <v>0.76580000000000004</v>
+      </c>
+      <c r="G43" s="20">
+        <v>0</v>
+      </c>
+      <c r="H43" s="19">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>366</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="E44">
+        <v>16</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.9556</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0</v>
+      </c>
+      <c r="H44" s="9">
+        <v>41.06</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>372</v>
+      </c>
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="E45">
+        <v>70</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>367</v>
+      </c>
+      <c r="C46" t="s">
+        <v>231</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E46">
+        <v>166</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.60059999999999991</v>
+      </c>
+      <c r="G46" s="9">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>368</v>
+      </c>
+      <c r="C47" t="s">
+        <v>232</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="E47">
+        <v>18</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94979999999999998</v>
+      </c>
+      <c r="G47" s="9">
+        <v>0</v>
+      </c>
+      <c r="H47" s="9">
+        <v>11.21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>373</v>
+      </c>
+      <c r="C48" t="s">
+        <v>233</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="E48">
+        <v>66</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77260000000000006</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E49">
+        <v>220</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0</v>
+      </c>
+      <c r="H49" s="9">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="9">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="E50">
+        <v>22</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79820000000000002</v>
+      </c>
+      <c r="G50" s="9">
+        <v>0</v>
+      </c>
+      <c r="H50" s="9">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="9">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="E51">
+        <v>68</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93480000000000008</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0</v>
+      </c>
+      <c r="H51" s="9">
+        <v>61.97</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.623</v>
+      </c>
+      <c r="E52">
+        <v>168</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.63980000000000004</v>
+      </c>
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="9">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="1"/>
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0</v>
+      </c>
+      <c r="H53" s="9">
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="E54">
+        <v>70</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="G54" s="9">
+        <v>0</v>
+      </c>
+      <c r="H54" s="9">
+        <v>62.05</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="9">
+        <v>0.156</v>
+      </c>
+      <c r="E55">
+        <v>144</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1704</v>
+      </c>
+      <c r="G55" s="9">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <v>34.67</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="9">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="E56">
+        <v>14</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30740000000000001</v>
+      </c>
+      <c r="G56" s="9">
+        <v>0</v>
+      </c>
+      <c r="H56" s="9">
+        <v>23.94</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="9">
+        <v>0.221</v>
+      </c>
+      <c r="E57">
+        <v>54</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="1"/>
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="G57" s="9">
+        <v>0</v>
+      </c>
+      <c r="H57" s="9">
+        <v>33.71</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E58">
+        <v>160</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16099999999999998</v>
+      </c>
+      <c r="G58" s="9">
+        <v>0</v>
+      </c>
+      <c r="H58" s="9">
+        <v>18.010000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D59" s="9">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E59">
+        <v>14</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39840000000000003</v>
+      </c>
+      <c r="G59" s="9">
+        <v>0</v>
+      </c>
+      <c r="H59" s="9">
+        <v>38.22</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" s="9">
+        <v>0.23</v>
+      </c>
+      <c r="E60">
+        <v>72</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23720000000000002</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9">
+        <v>30.65</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E61">
+        <v>212</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1542</v>
+      </c>
+      <c r="G61" s="9">
+        <v>0</v>
+      </c>
+      <c r="H61" s="9">
+        <v>13.72</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E62">
+        <v>14</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4264</v>
+      </c>
+      <c r="G62" s="9">
+        <v>0</v>
+      </c>
+      <c r="H62" s="9">
+        <v>30.65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="9">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E63">
+        <v>62</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17120000000000002</v>
+      </c>
+      <c r="G63" s="9">
+        <v>0</v>
+      </c>
+      <c r="H63" s="9">
+        <v>36.51</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D64" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="E64">
+        <v>170</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="1"/>
+        <v>0.187</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0</v>
+      </c>
+      <c r="H64" s="9">
+        <v>28.23</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0.435</v>
+      </c>
+      <c r="E65">
+        <v>14</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="1"/>
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="G65" s="9">
+        <v>0</v>
+      </c>
+      <c r="H65" s="9">
+        <v>29.64</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E66">
+        <v>50</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="G66" s="9">
+        <v>0</v>
+      </c>
+      <c r="H66" s="9">
+        <v>41.58</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="E67">
+        <v>28</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="G67" s="9">
+        <v>0</v>
+      </c>
+      <c r="H67" s="9">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B68" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
+      <c r="F68" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93920000000000003</v>
+      </c>
+      <c r="G68" s="9">
+        <v>0</v>
+      </c>
+      <c r="H68" s="9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B69" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D69" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E69">
+        <v>22</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7200000000000002E-2</v>
+      </c>
+      <c r="G69" s="9">
+        <v>0</v>
+      </c>
+      <c r="H69" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B70" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="E70">
+        <v>22</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93020000000000003</v>
+      </c>
+      <c r="G70" s="9">
+        <v>0</v>
+      </c>
+      <c r="H70" s="9">
+        <v>0.74</v>
       </c>
     </row>
   </sheetData>
@@ -6268,14 +7845,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
   <dimension ref="B1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="101" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.2">
@@ -6303,7 +7881,7 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>319</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -6314,9 +7892,9 @@
       <c r="E2">
         <v>25.515999999999998</v>
       </c>
-      <c r="F2" s="8">
-        <f>D2+E2*0.0001</f>
-        <v>2.5520368E-3</v>
+      <c r="F2" s="1">
+        <f>D2+E2*0.001</f>
+        <v>2.55164368E-2</v>
       </c>
       <c r="G2">
         <v>167.48099999999999</v>
@@ -6325,12 +7903,12 @@
         <v>1.42</v>
       </c>
       <c r="I2" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="C3" t="s">
         <v>229</v>
@@ -6341,9 +7919,9 @@
       <c r="E3" s="1">
         <v>18.72</v>
       </c>
-      <c r="F3" s="8">
-        <f t="shared" ref="F3:F23" si="0">D3+E3*0.0001</f>
-        <v>1.8722483000000001E-3</v>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F33" si="0">D3+E3*0.001</f>
+        <v>1.8720248299999999E-2</v>
       </c>
       <c r="G3" s="8">
         <v>5.553E-7</v>
@@ -6357,58 +7935,58 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="8">
-        <v>5.3229999999999997E-7</v>
+        <v>1.326E-5</v>
       </c>
       <c r="E4">
-        <v>2.0510000000000002</v>
-      </c>
-      <c r="F4" s="8">
+        <v>2.7440000000000002</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>2.0563230000000002E-4</v>
+        <v>2.7572600000000005E-3</v>
       </c>
       <c r="G4" s="8">
-        <v>2.1660000000000002E-9</v>
+        <v>3.0629999999999998E-7</v>
       </c>
       <c r="H4">
-        <v>54.19</v>
+        <v>39.86</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>230</v>
       </c>
       <c r="D5" s="8">
-        <v>2.8770000000000001E-5</v>
+        <v>1.237E-4</v>
       </c>
       <c r="E5">
-        <v>15.753</v>
-      </c>
-      <c r="F5" s="8">
+        <v>8.4209999999999994</v>
+      </c>
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>1.6040700000000002E-3</v>
-      </c>
-      <c r="G5" s="8">
-        <v>6.8670000000000005E-4</v>
+        <v>8.5446999999999988E-3</v>
+      </c>
+      <c r="G5" s="9">
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H5" s="3">
-        <v>167.13499999999999</v>
+        <v>154.05000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -6419,20 +7997,23 @@
       <c r="E6">
         <v>102</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>0.92920000000000003</v>
+        <v>1.0210000000000001</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" s="9">
-        <v>0.89</v>
+        <v>0.85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -6445,42 +8026,42 @@
       </c>
       <c r="F7" s="9">
         <f t="shared" si="0"/>
-        <v>0.71</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="G7" s="9">
         <v>0</v>
       </c>
       <c r="H7" s="9">
-        <v>29.77</v>
+        <v>32.47</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9">
-        <v>0.89500000000000002</v>
+      <c r="D8" s="1">
+        <v>0.77</v>
       </c>
       <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1">
+        <v>26</v>
+      </c>
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>0.89800000000000002</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="G8" s="9">
         <v>0</v>
       </c>
       <c r="H8" s="9">
-        <v>1.77</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="C9" t="s">
         <v>231</v>
@@ -6491,44 +8072,44 @@
       <c r="E9">
         <v>32</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
-        <v>2.4200000000000003E-2</v>
+        <v>5.3000000000000005E-2</v>
       </c>
       <c r="G9" s="9">
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <v>0.91800000000000004</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C10" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="1">
         <v>0.6</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
-        <v>0.6008</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="G10" s="9">
         <v>0</v>
       </c>
       <c r="H10" s="9">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C11" t="s">
         <v>233</v>
@@ -6539,81 +8120,81 @@
       <c r="E11">
         <v>22</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>2.8199999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G11" s="9">
         <v>0</v>
       </c>
       <c r="H11" s="9">
-        <v>1.42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="9">
-        <v>6.0000000000000001E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="E12">
-        <v>64</v>
-      </c>
-      <c r="F12" s="1">
+        <v>80</v>
+      </c>
+      <c r="F12" s="9">
         <f t="shared" si="0"/>
-        <v>1.2400000000000001E-2</v>
+        <v>0.11599999999999999</v>
       </c>
       <c r="G12" s="9">
         <v>0</v>
       </c>
       <c r="H12" s="9">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="51" x14ac:dyDescent="0.2">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="9">
-        <v>0.29499999999999998</v>
+        <v>6.3E-2</v>
       </c>
       <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>0.2954</v>
+        <v>7.1000000000000008E-2</v>
       </c>
       <c r="G13" s="9">
         <v>0</v>
       </c>
       <c r="H13" s="9">
-        <v>2.27</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="9">
-        <v>5.3999999999999999E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E14">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>5.6599999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
@@ -6624,127 +8205,127 @@
     </row>
     <row r="15" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="C15" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="9">
-        <v>2.8000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E15">
         <v>34</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
-        <v>3.1399999999999997E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="G15" s="9">
         <v>0</v>
       </c>
       <c r="H15" s="9">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="9">
-        <v>0.57899999999999996</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="9">
         <f t="shared" si="0"/>
-        <v>0.57979999999999998</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="9">
-        <v>2.5999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E17">
-        <v>22</v>
-      </c>
-      <c r="F17" s="1">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>2.8199999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="G17" s="9">
         <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>1.73</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="9">
-        <v>2.4E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E18">
-        <v>22</v>
-      </c>
-      <c r="F18" s="1">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9">
         <f t="shared" si="0"/>
-        <v>2.6200000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G18" s="9">
         <v>0</v>
       </c>
       <c r="H18" s="9">
-        <v>6.88</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="9">
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="9">
         <f t="shared" si="0"/>
-        <v>7.4000000000000003E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G19" s="9">
         <v>0</v>
       </c>
-      <c r="H19" s="9">
-        <v>5.57</v>
+      <c r="H19" s="3">
+        <v>5.4</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
@@ -6755,33 +8336,33 @@
       <c r="E20">
         <v>18</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
-        <v>4.8000000000000004E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G20" s="9">
         <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>5.35</v>
+        <v>4.88</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D21" s="9">
-        <v>1.4E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="E21">
-        <v>32</v>
-      </c>
-      <c r="F21" s="1">
+        <v>28</v>
+      </c>
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
-        <v>1.72E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G21" s="9">
         <v>0</v>
@@ -6792,7 +8373,7 @@
     </row>
     <row r="22" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>235</v>
@@ -6803,20 +8384,20 @@
       <c r="E22">
         <v>12</v>
       </c>
-      <c r="F22" s="1">
-        <f>D22+E22*0.0001</f>
-        <v>0.2462</v>
+      <c r="F22" s="9">
+        <f t="shared" si="0"/>
+        <v>0.25700000000000001</v>
       </c>
       <c r="G22" s="9">
         <v>0</v>
       </c>
       <c r="H22" s="9">
-        <v>15.67</v>
+        <v>16.73</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>236</v>
@@ -6827,177 +8408,177 @@
       <c r="E23">
         <v>18</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="9">
         <f t="shared" si="0"/>
-        <v>1.5800000000000002E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="G23" s="9">
         <v>0</v>
       </c>
       <c r="H23" s="9">
-        <v>2.81</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="9">
-        <v>6.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E24">
-        <v>64</v>
-      </c>
-      <c r="F24" s="1">
-        <f>D24+E24*0.0001</f>
-        <v>1.2400000000000001E-2</v>
+        <v>68</v>
+      </c>
+      <c r="F24" s="9">
+        <f>D24+E24*0.001</f>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="G24" s="9">
         <v>0</v>
       </c>
-      <c r="H24" s="9">
-        <v>1.8</v>
+      <c r="H24" s="3">
+        <v>4.7</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="9">
-        <v>7.0000000000000001E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25" s="1">
-        <f>D25+E25*0.0001</f>
-        <v>7.1999999999999998E-3</v>
+        <v>10</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G25" s="9">
         <v>0</v>
       </c>
       <c r="H25" s="9">
-        <v>6.38</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="9">
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E26">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1">
-        <f>D26+E26*0.0001</f>
-        <v>6.8000000000000005E-3</v>
+        <f t="shared" si="0"/>
+        <v>0.03</v>
       </c>
       <c r="G26" s="9">
         <v>0</v>
       </c>
       <c r="H26" s="9">
-        <v>5.85</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D27" s="9">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E27">
-        <v>30</v>
-      </c>
-      <c r="F27" s="1">
-        <f>D27+E27*0.0001</f>
-        <v>1.6E-2</v>
+        <v>32</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G27" s="9">
         <v>0</v>
       </c>
       <c r="H27" s="9">
-        <v>2.91</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D28" s="9">
-        <v>5.3999999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E28">
-        <v>10</v>
-      </c>
-      <c r="F28" s="1">
-        <f>D28+E28*0.0001</f>
-        <v>5.5E-2</v>
+        <v>2</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="0"/>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="G28" s="9">
         <v>0</v>
       </c>
       <c r="H28" s="9">
-        <v>4.8099999999999996</v>
+        <v>9.2100000000000009</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D29" s="9">
-        <v>1.4E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E29">
-        <v>18</v>
-      </c>
-      <c r="F29" s="1">
-        <f>D29+E29*0.0001</f>
-        <v>1.5800000000000002E-2</v>
+        <v>22</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="G29" s="9">
         <v>0</v>
       </c>
       <c r="H29" s="9">
-        <v>2.85</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="D30" s="9">
-        <v>4.8000000000000001E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1">
-        <f>D30+E30*0.0001</f>
-        <v>4.82E-2</v>
+        <v>4</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G30" s="9">
         <v>0</v>
@@ -7008,851 +8589,854 @@
     </row>
     <row r="31" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="D31" s="9">
-        <v>0.246</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
-      <c r="F31" s="1">
-        <f>D31+E31*0.0001</f>
-        <v>0.2462</v>
+      <c r="F31" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13300000000000001</v>
       </c>
       <c r="G31" s="9">
         <v>0</v>
       </c>
       <c r="H31" s="9">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D32" s="8">
-        <v>2.5309999999999998E-10</v>
+        <v>279</v>
+      </c>
+      <c r="D32" s="9">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E32">
-        <v>20</v>
-      </c>
-      <c r="F32" s="1">
-        <f>D32+E32*0.0001</f>
-        <v>2.0000002531000002E-3</v>
+        <v>8</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="G32" s="9">
         <v>0</v>
       </c>
       <c r="H32" s="9">
-        <v>0.21</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="D33" s="9">
-        <v>0.749</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="E33">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1">
-        <f>D33+E33*0.0001</f>
-        <v>0.75039999999999996</v>
+        <v>8</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="0"/>
+        <v>0.71399999999999997</v>
       </c>
       <c r="G33" s="9">
         <v>0</v>
       </c>
       <c r="H33" s="9">
-        <v>4.5599999999999996</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>345</v>
+        <v>382</v>
       </c>
       <c r="C38" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="8">
-        <v>4.5999999999999999E-2</v>
+        <v>2.683E-6</v>
       </c>
       <c r="E38">
-        <v>339.31900000000002</v>
-      </c>
-      <c r="F38" s="8">
-        <f>D38+E38*0.0001</f>
-        <v>7.99319E-2</v>
+        <v>487.33</v>
+      </c>
+      <c r="F38" s="1">
+        <f>D38+E38*0.001</f>
+        <v>0.48733268299999999</v>
       </c>
       <c r="G38">
-        <v>7090.22</v>
+        <v>6966.2030000000004</v>
       </c>
       <c r="H38">
-        <v>327.06</v>
+        <v>585.96</v>
       </c>
       <c r="I38" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>307</v>
+        <v>379</v>
       </c>
       <c r="C39" t="s">
         <v>229</v>
       </c>
-      <c r="D39" s="8">
-        <v>0.126</v>
+      <c r="D39" s="1">
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="E39" s="1">
-        <v>32.523000000000003</v>
-      </c>
-      <c r="F39" s="8">
-        <f>D39+E39*0.0001</f>
-        <v>0.12925230000000001</v>
-      </c>
-      <c r="G39" s="8">
-        <v>6.7670000000000002E-4</v>
+        <v>61.305</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" ref="F39:F69" si="1">D39+E39*0.001</f>
+        <v>0.120305</v>
+      </c>
+      <c r="G39" s="9">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H39">
-        <v>75.040000000000006</v>
+        <v>427.35</v>
       </c>
       <c r="I39" t="s">
-        <v>344</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>308</v>
+        <v>384</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="8">
-        <v>5.3229999999999997E-7</v>
+      <c r="D40" s="9">
+        <v>6.2E-2</v>
       </c>
       <c r="E40">
-        <v>2.0510000000000002</v>
-      </c>
-      <c r="F40" s="8">
-        <f t="shared" ref="F39:F57" si="1">D40+E40*0.0001</f>
-        <v>2.0563230000000002E-4</v>
-      </c>
-      <c r="G40" s="8">
-        <v>2.1660000000000002E-9</v>
+        <v>9.7609999999999992</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="1"/>
+        <v>7.1760999999999991E-2</v>
+      </c>
+      <c r="G40" s="9">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H40">
-        <v>54.19</v>
+        <v>647.66999999999996</v>
       </c>
       <c r="I40" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D41" s="8">
-        <v>2.8770000000000001E-5</v>
+      <c r="D41" s="9">
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="E41">
-        <v>15.753</v>
-      </c>
-      <c r="F41" s="8">
+        <v>57.478999999999999</v>
+      </c>
+      <c r="F41" s="1">
         <f t="shared" si="1"/>
-        <v>1.6040700000000002E-3</v>
-      </c>
-      <c r="G41" s="8">
-        <v>6.8670000000000005E-4</v>
+        <v>0.116479</v>
+      </c>
+      <c r="G41" s="9">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H41" s="3">
-        <v>167.13499999999999</v>
+        <v>1170.396</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>323</v>
+        <v>385</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
       </c>
       <c r="D42" s="9">
-        <v>0.91900000000000004</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="E42">
-        <v>102</v>
+        <v>288</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="1"/>
-        <v>0.92920000000000003</v>
+        <v>1.256</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42" s="9">
-        <v>0.89</v>
+        <v>12.45</v>
+      </c>
+      <c r="I42" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>324</v>
+        <v>386</v>
       </c>
       <c r="C43" t="s">
         <v>30</v>
       </c>
       <c r="D43" s="9">
-        <v>0.70899999999999996</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="E43">
-        <v>10</v>
-      </c>
-      <c r="F43" s="9">
+        <v>44</v>
+      </c>
+      <c r="F43" s="1">
         <f t="shared" si="1"/>
-        <v>0.71</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="G43" s="9">
         <v>0</v>
       </c>
-      <c r="H43" s="9">
-        <v>29.77</v>
+      <c r="H43" s="3">
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="C44" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="9">
-        <v>0.89500000000000002</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="E44">
-        <v>30</v>
+        <v>196</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="1"/>
-        <v>0.89800000000000002</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="G44" s="9">
         <v>0</v>
       </c>
       <c r="H44" s="9">
-        <v>1.77</v>
+        <v>13.23</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>312</v>
+        <v>388</v>
       </c>
       <c r="C45" t="s">
         <v>231</v>
       </c>
       <c r="D45" s="9">
-        <v>2.1000000000000001E-2</v>
+        <v>0.183</v>
       </c>
       <c r="E45">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="1"/>
-        <v>2.4200000000000003E-2</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="G45" s="9">
         <v>0</v>
       </c>
       <c r="H45" s="3">
-        <v>0.91800000000000004</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>313</v>
+        <v>389</v>
       </c>
       <c r="C46" t="s">
         <v>232</v>
       </c>
       <c r="D46" s="9">
-        <v>0.6</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="E46">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="1"/>
-        <v>0.6008</v>
+        <v>1.03</v>
       </c>
       <c r="G46" s="9">
         <v>0</v>
       </c>
       <c r="H46" s="9">
-        <v>0.92</v>
+        <v>72.52</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>314</v>
+        <v>390</v>
       </c>
       <c r="C47" t="s">
         <v>233</v>
       </c>
       <c r="D47" s="9">
-        <v>2.5999999999999999E-2</v>
+        <v>0.186</v>
       </c>
       <c r="E47">
-        <v>22</v>
+        <v>270</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="1"/>
-        <v>2.8199999999999999E-2</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="G47" s="9">
         <v>0</v>
       </c>
       <c r="H47" s="9">
-        <v>1.42</v>
+        <v>44.21</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>331</v>
+        <v>391</v>
       </c>
       <c r="C48" t="s">
         <v>32</v>
       </c>
       <c r="D48" s="9">
-        <v>6.0000000000000001E-3</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="E48">
-        <v>64</v>
+        <v>384</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="1"/>
-        <v>1.2400000000000001E-2</v>
+        <v>0.56099999999999994</v>
       </c>
       <c r="G48" s="9">
         <v>0</v>
       </c>
       <c r="H48" s="9">
-        <v>1.19</v>
+        <v>71.34</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>330</v>
+        <v>392</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="9">
-        <v>0.29499999999999998</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="1"/>
-        <v>0.2954</v>
+        <v>0.877</v>
       </c>
       <c r="G49" s="9">
         <v>0</v>
       </c>
       <c r="H49" s="9">
-        <v>2.27</v>
+        <v>70.92</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>329</v>
+        <v>393</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="9">
-        <v>5.3999999999999999E-2</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="E50">
-        <v>26</v>
+        <v>342</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="1"/>
-        <v>5.6599999999999998E-2</v>
+        <v>0.746</v>
       </c>
       <c r="G50" s="9">
         <v>0</v>
       </c>
       <c r="H50" s="9">
-        <v>60.76</v>
+        <v>70.849999999999994</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>315</v>
+        <v>394</v>
       </c>
       <c r="C51" t="s">
         <v>59</v>
       </c>
       <c r="D51" s="9">
-        <v>2.8000000000000001E-2</v>
+        <v>0.184</v>
       </c>
       <c r="E51">
-        <v>34</v>
+        <v>278</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="1"/>
-        <v>3.1399999999999997E-2</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="G51" s="9">
         <v>0</v>
       </c>
       <c r="H51" s="9">
-        <v>0.92</v>
+        <v>27.04</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>316</v>
+        <v>395</v>
       </c>
       <c r="C52" t="s">
         <v>35</v>
       </c>
       <c r="D52" s="9">
-        <v>0.57899999999999996</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="1"/>
-        <v>0.57979999999999998</v>
+        <v>1.0569999999999999</v>
       </c>
       <c r="G52" s="9">
         <v>0</v>
       </c>
       <c r="H52" s="9">
-        <v>0.88</v>
+        <v>70.83</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>332</v>
+        <v>396</v>
       </c>
       <c r="C53" t="s">
         <v>36</v>
       </c>
       <c r="D53" s="9">
-        <v>2.5999999999999999E-2</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="E53">
-        <v>22</v>
+        <v>264</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="1"/>
-        <v>2.8199999999999999E-2</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="G53" s="9">
         <v>0</v>
       </c>
       <c r="H53" s="9">
-        <v>1.73</v>
+        <v>40.54</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>333</v>
+        <v>397</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D54" s="9">
-        <v>2.4E-2</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="E54">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="1"/>
-        <v>2.6200000000000001E-2</v>
+        <v>0.749</v>
       </c>
       <c r="G54" s="9">
         <v>0</v>
       </c>
-      <c r="H54" s="9">
-        <v>6.88</v>
+      <c r="H54" s="3">
+        <v>39.9</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>342</v>
+        <v>398</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D55" s="9">
-        <v>7.0000000000000001E-3</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="1"/>
-        <v>7.4000000000000003E-3</v>
+        <v>0.85200000000000009</v>
       </c>
       <c r="G55" s="9">
         <v>0</v>
       </c>
       <c r="H55" s="9">
-        <v>5.57</v>
+        <v>88.08</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>317</v>
+        <v>399</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D56" s="9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="E56">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="1"/>
-        <v>4.8000000000000004E-3</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="G56" s="9">
         <v>0</v>
       </c>
       <c r="H56" s="9">
-        <v>5.35</v>
+        <v>22.98</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
-        <v>318</v>
+        <v>400</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D57" s="9">
-        <v>1.4E-2</v>
+        <v>0.183</v>
       </c>
       <c r="E57">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="1"/>
-        <v>1.72E-2</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="G57" s="9">
         <v>0</v>
       </c>
       <c r="H57" s="9">
-        <v>3.21</v>
+        <v>9.67</v>
       </c>
     </row>
     <row r="58" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
-        <v>341</v>
+        <v>401</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="9">
-        <v>0.245</v>
+      <c r="D58" s="1">
+        <v>0.62</v>
       </c>
       <c r="E58">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F58" s="1">
-        <f>D58+E58*0.0001</f>
-        <v>0.2462</v>
+        <f t="shared" si="1"/>
+        <v>0.64</v>
       </c>
       <c r="G58" s="9">
         <v>0</v>
       </c>
       <c r="H58" s="9">
-        <v>15.67</v>
+        <v>60.18</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>340</v>
+        <v>402</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>236</v>
       </c>
       <c r="D59" s="9">
-        <v>1.4E-2</v>
+        <v>0.186</v>
       </c>
       <c r="E59">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" ref="F59" si="2">D59+E59*0.0001</f>
-        <v>1.5800000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.45600000000000002</v>
       </c>
       <c r="G59" s="9">
         <v>0</v>
       </c>
       <c r="H59" s="9">
-        <v>2.81</v>
+        <v>10.55</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>339</v>
+        <v>403</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D60" s="9">
-        <v>6.0000000000000001E-3</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="E60">
-        <v>64</v>
+        <v>384</v>
       </c>
       <c r="F60" s="1">
-        <f>D60+E60*0.0001</f>
-        <v>1.2400000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.56099999999999994</v>
       </c>
       <c r="G60" s="9">
         <v>0</v>
       </c>
       <c r="H60" s="9">
-        <v>1.8</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>338</v>
+        <v>404</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D61" s="9">
-        <v>7.0000000000000001E-3</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="E61">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="F61" s="1">
-        <f>D61+E61*0.0001</f>
-        <v>7.1999999999999998E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.55699999999999994</v>
       </c>
       <c r="G61" s="9">
         <v>0</v>
       </c>
       <c r="H61" s="9">
-        <v>6.38</v>
+        <v>96.51</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>337</v>
+        <v>405</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D62" s="9">
-        <v>5.0000000000000001E-3</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="E62">
-        <v>18</v>
+        <v>342</v>
       </c>
       <c r="F62" s="1">
-        <f>D62+E62*0.0001</f>
-        <v>6.8000000000000005E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.53600000000000003</v>
       </c>
       <c r="G62" s="9">
         <v>0</v>
       </c>
       <c r="H62" s="9">
-        <v>5.85</v>
+        <v>42.98</v>
       </c>
     </row>
     <row r="63" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>336</v>
+        <v>406</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D63" s="9">
-        <v>1.2999999999999999E-2</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="E63">
-        <v>30</v>
+        <v>278</v>
       </c>
       <c r="F63" s="1">
-        <f>D63+E63*0.0001</f>
-        <v>1.6E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.44600000000000006</v>
       </c>
       <c r="G63" s="9">
         <v>0</v>
       </c>
-      <c r="H63" s="9">
-        <v>2.91</v>
+      <c r="H63" s="3">
+        <v>27.2</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>335</v>
+        <v>407</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D64" s="9">
-        <v>5.3999999999999999E-2</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="E64">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F64" s="1">
-        <f>D64+E64*0.0001</f>
-        <v>5.5E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.98199999999999998</v>
       </c>
       <c r="G64" s="9">
         <v>0</v>
       </c>
       <c r="H64" s="9">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+        <v>31.96</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>334</v>
+        <v>408</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D65" s="9">
-        <v>1.4E-2</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="E65">
-        <v>18</v>
+        <v>264</v>
       </c>
       <c r="F65" s="1">
-        <f>D65+E65*0.0001</f>
-        <v>1.5800000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.44</v>
       </c>
       <c r="G65" s="9">
         <v>0</v>
       </c>
-      <c r="H65" s="9">
-        <v>2.85</v>
+      <c r="H65" s="3">
+        <v>21.6</v>
       </c>
     </row>
     <row r="66" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>325</v>
+        <v>409</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="D66" s="9">
-        <v>4.8000000000000001E-2</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F66" s="1">
-        <f>D66+E66*0.0001</f>
-        <v>4.82E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.73399999999999999</v>
       </c>
       <c r="G66" s="9">
         <v>0</v>
       </c>
       <c r="H66" s="9">
-        <v>0.02</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="67" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>326</v>
+        <v>410</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="D67" s="9">
-        <v>0.246</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F67" s="1">
-        <f>D67+E67*0.0001</f>
-        <v>0.2462</v>
+        <f t="shared" si="1"/>
+        <v>0.73699999999999999</v>
       </c>
       <c r="G67" s="9">
         <v>0</v>
       </c>
       <c r="H67" s="9">
-        <v>0.02</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>327</v>
+        <v>411</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D68" s="8">
-        <v>2.5309999999999998E-10</v>
+        <v>279</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.08</v>
       </c>
       <c r="E68">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F68" s="1">
-        <f>D68+E68*0.0001</f>
-        <v>2.0000002531000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.14600000000000002</v>
       </c>
       <c r="G68" s="9">
         <v>0</v>
       </c>
       <c r="H68" s="9">
-        <v>0.21</v>
+        <v>39.58</v>
       </c>
     </row>
     <row r="69" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>328</v>
+        <v>412</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="D69" s="9">
-        <v>0.749</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="E69">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F69" s="1">
-        <f>D69+E69*0.0001</f>
-        <v>0.75039999999999996</v>
+        <f t="shared" si="1"/>
+        <v>0.73799999999999999</v>
       </c>
       <c r="G69" s="9">
         <v>0</v>
       </c>
       <c r="H69" s="9">
-        <v>4.5599999999999996</v>
+        <v>11.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update control figures and VQE example
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703723B8-1C90-EC49-A0DE-FE93CFD475AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9802A752-3858-7A4C-BEA7-184032566E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
@@ -7821,8 +7821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
   <dimension ref="B1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69:H69"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test example with 8 qubits, update results in excel file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DD674-C171-3840-8DAE-3909219086C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D15C9C6-E842-BD46-9C74-F68089FA9F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="5" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="431">
   <si>
     <t>Name</t>
   </si>
@@ -1341,6 +1342,30 @@
   </si>
   <si>
     <t>all switches: 3</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Input for QC</t>
+  </si>
+  <si>
+    <t>Output from QC</t>
+  </si>
+  <si>
+    <t>TR/ALB</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Control sequence, initial and target operator</t>
+  </si>
+  <si>
+    <t>Objective function, state value of time evolution and back propagation</t>
+  </si>
+  <si>
+    <t>Objective function</t>
   </si>
 </sst>
 </file>
@@ -1756,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:H294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B267" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D284" sqref="D284:G284"/>
+    <sheetView topLeftCell="B267" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10703,7 +10728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
   <dimension ref="B1:I105"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="112" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="112" workbookViewId="0">
       <selection activeCell="D105" sqref="D105:H105"/>
     </sheetView>
   </sheetViews>
@@ -13068,4 +13093,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B1B372-4CC2-8848-A040-A5C43187FDD8}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update results of optimization solvers
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3F2B3F-A7C5-C44E-A8D5-F7AD2E835710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CFB7A1-CB32-BA40-A913-194DCC8736C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="5" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="436">
   <si>
     <t>Name</t>
   </si>
@@ -1366,14 +1366,30 @@
   </si>
   <si>
     <t>Objective function</t>
+  </si>
+  <si>
+    <t>Couenne</t>
+  </si>
+  <si>
+    <t>SCIP</t>
+  </si>
+  <si>
+    <t>MUCOD-II</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>run out of memory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="173" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -1430,7 +1446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1464,6 +1480,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1779,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:H294"/>
+  <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView topLeftCell="B267" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B278" sqref="B278"/>
+    <sheetView tabSelected="1" topLeftCell="B317" zoomScale="118" workbookViewId="0">
+      <selection activeCell="D340" sqref="D340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3792,7 +3809,7 @@
         <v>16.36</v>
       </c>
     </row>
-    <row r="97" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B97" s="2" t="s">
         <v>99</v>
       </c>
@@ -3813,7 +3830,7 @@
         <v>79.12</v>
       </c>
     </row>
-    <row r="98" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
         <v>150</v>
       </c>
@@ -3834,7 +3851,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B99" s="2" t="s">
         <v>100</v>
       </c>
@@ -3855,7 +3872,7 @@
         <v>88.38</v>
       </c>
     </row>
-    <row r="100" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="2" t="s">
         <v>420</v>
@@ -3865,8 +3882,8 @@
       </c>
       <c r="F100" s="1"/>
     </row>
-    <row r="102" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>129</v>
       </c>
@@ -3886,8 +3903,12 @@
       <c r="G103">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I103">
+        <f>D103/D131</f>
+        <v>0.99975000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>130</v>
       </c>
@@ -3910,8 +3931,12 @@
       <c r="H104" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="105" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I104">
+        <f>D104/D131</f>
+        <v>0.99824999999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>131</v>
       </c>
@@ -3931,8 +3956,12 @@
       <c r="G105">
         <v>43.35</v>
       </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I105">
+        <f>D105/D131</f>
+        <v>0.99975000000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>132</v>
       </c>
@@ -3953,7 +3982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>133</v>
       </c>
@@ -3974,7 +4003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>134</v>
       </c>
@@ -3995,7 +4024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>135</v>
       </c>
@@ -4016,7 +4045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>136</v>
       </c>
@@ -4037,7 +4066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>137</v>
       </c>
@@ -4058,7 +4087,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>138</v>
       </c>
@@ -4415,7 +4444,7 @@
         <v>22.66</v>
       </c>
     </row>
-    <row r="129" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B129" s="2" t="s">
         <v>149</v>
       </c>
@@ -4436,7 +4465,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="130" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B130" s="2" t="s">
         <v>148</v>
       </c>
@@ -4457,7 +4486,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="131" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B131" s="2"/>
       <c r="C131" s="2" t="s">
         <v>421</v>
@@ -4467,8 +4496,8 @@
       </c>
       <c r="F131" s="1"/>
     </row>
-    <row r="133" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C134" t="s">
         <v>27</v>
       </c>
@@ -4485,8 +4514,12 @@
       <c r="G134">
         <v>21.47</v>
       </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H134">
+        <f>D134/D159</f>
+        <v>0.72816759212518922</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
         <v>28</v>
       </c>
@@ -4503,8 +4536,12 @@
       <c r="G135">
         <v>839.77</v>
       </c>
-    </row>
-    <row r="136" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H135">
+        <f>D135/D159</f>
+        <v>0.71706208985360931</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
         <v>46</v>
       </c>
@@ -4521,8 +4558,12 @@
       <c r="G136">
         <v>183.61</v>
       </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H136">
+        <f>D136/D159</f>
+        <v>0.72715800100959105</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C137" t="s">
         <v>29</v>
       </c>
@@ -4540,7 +4581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C138" t="s">
         <v>30</v>
       </c>
@@ -4558,7 +4599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C139" t="s">
         <v>31</v>
       </c>
@@ -4576,7 +4617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C140" t="s">
         <v>32</v>
       </c>
@@ -4594,7 +4635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
         <v>33</v>
       </c>
@@ -4612,7 +4653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C142" t="s">
         <v>34</v>
       </c>
@@ -4630,7 +4671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C143" t="s">
         <v>59</v>
       </c>
@@ -4648,7 +4689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
         <v>35</v>
       </c>
@@ -4930,7 +4971,7 @@
       </c>
     </row>
     <row r="160" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
         <v>27</v>
       </c>
@@ -4947,8 +4988,12 @@
       <c r="G161">
         <v>32.619999999999997</v>
       </c>
-    </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H161">
+        <f>D161/D186</f>
+        <v>0.84537228131449438</v>
+      </c>
+    </row>
+    <row r="162" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C162" t="s">
         <v>28</v>
       </c>
@@ -4965,8 +5010,12 @@
       <c r="G162">
         <v>1275.9000000000001</v>
       </c>
-    </row>
-    <row r="163" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H162">
+        <f>D162/D186</f>
+        <v>0.84172090808064759</v>
+      </c>
+    </row>
+    <row r="163" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C163" s="2" t="s">
         <v>46</v>
       </c>
@@ -4983,8 +5032,12 @@
       <c r="G163">
         <v>584.21</v>
       </c>
-    </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H163">
+        <f>D163/D186</f>
+        <v>0.84473725988252091</v>
+      </c>
+    </row>
+    <row r="164" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
         <v>29</v>
       </c>
@@ -4999,7 +5052,7 @@
         <v>-4.8879999999999999</v>
       </c>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
         <v>30</v>
       </c>
@@ -5014,7 +5067,7 @@
         <v>-2.04</v>
       </c>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C166" t="s">
         <v>31</v>
       </c>
@@ -5029,7 +5082,7 @@
         <v>-5.0860000000000003</v>
       </c>
     </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C167" t="s">
         <v>32</v>
       </c>
@@ -5044,7 +5097,7 @@
         <v>-4.7130000000000001</v>
       </c>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C168" t="s">
         <v>33</v>
       </c>
@@ -5059,7 +5112,7 @@
         <v>-2.04</v>
       </c>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C169" t="s">
         <v>34</v>
       </c>
@@ -5074,7 +5127,7 @@
         <v>-5.0140000000000002</v>
       </c>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C170" t="s">
         <v>59</v>
       </c>
@@ -5089,7 +5142,7 @@
         <v>-4.8029999999999999</v>
       </c>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C171" t="s">
         <v>35</v>
       </c>
@@ -5104,7 +5157,7 @@
         <v>-2.04</v>
       </c>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
         <v>36</v>
       </c>
@@ -5119,7 +5172,7 @@
         <v>-4.907</v>
       </c>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
         <v>63</v>
       </c>
@@ -5137,7 +5190,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C174" t="s">
         <v>62</v>
       </c>
@@ -5155,7 +5208,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C175" t="s">
         <v>68</v>
       </c>
@@ -5173,7 +5226,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="176" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:8" ht="51" x14ac:dyDescent="0.2">
       <c r="C176" s="2" t="s">
         <v>69</v>
       </c>
@@ -5191,7 +5244,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="177" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C177" s="2" t="s">
         <v>42</v>
       </c>
@@ -5209,7 +5262,7 @@
         <v>6.58</v>
       </c>
     </row>
-    <row r="178" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C178" s="2" t="s">
         <v>35</v>
       </c>
@@ -5227,7 +5280,7 @@
         <v>7.09</v>
       </c>
     </row>
-    <row r="179" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C179" s="2" t="s">
         <v>36</v>
       </c>
@@ -5245,7 +5298,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="180" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C180" s="2" t="s">
         <v>43</v>
       </c>
@@ -5263,7 +5316,7 @@
         <v>6.18</v>
       </c>
     </row>
-    <row r="181" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C181" s="2" t="s">
         <v>37</v>
       </c>
@@ -5281,7 +5334,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="182" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C182" s="2" t="s">
         <v>38</v>
       </c>
@@ -5299,7 +5352,7 @@
         <v>18.149999999999999</v>
       </c>
     </row>
-    <row r="183" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C183" s="2" t="s">
         <v>237</v>
       </c>
@@ -5317,7 +5370,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="184" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C184" s="2" t="s">
         <v>238</v>
       </c>
@@ -5335,7 +5388,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="185" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C185" s="2" t="s">
         <v>239</v>
       </c>
@@ -5353,7 +5406,7 @@
         <v>22.66</v>
       </c>
     </row>
-    <row r="186" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C186" s="2" t="s">
         <v>419</v>
       </c>
@@ -5361,8 +5414,8 @@
         <v>-6.2990000000000004</v>
       </c>
     </row>
-    <row r="187" spans="3:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="188" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C188" t="s">
         <v>27</v>
       </c>
@@ -5379,8 +5432,12 @@
       <c r="G188">
         <v>34.11</v>
       </c>
-    </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H188">
+        <f>D188/D213</f>
+        <v>0.78557914652091665</v>
+      </c>
+    </row>
+    <row r="189" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C189" t="s">
         <v>28</v>
       </c>
@@ -5397,8 +5454,12 @@
       <c r="G189">
         <v>1184.73</v>
       </c>
-    </row>
-    <row r="190" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H189">
+        <f>D189/D213</f>
+        <v>0.77927265083035524</v>
+      </c>
+    </row>
+    <row r="190" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C190" s="2" t="s">
         <v>46</v>
       </c>
@@ -5415,8 +5476,12 @@
       <c r="G190">
         <v>267.57</v>
       </c>
-    </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H190">
+        <f>D190/D213</f>
+        <v>0.7851587134748792</v>
+      </c>
+    </row>
+    <row r="191" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C191" t="s">
         <v>29</v>
       </c>
@@ -5431,7 +5496,7 @@
         <v>-3.306</v>
       </c>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C192" t="s">
         <v>30</v>
       </c>
@@ -5713,7 +5778,7 @@
         <v>40.97</v>
       </c>
     </row>
-    <row r="209" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C209" s="2" t="s">
         <v>38</v>
       </c>
@@ -5731,7 +5796,7 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="210" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C210" s="2" t="s">
         <v>237</v>
       </c>
@@ -5749,7 +5814,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="211" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C211" s="2" t="s">
         <v>238</v>
       </c>
@@ -5767,7 +5832,7 @@
         <v>46.45</v>
       </c>
     </row>
-    <row r="212" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C212" s="2" t="s">
         <v>239</v>
       </c>
@@ -5785,7 +5850,7 @@
         <v>17.64</v>
       </c>
     </row>
-    <row r="213" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C213" s="2" t="s">
         <v>419</v>
       </c>
@@ -5793,8 +5858,8 @@
         <v>-4.7569999999999997</v>
       </c>
     </row>
-    <row r="214" spans="3:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="215" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C215" t="s">
         <v>27</v>
       </c>
@@ -5811,8 +5876,12 @@
       <c r="G215">
         <v>33.51</v>
       </c>
-    </row>
-    <row r="216" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H215">
+        <f>D215/D240</f>
+        <v>0.77285579641847313</v>
+      </c>
+    </row>
+    <row r="216" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C216" t="s">
         <v>28</v>
       </c>
@@ -5829,8 +5898,12 @@
       <c r="G216">
         <v>1189.02</v>
       </c>
-    </row>
-    <row r="217" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H216">
+        <f>D216/D240</f>
+        <v>0.76927426955702183</v>
+      </c>
+    </row>
+    <row r="217" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C217" s="2" t="s">
         <v>46</v>
       </c>
@@ -5847,8 +5920,12 @@
       <c r="G217">
         <v>402.05</v>
       </c>
-    </row>
-    <row r="218" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H217">
+        <f>D217/D240</f>
+        <v>0.77229029217719147</v>
+      </c>
+    </row>
+    <row r="218" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C218" t="s">
         <v>29</v>
       </c>
@@ -5863,7 +5940,7 @@
         <v>-3.6749999999999998</v>
       </c>
     </row>
-    <row r="219" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C219" t="s">
         <v>30</v>
       </c>
@@ -5878,7 +5955,7 @@
         <v>-2.0259999999999998</v>
       </c>
     </row>
-    <row r="220" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C220" t="s">
         <v>31</v>
       </c>
@@ -5893,7 +5970,7 @@
         <v>-3.8220000000000001</v>
       </c>
     </row>
-    <row r="221" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C221" t="s">
         <v>32</v>
       </c>
@@ -5908,7 +5985,7 @@
         <v>-3.5830000000000002</v>
       </c>
     </row>
-    <row r="222" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C222" t="s">
         <v>33</v>
       </c>
@@ -5923,7 +6000,7 @@
         <v>-2.0259999999999998</v>
       </c>
     </row>
-    <row r="223" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C223" t="s">
         <v>34</v>
       </c>
@@ -5938,7 +6015,7 @@
         <v>-3.8279999999999998</v>
       </c>
     </row>
-    <row r="224" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C224" t="s">
         <v>59</v>
       </c>
@@ -6225,8 +6302,8 @@
         <v>-5.3049999999999997</v>
       </c>
     </row>
-    <row r="241" spans="3:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="242" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="242" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C242" t="s">
         <v>27</v>
       </c>
@@ -6243,8 +6320,12 @@
       <c r="G242">
         <v>17.98</v>
       </c>
-    </row>
-    <row r="243" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H242">
+        <f>D242/D267</f>
+        <v>0.80111976630963977</v>
+      </c>
+    </row>
+    <row r="243" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C243" t="s">
         <v>28</v>
       </c>
@@ -6261,8 +6342,12 @@
       <c r="G243">
         <v>1487.63</v>
       </c>
-    </row>
-    <row r="244" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H243">
+        <f>D243/D267</f>
+        <v>0.79333008763388513</v>
+      </c>
+    </row>
+    <row r="244" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C244" s="2" t="s">
         <v>46</v>
       </c>
@@ -6279,8 +6364,12 @@
       <c r="G244">
         <v>269.70999999999998</v>
       </c>
-    </row>
-    <row r="245" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H244">
+        <f>D244/D267</f>
+        <v>0.80111976630963977</v>
+      </c>
+    </row>
+    <row r="245" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C245" t="s">
         <v>29</v>
       </c>
@@ -6295,7 +6384,7 @@
         <v>-2.8930000000000002</v>
       </c>
     </row>
-    <row r="246" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C246" t="s">
         <v>30</v>
       </c>
@@ -6310,7 +6399,7 @@
         <v>-1.331</v>
       </c>
     </row>
-    <row r="247" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C247" t="s">
         <v>31</v>
       </c>
@@ -6325,7 +6414,7 @@
         <v>-2.9750000000000001</v>
       </c>
     </row>
-    <row r="248" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C248" t="s">
         <v>32</v>
       </c>
@@ -6340,7 +6429,7 @@
         <v>-2.758</v>
       </c>
     </row>
-    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C249" t="s">
         <v>33</v>
       </c>
@@ -6355,7 +6444,7 @@
         <v>-1.5449999999999999</v>
       </c>
     </row>
-    <row r="250" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C250" t="s">
         <v>34</v>
       </c>
@@ -6370,7 +6459,7 @@
         <v>-3.0989999999999998</v>
       </c>
     </row>
-    <row r="251" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C251" t="s">
         <v>59</v>
       </c>
@@ -6385,7 +6474,7 @@
         <v>-2.8580000000000001</v>
       </c>
     </row>
-    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C252" t="s">
         <v>35</v>
       </c>
@@ -6400,7 +6489,7 @@
         <v>-1.331</v>
       </c>
     </row>
-    <row r="253" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C253" t="s">
         <v>36</v>
       </c>
@@ -6415,7 +6504,7 @@
         <v>-2.9750000000000001</v>
       </c>
     </row>
-    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C254" t="s">
         <v>63</v>
       </c>
@@ -6433,7 +6522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C255" t="s">
         <v>62</v>
       </c>
@@ -6451,7 +6540,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C256" t="s">
         <v>68</v>
       </c>
@@ -6469,7 +6558,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="257" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:8" ht="51" x14ac:dyDescent="0.2">
       <c r="C257" s="2" t="s">
         <v>69</v>
       </c>
@@ -6487,7 +6576,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="258" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C258" s="2" t="s">
         <v>42</v>
       </c>
@@ -6505,7 +6594,7 @@
         <v>43.22</v>
       </c>
     </row>
-    <row r="259" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C259" s="2" t="s">
         <v>35</v>
       </c>
@@ -6523,7 +6612,7 @@
         <v>41.39</v>
       </c>
     </row>
-    <row r="260" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C260" s="2" t="s">
         <v>36</v>
       </c>
@@ -6541,7 +6630,7 @@
         <v>27.34</v>
       </c>
     </row>
-    <row r="261" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C261" s="2" t="s">
         <v>43</v>
       </c>
@@ -6559,7 +6648,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="262" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C262" s="2" t="s">
         <v>37</v>
       </c>
@@ -6577,7 +6666,7 @@
         <v>9.19</v>
       </c>
     </row>
-    <row r="263" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C263" s="2" t="s">
         <v>38</v>
       </c>
@@ -6595,7 +6684,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="264" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C264" s="2" t="s">
         <v>237</v>
       </c>
@@ -6613,7 +6702,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="265" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C265" s="2" t="s">
         <v>238</v>
       </c>
@@ -6631,7 +6720,7 @@
         <v>34.65</v>
       </c>
     </row>
-    <row r="266" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C266" s="2" t="s">
         <v>239</v>
       </c>
@@ -6649,7 +6738,7 @@
         <v>28.48</v>
       </c>
     </row>
-    <row r="267" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C267" s="2" t="s">
         <v>419</v>
       </c>
@@ -6657,8 +6746,8 @@
         <v>-4.1079999999999997</v>
       </c>
     </row>
-    <row r="268" spans="3:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="269" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="269" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C269" t="s">
         <v>27</v>
       </c>
@@ -6678,8 +6767,12 @@
         <f>AVERAGE(G134,G161,G188,G215,G242)</f>
         <v>27.937999999999995</v>
       </c>
-    </row>
-    <row r="270" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H269" s="1">
+        <f>AVERAGE(H134,H161,H188,H215,H242)</f>
+        <v>0.78661891653774263</v>
+      </c>
+    </row>
+    <row r="270" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C270" t="s">
         <v>28</v>
       </c>
@@ -6699,42 +6792,50 @@
         <f>AVERAGE(G135,G162,G189,G216,G243)</f>
         <v>1195.4100000000001</v>
       </c>
-    </row>
-    <row r="271" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H270" s="1">
+        <f t="shared" ref="H270:H271" si="15">AVERAGE(H135,H162,H189,H216,H243)</f>
+        <v>0.78013200119110382</v>
+      </c>
+    </row>
+    <row r="271" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C271" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D271" s="1">
-        <f t="shared" ref="D271:G294" si="15">AVERAGE(D136,D163,D190,D217,D244)</f>
+        <f t="shared" ref="D271:G294" si="16">AVERAGE(D136,D163,D190,D217,D244)</f>
         <v>-3.8649999999999998</v>
       </c>
       <c r="E271" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.5077999999999996</v>
       </c>
       <c r="F271" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8199219999999996</v>
       </c>
       <c r="G271" s="3">
         <f>AVERAGE(G136,G163,G190,G217,G244)</f>
         <v>341.43</v>
       </c>
-    </row>
-    <row r="272" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="H271" s="1">
+        <f t="shared" si="15"/>
+        <v>0.78609280657076452</v>
+      </c>
+    </row>
+    <row r="272" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C272" t="s">
         <v>29</v>
       </c>
       <c r="D272" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8537999999999997</v>
       </c>
-      <c r="E272" s="19">
-        <f t="shared" si="15"/>
+      <c r="E272" s="20">
+        <f t="shared" si="16"/>
         <v>38.799999999999997</v>
       </c>
       <c r="F272" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.4658000000000002</v>
       </c>
       <c r="G272" s="3"/>
@@ -6744,15 +6845,15 @@
         <v>30</v>
       </c>
       <c r="D273" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.5484000000000002</v>
       </c>
-      <c r="E273" s="19">
-        <f t="shared" si="15"/>
+      <c r="E273" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F273" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.4883999999999999</v>
       </c>
       <c r="G273" s="3"/>
@@ -6762,15 +6863,15 @@
         <v>31</v>
       </c>
       <c r="D274" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.7063999999999999</v>
       </c>
-      <c r="E274" s="19">
-        <f t="shared" si="15"/>
+      <c r="E274" s="20">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="F274" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6063999999999998</v>
       </c>
       <c r="G274" s="3"/>
@@ -6780,15 +6881,15 @@
         <v>32</v>
       </c>
       <c r="D275" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8326000000000002</v>
       </c>
-      <c r="E275" s="19">
-        <f t="shared" si="15"/>
+      <c r="E275" s="20">
+        <f t="shared" si="16"/>
         <v>52.8</v>
       </c>
       <c r="F275" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.3045999999999998</v>
       </c>
       <c r="G275" s="3"/>
@@ -6798,15 +6899,15 @@
         <v>33</v>
       </c>
       <c r="D276" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.9104000000000003</v>
       </c>
-      <c r="E276" s="19">
-        <f t="shared" si="15"/>
+      <c r="E276" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F276" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.8503999999999998</v>
       </c>
       <c r="G276" s="3"/>
@@ -6816,15 +6917,15 @@
         <v>34</v>
       </c>
       <c r="D277" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.7299999999999995</v>
       </c>
-      <c r="E277" s="19">
-        <f t="shared" si="15"/>
+      <c r="E277" s="20">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="F277" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.63</v>
       </c>
       <c r="G277" s="3"/>
@@ -6834,15 +6935,15 @@
         <v>59</v>
       </c>
       <c r="D278" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8540000000000001</v>
       </c>
-      <c r="E278" s="19">
-        <f t="shared" si="15"/>
+      <c r="E278" s="20">
+        <f t="shared" si="16"/>
         <v>43.6</v>
       </c>
       <c r="F278" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.4180000000000001</v>
       </c>
       <c r="G278" s="3"/>
@@ -6852,15 +6953,15 @@
         <v>35</v>
       </c>
       <c r="D279" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.8676000000000001</v>
       </c>
-      <c r="E279" s="19">
-        <f t="shared" si="15"/>
+      <c r="E279" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F279" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.8076000000000001</v>
       </c>
       <c r="G279" s="3"/>
@@ -6870,15 +6971,15 @@
         <v>36</v>
       </c>
       <c r="D280" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6514000000000002</v>
       </c>
-      <c r="E280" s="19">
-        <f t="shared" si="15"/>
+      <c r="E280" s="20">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="F280" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.5514000000000001</v>
       </c>
       <c r="G280" s="3"/>
@@ -6888,15 +6989,15 @@
         <v>63</v>
       </c>
       <c r="D281" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.7986</v>
       </c>
-      <c r="E281" s="19">
-        <f t="shared" si="15"/>
+      <c r="E281" s="20">
+        <f t="shared" si="16"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="F281" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.7545999999999999</v>
       </c>
       <c r="G281" s="3">
@@ -6909,19 +7010,19 @@
         <v>62</v>
       </c>
       <c r="D282" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.0702000000000003</v>
       </c>
-      <c r="E282" s="19">
-        <f t="shared" si="15"/>
+      <c r="E282" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F282" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.0101999999999998</v>
       </c>
       <c r="G282" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.20200000000000001</v>
       </c>
     </row>
@@ -6930,19 +7031,19 @@
         <v>68</v>
       </c>
       <c r="D283" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.7986</v>
       </c>
-      <c r="E283" s="19">
-        <f t="shared" si="15"/>
+      <c r="E283" s="20">
+        <f t="shared" si="16"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="F283" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.7545999999999999</v>
       </c>
       <c r="G283" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.78200000000000003</v>
       </c>
     </row>
@@ -6951,19 +7052,19 @@
         <v>69</v>
       </c>
       <c r="D284" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.0702000000000003</v>
       </c>
-      <c r="E284" s="19">
-        <f t="shared" si="15"/>
+      <c r="E284" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F284" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.0101999999999998</v>
       </c>
       <c r="G284" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.23199999999999998</v>
       </c>
     </row>
@@ -6972,19 +7073,19 @@
         <v>42</v>
       </c>
       <c r="D285" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8457999999999992</v>
       </c>
-      <c r="E285" s="19">
-        <f t="shared" si="15"/>
+      <c r="E285" s="20">
+        <f t="shared" si="16"/>
         <v>32.4</v>
       </c>
       <c r="F285" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.5218000000000003</v>
       </c>
       <c r="G285" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>16.948</v>
       </c>
     </row>
@@ -6993,19 +7094,19 @@
         <v>35</v>
       </c>
       <c r="D286" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.7090000000000005</v>
       </c>
-      <c r="E286" s="19">
-        <f t="shared" si="15"/>
+      <c r="E286" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F286" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.649</v>
       </c>
       <c r="G286" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>41.423999999999999</v>
       </c>
     </row>
@@ -7014,19 +7115,19 @@
         <v>36</v>
       </c>
       <c r="D287" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.7887999999999997</v>
       </c>
-      <c r="E287" s="19">
-        <f t="shared" si="15"/>
+      <c r="E287" s="20">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="F287" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6888000000000005</v>
       </c>
       <c r="G287" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18.510000000000002</v>
       </c>
     </row>
@@ -7035,134 +7136,902 @@
         <v>43</v>
       </c>
       <c r="D288" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8404000000000003</v>
       </c>
-      <c r="E288" s="19">
-        <f t="shared" si="15"/>
+      <c r="E288" s="20">
+        <f t="shared" si="16"/>
         <v>50</v>
       </c>
       <c r="F288" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.3404000000000003</v>
       </c>
       <c r="G288" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.8780000000000019</v>
       </c>
     </row>
-    <row r="289" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C289" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D289" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.6142000000000003</v>
       </c>
-      <c r="E289" s="19">
-        <f t="shared" si="15"/>
+      <c r="E289" s="20">
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F289" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.5541999999999998</v>
       </c>
       <c r="G289" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>33.363999999999997</v>
       </c>
     </row>
-    <row r="290" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C290" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D290" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.7518000000000002</v>
       </c>
-      <c r="E290" s="19">
-        <f t="shared" si="15"/>
+      <c r="E290" s="20">
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="F290" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6518000000000002</v>
       </c>
       <c r="G290" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10.843999999999999</v>
       </c>
     </row>
-    <row r="291" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C291" s="2" t="s">
         <v>237</v>
       </c>
       <c r="D291" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.8536000000000001</v>
       </c>
-      <c r="E291" s="19">
-        <f t="shared" si="15"/>
+      <c r="E291" s="20">
+        <f t="shared" si="16"/>
         <v>40.4</v>
       </c>
       <c r="F291" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.4495999999999993</v>
       </c>
       <c r="G291" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11.112</v>
       </c>
     </row>
-    <row r="292" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C292" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D292" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.7090000000000005</v>
       </c>
-      <c r="E292" s="19">
-        <f t="shared" ref="E292:G292" si="16">AVERAGE(E157,E184,E211,E238,E265)</f>
+      <c r="E292" s="20">
+        <f t="shared" ref="E292:G292" si="17">AVERAGE(E157,E184,E211,E238,E265)</f>
         <v>6</v>
       </c>
       <c r="F292" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-2.649</v>
       </c>
       <c r="G292" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>39.532000000000004</v>
       </c>
     </row>
-    <row r="293" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C293" s="2" t="s">
         <v>239</v>
       </c>
       <c r="D293" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.7814000000000001</v>
       </c>
-      <c r="E293" s="19">
-        <f t="shared" ref="E293:G293" si="17">AVERAGE(E158,E185,E212,E239,E266)</f>
+      <c r="E293" s="20">
+        <f t="shared" ref="E293:G293" si="18">AVERAGE(E158,E185,E212,E239,E266)</f>
         <v>10</v>
       </c>
       <c r="F293" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-3.6814000000000009</v>
       </c>
       <c r="G293" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>24.024000000000001</v>
       </c>
     </row>
-    <row r="294" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C294" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D294" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-4.8862000000000005</v>
+      </c>
+    </row>
+    <row r="295" spans="3:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="296" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C296" t="s">
+        <v>27</v>
+      </c>
+      <c r="D296" s="1">
+        <f>STDEV(D134,D161,D188,D215,D242)</f>
+        <v>0.9344853128861893</v>
+      </c>
+      <c r="E296" s="1">
+        <f t="shared" ref="E296:G296" si="19">STDEV(E134,E161,E188,E215,E242)</f>
+        <v>0.59964722962755368</v>
+      </c>
+      <c r="F296" s="1">
+        <f t="shared" si="19"/>
+        <v>0.93481350101504268</v>
+      </c>
+      <c r="G296" s="1">
+        <f t="shared" si="19"/>
+        <v>7.616736177655115</v>
+      </c>
+      <c r="H296" s="19">
+        <f>STDEV(H134,H161,H188,H215,H242)</f>
+        <v>4.2630078698567039E-2</v>
+      </c>
+    </row>
+    <row r="297" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C297" t="s">
+        <v>28</v>
+      </c>
+      <c r="D297" s="1">
+        <f t="shared" ref="D297:H321" si="20">STDEV(D135,D162,D189,D216,D243)</f>
+        <v>0.94190710794642551</v>
+      </c>
+      <c r="E297" s="1">
+        <f t="shared" si="20"/>
+        <v>0.6433507596948993</v>
+      </c>
+      <c r="F297" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93736643582966095</v>
+      </c>
+      <c r="G297" s="1">
+        <f t="shared" si="20"/>
+        <v>233.72305866131413</v>
+      </c>
+      <c r="H297" s="19">
+        <f t="shared" si="20"/>
+        <v>4.4899402760503679E-2</v>
+      </c>
+    </row>
+    <row r="298" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C298" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D298" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93386187415484589</v>
+      </c>
+      <c r="E298" s="1">
+        <f t="shared" si="20"/>
+        <v>0.27504581436553449</v>
+      </c>
+      <c r="F298" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93445987876419856</v>
+      </c>
+      <c r="G298" s="1">
+        <f t="shared" si="20"/>
+        <v>156.62305322014373</v>
+      </c>
+      <c r="H298" s="19">
+        <f t="shared" si="20"/>
+        <v>4.2806759580872412E-2</v>
+      </c>
+    </row>
+    <row r="299" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C299" t="s">
+        <v>29</v>
+      </c>
+      <c r="D299" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93545587816850329</v>
+      </c>
+      <c r="E299" s="1">
+        <f t="shared" si="20"/>
+        <v>5.2153619241621234</v>
+      </c>
+      <c r="F299" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89831714889564496</v>
+      </c>
+      <c r="G299" s="1"/>
+    </row>
+    <row r="300" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C300" t="s">
+        <v>30</v>
+      </c>
+      <c r="D300" s="1">
+        <f t="shared" si="20"/>
+        <v>0.56778895727197753</v>
+      </c>
+      <c r="E300" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F300" s="1">
+        <f t="shared" si="20"/>
+        <v>0.56778895727197787</v>
+      </c>
+      <c r="G300" s="1"/>
+    </row>
+    <row r="301" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C301" t="s">
+        <v>31</v>
+      </c>
+      <c r="D301" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93950588076924879</v>
+      </c>
+      <c r="E301" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F301" s="1">
+        <f t="shared" si="20"/>
+        <v>0.9395058807692469</v>
+      </c>
+      <c r="G301" s="1"/>
+    </row>
+    <row r="302" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C302" t="s">
+        <v>32</v>
+      </c>
+      <c r="D302" s="1">
+        <f t="shared" si="20"/>
+        <v>0.9451736877421002</v>
+      </c>
+      <c r="E302" s="1">
+        <f t="shared" si="20"/>
+        <v>3.3466401061363023</v>
+      </c>
+      <c r="F302" s="1">
+        <f t="shared" si="20"/>
+        <v>0.92120318062846507</v>
+      </c>
+      <c r="G302" s="1"/>
+    </row>
+    <row r="303" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C303" t="s">
+        <v>33</v>
+      </c>
+      <c r="D303" s="1">
+        <f t="shared" si="20"/>
+        <v>0.37853837321994011</v>
+      </c>
+      <c r="E303" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F303" s="1">
+        <f t="shared" si="20"/>
+        <v>0.37853837321994249</v>
+      </c>
+      <c r="G303" s="1"/>
+    </row>
+    <row r="304" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
+        <v>34</v>
+      </c>
+      <c r="D304" s="1">
+        <f t="shared" si="20"/>
+        <v>0.87387670755090152</v>
+      </c>
+      <c r="E304" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F304" s="1">
+        <f t="shared" si="20"/>
+        <v>0.87387670755090152</v>
+      </c>
+      <c r="G304" s="1"/>
+    </row>
+    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C305" t="s">
+        <v>59</v>
+      </c>
+      <c r="D305" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93090305617717128</v>
+      </c>
+      <c r="E305" s="1">
+        <f t="shared" si="20"/>
+        <v>3.577708763999663</v>
+      </c>
+      <c r="F305" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89994472052454388</v>
+      </c>
+      <c r="G305" s="1"/>
+    </row>
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C306" t="s">
+        <v>35</v>
+      </c>
+      <c r="D306" s="1">
+        <f t="shared" si="20"/>
+        <v>0.43026538322295788</v>
+      </c>
+      <c r="E306" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F306" s="1">
+        <f t="shared" si="20"/>
+        <v>0.43026538322295893</v>
+      </c>
+      <c r="G306" s="1"/>
+    </row>
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C307" t="s">
+        <v>36</v>
+      </c>
+      <c r="D307" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89544586659384318</v>
+      </c>
+      <c r="E307" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F307" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89544586659384318</v>
+      </c>
+      <c r="G307" s="1"/>
+    </row>
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C308" t="s">
+        <v>63</v>
+      </c>
+      <c r="D308" s="1">
+        <f t="shared" si="20"/>
+        <v>1.5231763850585396</v>
+      </c>
+      <c r="E308" s="1">
+        <f t="shared" si="20"/>
+        <v>2.1908902300206647</v>
+      </c>
+      <c r="F308" s="1">
+        <f t="shared" si="20"/>
+        <v>1.5019395127634139</v>
+      </c>
+      <c r="G308" s="1">
+        <f t="shared" si="20"/>
+        <v>0.36148305631108085</v>
+      </c>
+    </row>
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C309" t="s">
+        <v>62</v>
+      </c>
+      <c r="D309" s="1">
+        <f t="shared" si="20"/>
+        <v>0.7127921857035181</v>
+      </c>
+      <c r="E309" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F309" s="1">
+        <f t="shared" si="20"/>
+        <v>0.71279218570351943</v>
+      </c>
+      <c r="G309" s="1">
+        <f t="shared" si="20"/>
+        <v>3.9623225512317922E-2</v>
+      </c>
+    </row>
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C310" t="s">
+        <v>68</v>
+      </c>
+      <c r="D310" s="1">
+        <f t="shared" si="20"/>
+        <v>1.5231763850585396</v>
+      </c>
+      <c r="E310" s="1">
+        <f t="shared" si="20"/>
+        <v>2.1908902300206647</v>
+      </c>
+      <c r="F310" s="1">
+        <f t="shared" si="20"/>
+        <v>1.5019395127634139</v>
+      </c>
+      <c r="G310" s="1">
+        <f t="shared" si="20"/>
+        <v>0.4297324749189893</v>
+      </c>
+    </row>
+    <row r="311" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C311" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D311" s="1">
+        <f t="shared" si="20"/>
+        <v>0.7127921857035181</v>
+      </c>
+      <c r="E311" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F311" s="1">
+        <f t="shared" si="20"/>
+        <v>0.71279218570351943</v>
+      </c>
+      <c r="G311" s="1">
+        <f t="shared" si="20"/>
+        <v>6.7230945255886521E-2</v>
+      </c>
+    </row>
+    <row r="312" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C312" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D312" s="1">
+        <f t="shared" si="20"/>
+        <v>0.94343505340855793</v>
+      </c>
+      <c r="E312" s="1">
+        <f t="shared" si="20"/>
+        <v>13.446189051177287</v>
+      </c>
+      <c r="F312" s="1">
+        <f t="shared" si="20"/>
+        <v>0.84213876528752396</v>
+      </c>
+      <c r="G312" s="1">
+        <f t="shared" si="20"/>
+        <v>16.858864730461537</v>
+      </c>
+    </row>
+    <row r="313" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C313" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D313" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53540311915415606</v>
+      </c>
+      <c r="E313" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F313" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53540311915415773</v>
+      </c>
+      <c r="G313" s="1">
+        <f t="shared" si="20"/>
+        <v>20.13904367143585</v>
+      </c>
+    </row>
+    <row r="314" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C314" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D314" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89669431803709143</v>
+      </c>
+      <c r="E314" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F314" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89669431803708743</v>
+      </c>
+      <c r="G314" s="1">
+        <f t="shared" si="20"/>
+        <v>5.7204501571117525</v>
+      </c>
+    </row>
+    <row r="315" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C315" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D315" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93548131996314976</v>
+      </c>
+      <c r="E315" s="1">
+        <f t="shared" si="20"/>
+        <v>4.8989794855663558</v>
+      </c>
+      <c r="F315" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89284113928514619</v>
+      </c>
+      <c r="G315" s="1">
+        <f t="shared" si="20"/>
+        <v>5.7033560295671473</v>
+      </c>
+    </row>
+    <row r="316" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C316" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D316" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53019873632440817</v>
+      </c>
+      <c r="E316" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F316" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53019873632440817</v>
+      </c>
+      <c r="G316" s="1">
+        <f t="shared" si="20"/>
+        <v>24.73217701699549</v>
+      </c>
+    </row>
+    <row r="317" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C317" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D317" s="1">
+        <f t="shared" si="20"/>
+        <v>0.8815246451461245</v>
+      </c>
+      <c r="E317" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F317" s="1">
+        <f t="shared" si="20"/>
+        <v>0.8815246451461265</v>
+      </c>
+      <c r="G317" s="1">
+        <f t="shared" si="20"/>
+        <v>4.3649776631730868</v>
+      </c>
+    </row>
+    <row r="318" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C318" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D318" s="1">
+        <f t="shared" si="20"/>
+        <v>0.93121281133798772</v>
+      </c>
+      <c r="E318" s="1">
+        <f t="shared" si="20"/>
+        <v>8.7635609200826554</v>
+      </c>
+      <c r="F318" s="1">
+        <f t="shared" si="20"/>
+        <v>0.87786861203713529</v>
+      </c>
+      <c r="G318" s="1">
+        <f t="shared" si="20"/>
+        <v>13.374143710907253</v>
+      </c>
+    </row>
+    <row r="319" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C319" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D319" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53540311915415606</v>
+      </c>
+      <c r="E319" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F319" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53540311915415773</v>
+      </c>
+      <c r="G319" s="1">
+        <f t="shared" si="20"/>
+        <v>20.665585401822014</v>
+      </c>
+    </row>
+    <row r="320" spans="3:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="C320" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D320" s="1">
+        <f t="shared" si="20"/>
+        <v>0.88230822278838672</v>
+      </c>
+      <c r="E320" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F320" s="1">
+        <f t="shared" si="20"/>
+        <v>0.88230822278838261</v>
+      </c>
+      <c r="G320" s="1">
+        <f t="shared" si="20"/>
+        <v>6.8898969513338804</v>
+      </c>
+    </row>
+    <row r="321" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C321" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D321" s="1">
+        <f t="shared" si="20"/>
+        <v>0.95496476374785422</v>
+      </c>
+      <c r="E321" s="1"/>
+    </row>
+    <row r="324" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C324" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D324">
+        <v>-2.516</v>
+      </c>
+      <c r="E324">
+        <v>2.74</v>
+      </c>
+      <c r="F324">
+        <f>D324+E324*0.01</f>
+        <v>-2.4885999999999999</v>
+      </c>
+      <c r="G324">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="325" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C325" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D325">
+        <v>-2.516</v>
+      </c>
+      <c r="E325">
+        <v>2.74</v>
+      </c>
+      <c r="F325">
+        <f>D325+E325*0.01</f>
+        <v>-2.4885999999999999</v>
+      </c>
+      <c r="G325">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="326" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C326" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D326">
+        <v>-0.47499999999999998</v>
+      </c>
+      <c r="E326">
+        <v>2</v>
+      </c>
+      <c r="F326">
+        <f>D326+E326*0.01</f>
+        <v>-0.45499999999999996</v>
+      </c>
+      <c r="G326">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="327" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C327" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D327">
+        <v>-2.141</v>
+      </c>
+      <c r="E327">
+        <v>6</v>
+      </c>
+      <c r="F327">
+        <f t="shared" ref="F327:F330" si="21">D327+E327*0.01</f>
+        <v>-2.081</v>
+      </c>
+      <c r="G327">
+        <v>301.01</v>
+      </c>
+    </row>
+    <row r="328" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C328" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G328">
+        <v>300.20999999999998</v>
+      </c>
+    </row>
+    <row r="329" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C329" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D329">
+        <v>-1.748</v>
+      </c>
+      <c r="E329">
+        <v>22</v>
+      </c>
+      <c r="F329">
+        <f t="shared" si="21"/>
+        <v>-1.528</v>
+      </c>
+      <c r="G329">
+        <v>300.81</v>
+      </c>
+    </row>
+    <row r="330" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C330" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D330">
+        <v>-3.9990000000000001</v>
+      </c>
+      <c r="E330">
+        <v>14.36</v>
+      </c>
+      <c r="F330">
+        <f t="shared" si="21"/>
+        <v>-3.8553999999999999</v>
+      </c>
+      <c r="G330">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="331" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C331" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D331">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="333" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C333" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D333">
+        <v>-1.659</v>
+      </c>
+      <c r="E333">
+        <v>4.76</v>
+      </c>
+      <c r="F333">
+        <f>D333+E333*0.01</f>
+        <v>-1.6113999999999999</v>
+      </c>
+      <c r="G333">
+        <v>199.64</v>
+      </c>
+    </row>
+    <row r="334" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C334" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D334">
+        <v>-1.659</v>
+      </c>
+      <c r="E334">
+        <v>4.76</v>
+      </c>
+      <c r="F334">
+        <f>D334+E334*0.01</f>
+        <v>-1.6113999999999999</v>
+      </c>
+      <c r="G334">
+        <v>46.85</v>
+      </c>
+    </row>
+    <row r="335" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C335" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H335" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="336" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C336" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D336">
+        <v>-1.3009999999999999</v>
+      </c>
+      <c r="E336">
+        <v>6</v>
+      </c>
+      <c r="F336">
+        <f t="shared" ref="F336:F339" si="22">D336+E336*0.01</f>
+        <v>-1.2409999999999999</v>
+      </c>
+      <c r="G336">
+        <v>311.10000000000002</v>
+      </c>
+    </row>
+    <row r="337" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C337" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H337" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="338" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C338" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+      <c r="E338">
+        <v>0</v>
+      </c>
+      <c r="F338">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G338">
+        <v>300.88</v>
+      </c>
+    </row>
+    <row r="339" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C339" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D339">
+        <v>-5.3029999999999999</v>
+      </c>
+      <c r="E339" t="s">
+        <v>434</v>
+      </c>
+      <c r="F339" t="s">
+        <v>434</v>
+      </c>
+      <c r="G339">
+        <v>320.61</v>
+      </c>
+    </row>
+    <row r="340" spans="3:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C340" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D340">
+        <v>-6.2990000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -13099,7 +13968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B1B372-4CC2-8848-A040-A5C43187FDD8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add modified version of switching time optimization
add experimental results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706B8ADC-DF3D-F143-BAD2-952C80EDE8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90881D39-1545-5C46-AECE-3CA22904F241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="4" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="442">
   <si>
     <t>Name</t>
   </si>
@@ -1378,6 +1378,27 @@
   </si>
   <si>
     <t>run out of memory</t>
+  </si>
+  <si>
+    <t>GRAPE+ST</t>
+  </si>
+  <si>
+    <t>TR+ST</t>
+  </si>
+  <si>
+    <t>GRAPE+STMT</t>
+  </si>
+  <si>
+    <t>ADMM+STMT</t>
+  </si>
+  <si>
+    <t>TR+STMT</t>
+  </si>
+  <si>
+    <t>p-GRAPE+ST</t>
+  </si>
+  <si>
+    <t>p-GRAPE+STMT</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1408,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1477,15 +1498,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1800,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
-  <dimension ref="A1:I343"/>
+  <dimension ref="A1:I409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B322" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D343" sqref="D343:G343"/>
+    <sheetView topLeftCell="B390" zoomScale="118" workbookViewId="0">
+      <selection activeCell="F407" sqref="F407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2251,14 +2272,14 @@
         <v>35</v>
       </c>
       <c r="D19">
-        <v>-0.996</v>
+        <v>-0.997</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>-0.91600000000000004</v>
+        <v>-0.95699999999999996</v>
       </c>
       <c r="G19">
         <v>3.15</v>
@@ -4162,17 +4183,17 @@
         <v>63</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>-3.9969999999999999</v>
       </c>
       <c r="E115">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F115" s="1">
         <f t="shared" si="6"/>
-        <v>0.02</v>
+        <v>-3.9369999999999998</v>
       </c>
       <c r="G115">
-        <v>0.04</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.2">
@@ -4183,17 +4204,17 @@
         <v>62</v>
       </c>
       <c r="D116">
-        <v>-3.8839999999999999</v>
+        <v>-3.9340000000000002</v>
       </c>
       <c r="E116">
         <v>6</v>
       </c>
       <c r="F116" s="1">
         <f t="shared" si="6"/>
-        <v>-3.8239999999999998</v>
+        <v>-3.8740000000000001</v>
       </c>
       <c r="G116">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.2">
@@ -4204,17 +4225,17 @@
         <v>68</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>-3.9969999999999999</v>
       </c>
       <c r="E117">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F117" s="1">
         <f t="shared" si="6"/>
-        <v>0.02</v>
+        <v>-3.9369999999999998</v>
       </c>
       <c r="G117">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4225,17 +4246,17 @@
         <v>69</v>
       </c>
       <c r="D118">
-        <v>-3.8839999999999999</v>
+        <v>-3.9340000000000002</v>
       </c>
       <c r="E118">
         <v>6</v>
       </c>
       <c r="F118" s="1">
         <f t="shared" si="6"/>
-        <v>-3.8239999999999998</v>
+        <v>-3.8740000000000001</v>
       </c>
       <c r="G118">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="34" x14ac:dyDescent="0.2">
@@ -4744,7 +4765,7 @@
         <v>-2.2549999999999999</v>
       </c>
       <c r="G146">
-        <v>1.04</v>
+        <v>0.77</v>
       </c>
       <c r="H146" t="s">
         <v>422</v>
@@ -4755,17 +4776,17 @@
         <v>62</v>
       </c>
       <c r="D147">
-        <v>-1.427</v>
+        <v>-2.2130000000000001</v>
       </c>
       <c r="E147">
         <v>6</v>
       </c>
       <c r="F147" s="1">
         <f t="shared" ref="F147:F149" si="8">D147+E147*0.01</f>
-        <v>-1.367</v>
+        <v>-2.153</v>
       </c>
       <c r="G147">
-        <v>0.18</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="148" spans="3:8" x14ac:dyDescent="0.2">
@@ -4783,7 +4804,7 @@
         <v>-2.2549999999999999</v>
       </c>
       <c r="G148">
-        <v>0.95</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="149" spans="3:8" ht="51" x14ac:dyDescent="0.2">
@@ -4791,17 +4812,17 @@
         <v>69</v>
       </c>
       <c r="D149" s="7">
-        <v>-1.427</v>
+        <v>-2.2130000000000001</v>
       </c>
       <c r="E149">
         <v>6</v>
       </c>
       <c r="F149" s="1">
         <f t="shared" si="8"/>
-        <v>-1.367</v>
+        <v>-2.153</v>
       </c>
       <c r="G149">
-        <v>0.17</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="150" spans="3:8" ht="17" x14ac:dyDescent="0.2">
@@ -5181,17 +5202,17 @@
         <v>63</v>
       </c>
       <c r="D173">
-        <v>-0.36099999999999999</v>
+        <v>-4.4039999999999999</v>
       </c>
       <c r="E173">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F173" s="1">
         <f t="shared" si="9"/>
-        <v>-0.34099999999999997</v>
+        <v>-4.3440000000000003</v>
       </c>
       <c r="G173">
-        <v>0.47</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="174" spans="3:8" x14ac:dyDescent="0.2">
@@ -5199,14 +5220,14 @@
         <v>62</v>
       </c>
       <c r="D174">
-        <v>-3.113</v>
+        <v>-3.6659999999999999</v>
       </c>
       <c r="E174">
         <v>6</v>
       </c>
       <c r="F174" s="1">
         <f t="shared" si="9"/>
-        <v>-3.0529999999999999</v>
+        <v>-3.6059999999999999</v>
       </c>
       <c r="G174">
         <v>0.25</v>
@@ -5217,17 +5238,17 @@
         <v>68</v>
       </c>
       <c r="D175">
-        <v>-0.36099999999999999</v>
+        <v>-4.4039999999999999</v>
       </c>
       <c r="E175">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F175" s="1">
         <f>D175+E175*0.01</f>
-        <v>-0.34099999999999997</v>
+        <v>-4.3440000000000003</v>
       </c>
       <c r="G175">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="176" spans="3:8" ht="51" x14ac:dyDescent="0.2">
@@ -5235,14 +5256,14 @@
         <v>69</v>
       </c>
       <c r="D176">
-        <v>-3.113</v>
+        <v>-3.6659999999999999</v>
       </c>
       <c r="E176">
         <v>6</v>
       </c>
       <c r="F176" s="1">
         <f>D176+E176*0.01</f>
-        <v>-3.0529999999999999</v>
+        <v>-3.6059999999999999</v>
       </c>
       <c r="G176">
         <v>0.26</v>
@@ -5643,17 +5664,17 @@
         <v>62</v>
       </c>
       <c r="D201">
-        <v>-2.3340000000000001</v>
+        <v>-2.9649999999999999</v>
       </c>
       <c r="E201">
         <v>6</v>
       </c>
       <c r="F201" s="1">
         <f t="shared" si="10"/>
-        <v>-2.274</v>
+        <v>-2.9049999999999998</v>
       </c>
       <c r="G201">
-        <v>0.17</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.2">
@@ -5679,17 +5700,17 @@
         <v>69</v>
       </c>
       <c r="D203">
-        <v>-2.3340000000000001</v>
+        <v>-2.9649999999999999</v>
       </c>
       <c r="E203">
         <v>6</v>
       </c>
       <c r="F203" s="1">
         <f t="shared" si="11"/>
-        <v>-2.274</v>
+        <v>-2.9049999999999998</v>
       </c>
       <c r="G203">
-        <v>0.33</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="204" spans="3:7" ht="17" x14ac:dyDescent="0.2">
@@ -6069,17 +6090,17 @@
         <v>63</v>
       </c>
       <c r="D227">
-        <v>0</v>
+        <v>-3.613</v>
       </c>
       <c r="E227">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F227" s="1">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>-3.5529999999999999</v>
       </c>
       <c r="G227">
-        <v>0.23</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="228" spans="3:7" x14ac:dyDescent="0.2">
@@ -6087,17 +6108,17 @@
         <v>62</v>
       </c>
       <c r="D228">
-        <v>-2.0859999999999999</v>
+        <v>-3.371</v>
       </c>
       <c r="E228">
         <v>6</v>
       </c>
       <c r="F228" s="1">
         <f t="shared" si="13"/>
-        <v>-2.0259999999999998</v>
+        <v>-3.3109999999999999</v>
       </c>
       <c r="G228">
-        <v>0.24</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="229" spans="3:7" x14ac:dyDescent="0.2">
@@ -6105,17 +6126,17 @@
         <v>68</v>
       </c>
       <c r="D229">
-        <v>0</v>
+        <v>-3.613</v>
       </c>
       <c r="E229">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F229" s="1">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>-3.5529999999999999</v>
       </c>
       <c r="G229">
-        <v>0.19</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="230" spans="3:7" ht="51" x14ac:dyDescent="0.2">
@@ -6123,17 +6144,17 @@
         <v>69</v>
       </c>
       <c r="D230">
-        <v>-2.0859999999999999</v>
+        <v>-3.371</v>
       </c>
       <c r="E230">
         <v>6</v>
       </c>
       <c r="F230" s="1">
         <f t="shared" si="13"/>
-        <v>-2.0259999999999998</v>
+        <v>-3.3109999999999999</v>
       </c>
       <c r="G230">
-        <v>0.23</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="231" spans="3:7" ht="17" x14ac:dyDescent="0.2">
@@ -6531,17 +6552,17 @@
         <v>62</v>
       </c>
       <c r="D255">
-        <v>-1.391</v>
+        <v>-2.9649999999999999</v>
       </c>
       <c r="E255">
         <v>6</v>
       </c>
       <c r="F255" s="1">
         <f t="shared" si="14"/>
-        <v>-1.331</v>
+        <v>-2.9049999999999998</v>
       </c>
       <c r="G255">
-        <v>0.17</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="256" spans="3:8" x14ac:dyDescent="0.2">
@@ -6567,17 +6588,17 @@
         <v>69</v>
       </c>
       <c r="D257">
-        <v>-1.391</v>
+        <v>-2.9649999999999999</v>
       </c>
       <c r="E257">
         <v>6</v>
       </c>
       <c r="F257" s="1">
         <f t="shared" si="14"/>
-        <v>-1.331</v>
+        <v>-2.9049999999999998</v>
       </c>
       <c r="G257">
-        <v>0.17</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="258" spans="3:8" ht="17" x14ac:dyDescent="0.2">
@@ -6834,7 +6855,7 @@
         <f t="shared" si="16"/>
         <v>-3.8537999999999997</v>
       </c>
-      <c r="E272" s="20">
+      <c r="E272" s="18">
         <f t="shared" si="16"/>
         <v>38.799999999999997</v>
       </c>
@@ -6852,7 +6873,7 @@
         <f t="shared" si="16"/>
         <v>-1.5484000000000002</v>
       </c>
-      <c r="E273" s="20">
+      <c r="E273" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
@@ -6870,7 +6891,7 @@
         <f t="shared" si="16"/>
         <v>-3.7063999999999999</v>
       </c>
-      <c r="E274" s="20">
+      <c r="E274" s="18">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
@@ -6888,7 +6909,7 @@
         <f t="shared" si="16"/>
         <v>-3.8326000000000002</v>
       </c>
-      <c r="E275" s="20">
+      <c r="E275" s="18">
         <f t="shared" si="16"/>
         <v>52.8</v>
       </c>
@@ -6906,7 +6927,7 @@
         <f t="shared" si="16"/>
         <v>-1.9104000000000003</v>
       </c>
-      <c r="E276" s="20">
+      <c r="E276" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
@@ -6924,7 +6945,7 @@
         <f t="shared" si="16"/>
         <v>-3.7299999999999995</v>
       </c>
-      <c r="E277" s="20">
+      <c r="E277" s="18">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
@@ -6942,7 +6963,7 @@
         <f t="shared" si="16"/>
         <v>-3.8540000000000001</v>
       </c>
-      <c r="E278" s="20">
+      <c r="E278" s="18">
         <f t="shared" si="16"/>
         <v>43.6</v>
       </c>
@@ -6960,7 +6981,7 @@
         <f t="shared" si="16"/>
         <v>-1.8676000000000001</v>
       </c>
-      <c r="E279" s="20">
+      <c r="E279" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
@@ -6978,7 +6999,7 @@
         <f t="shared" si="16"/>
         <v>-3.6514000000000002</v>
       </c>
-      <c r="E280" s="20">
+      <c r="E280" s="18">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
@@ -6994,19 +7015,19 @@
       </c>
       <c r="D281" s="1">
         <f t="shared" si="16"/>
-        <v>-1.7986</v>
-      </c>
-      <c r="E281" s="20">
+        <v>-3.3298000000000001</v>
+      </c>
+      <c r="E281" s="18">
         <f t="shared" si="16"/>
-        <v>4.4000000000000004</v>
+        <v>6</v>
       </c>
       <c r="F281" s="1">
         <f t="shared" si="16"/>
-        <v>-1.7545999999999999</v>
+        <v>-3.2698</v>
       </c>
       <c r="G281" s="3">
         <f>AVERAGE(G146,G173,G200,G227,G254)</f>
-        <v>0.73199999999999998</v>
+        <v>0.85399999999999987</v>
       </c>
     </row>
     <row r="282" spans="3:7" x14ac:dyDescent="0.2">
@@ -7015,19 +7036,19 @@
       </c>
       <c r="D282" s="1">
         <f t="shared" si="16"/>
-        <v>-2.0702000000000003</v>
-      </c>
-      <c r="E282" s="20">
+        <v>-3.036</v>
+      </c>
+      <c r="E282" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F282" s="1">
         <f t="shared" si="16"/>
-        <v>-2.0101999999999998</v>
+        <v>-2.976</v>
       </c>
       <c r="G282" s="3">
         <f t="shared" si="16"/>
-        <v>0.20200000000000001</v>
+        <v>0.49800000000000005</v>
       </c>
     </row>
     <row r="283" spans="3:7" x14ac:dyDescent="0.2">
@@ -7036,19 +7057,19 @@
       </c>
       <c r="D283" s="1">
         <f t="shared" si="16"/>
-        <v>-1.7986</v>
-      </c>
-      <c r="E283" s="20">
+        <v>-3.3298000000000001</v>
+      </c>
+      <c r="E283" s="18">
         <f t="shared" si="16"/>
-        <v>4.4000000000000004</v>
+        <v>6</v>
       </c>
       <c r="F283" s="1">
         <f t="shared" si="16"/>
-        <v>-1.7545999999999999</v>
+        <v>-3.2698</v>
       </c>
       <c r="G283" s="3">
         <f t="shared" si="16"/>
-        <v>0.78200000000000003</v>
+        <v>0.89599999999999991</v>
       </c>
     </row>
     <row r="284" spans="3:7" ht="51" x14ac:dyDescent="0.2">
@@ -7057,19 +7078,19 @@
       </c>
       <c r="D284" s="1">
         <f t="shared" si="16"/>
-        <v>-2.0702000000000003</v>
-      </c>
-      <c r="E284" s="20">
+        <v>-3.036</v>
+      </c>
+      <c r="E284" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F284" s="1">
         <f t="shared" si="16"/>
-        <v>-2.0101999999999998</v>
+        <v>-2.976</v>
       </c>
       <c r="G284" s="3">
         <f t="shared" si="16"/>
-        <v>0.23199999999999998</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="285" spans="3:7" ht="17" x14ac:dyDescent="0.2">
@@ -7080,7 +7101,7 @@
         <f t="shared" si="16"/>
         <v>-3.8457999999999992</v>
       </c>
-      <c r="E285" s="20">
+      <c r="E285" s="18">
         <f t="shared" si="16"/>
         <v>32.4</v>
       </c>
@@ -7101,7 +7122,7 @@
         <f t="shared" si="16"/>
         <v>-2.7090000000000005</v>
       </c>
-      <c r="E286" s="20">
+      <c r="E286" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
@@ -7122,7 +7143,7 @@
         <f t="shared" si="16"/>
         <v>-3.7887999999999997</v>
       </c>
-      <c r="E287" s="20">
+      <c r="E287" s="18">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
@@ -7143,7 +7164,7 @@
         <f t="shared" si="16"/>
         <v>-3.8404000000000003</v>
       </c>
-      <c r="E288" s="20">
+      <c r="E288" s="18">
         <f t="shared" si="16"/>
         <v>50</v>
       </c>
@@ -7164,7 +7185,7 @@
         <f t="shared" si="16"/>
         <v>-2.6142000000000003</v>
       </c>
-      <c r="E289" s="20">
+      <c r="E289" s="18">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
@@ -7185,7 +7206,7 @@
         <f t="shared" si="16"/>
         <v>-3.7518000000000002</v>
       </c>
-      <c r="E290" s="20">
+      <c r="E290" s="18">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
@@ -7206,7 +7227,7 @@
         <f t="shared" si="16"/>
         <v>-3.8536000000000001</v>
       </c>
-      <c r="E291" s="20">
+      <c r="E291" s="18">
         <f t="shared" si="16"/>
         <v>40.4</v>
       </c>
@@ -7227,7 +7248,7 @@
         <f t="shared" si="16"/>
         <v>-2.7090000000000005</v>
       </c>
-      <c r="E292" s="20">
+      <c r="E292" s="18">
         <f t="shared" ref="E292:G292" si="17">AVERAGE(E157,E184,E211,E238,E265)</f>
         <v>6</v>
       </c>
@@ -7248,7 +7269,7 @@
         <f t="shared" si="16"/>
         <v>-3.7814000000000001</v>
       </c>
-      <c r="E293" s="20">
+      <c r="E293" s="18">
         <f t="shared" ref="E293:G293" si="18">AVERAGE(E158,E185,E212,E239,E266)</f>
         <v>10</v>
       </c>
@@ -7291,7 +7312,7 @@
         <f t="shared" si="19"/>
         <v>7.616736177655115</v>
       </c>
-      <c r="H296" s="19">
+      <c r="H296" s="17">
         <f>STDEV(H134,H161,H188,H215,H242)</f>
         <v>4.2630078698567039E-2</v>
       </c>
@@ -7316,7 +7337,7 @@
         <f t="shared" si="20"/>
         <v>233.72305866131413</v>
       </c>
-      <c r="H297" s="19">
+      <c r="H297" s="17">
         <f t="shared" si="20"/>
         <v>4.4899402760503679E-2</v>
       </c>
@@ -7341,7 +7362,7 @@
         <f t="shared" si="20"/>
         <v>156.62305322014373</v>
       </c>
-      <c r="H298" s="19">
+      <c r="H298" s="17">
         <f t="shared" si="20"/>
         <v>4.2806759580872412E-2</v>
       </c>
@@ -7514,19 +7535,19 @@
       </c>
       <c r="D308" s="1">
         <f t="shared" si="20"/>
-        <v>1.5231763850585396</v>
+        <v>0.76418237352087437</v>
       </c>
       <c r="E308" s="1">
         <f t="shared" si="20"/>
-        <v>2.1908902300206647</v>
+        <v>0</v>
       </c>
       <c r="F308" s="1">
         <f t="shared" si="20"/>
-        <v>1.5019395127634139</v>
+        <v>0.76418237352087659</v>
       </c>
       <c r="G308" s="1">
         <f t="shared" si="20"/>
-        <v>0.36148305631108085</v>
+        <v>0.10968135666557105</v>
       </c>
     </row>
     <row r="309" spans="3:7" x14ac:dyDescent="0.2">
@@ -7535,7 +7556,7 @@
       </c>
       <c r="D309" s="1">
         <f t="shared" si="20"/>
-        <v>0.7127921857035181</v>
+        <v>0.54693143994471438</v>
       </c>
       <c r="E309" s="1">
         <f t="shared" si="20"/>
@@ -7543,11 +7564,11 @@
       </c>
       <c r="F309" s="1">
         <f t="shared" si="20"/>
-        <v>0.71279218570351943</v>
+        <v>0.5469314399447176</v>
       </c>
       <c r="G309" s="1">
         <f t="shared" si="20"/>
-        <v>3.9623225512317922E-2</v>
+        <v>0.17683325479106005</v>
       </c>
     </row>
     <row r="310" spans="3:7" x14ac:dyDescent="0.2">
@@ -7556,19 +7577,19 @@
       </c>
       <c r="D310" s="1">
         <f t="shared" si="20"/>
-        <v>1.5231763850585396</v>
+        <v>0.76418237352087437</v>
       </c>
       <c r="E310" s="1">
         <f t="shared" si="20"/>
-        <v>2.1908902300206647</v>
+        <v>0</v>
       </c>
       <c r="F310" s="1">
         <f t="shared" si="20"/>
-        <v>1.5019395127634139</v>
+        <v>0.76418237352087659</v>
       </c>
       <c r="G310" s="1">
         <f t="shared" si="20"/>
-        <v>0.4297324749189893</v>
+        <v>0.2369177072318577</v>
       </c>
     </row>
     <row r="311" spans="3:7" ht="51" x14ac:dyDescent="0.2">
@@ -7577,7 +7598,7 @@
       </c>
       <c r="D311" s="1">
         <f t="shared" si="20"/>
-        <v>0.7127921857035181</v>
+        <v>0.54693143994471438</v>
       </c>
       <c r="E311" s="1">
         <f t="shared" si="20"/>
@@ -7585,11 +7606,11 @@
       </c>
       <c r="F311" s="1">
         <f t="shared" si="20"/>
-        <v>0.71279218570351943</v>
+        <v>0.5469314399447176</v>
       </c>
       <c r="G311" s="1">
         <f t="shared" si="20"/>
-        <v>6.7230945255886521E-2</v>
+        <v>0.20554804791094469</v>
       </c>
     </row>
     <row r="312" spans="3:7" ht="17" x14ac:dyDescent="0.2">
@@ -8053,7 +8074,7 @@
         <f>D342+E342*0.01</f>
         <v>-1.2429999999999999</v>
       </c>
-      <c r="G342" s="21">
+      <c r="G342" s="19">
         <v>4877.3500000000004</v>
       </c>
     </row>
@@ -8073,6 +8094,1188 @@
       </c>
       <c r="G343">
         <v>4399.54</v>
+      </c>
+    </row>
+    <row r="348" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C348" t="s">
+        <v>435</v>
+      </c>
+      <c r="D348">
+        <v>-0.999</v>
+      </c>
+      <c r="E348">
+        <v>8</v>
+      </c>
+      <c r="F348">
+        <f>D348+E348*0.01</f>
+        <v>-0.91900000000000004</v>
+      </c>
+      <c r="G348">
+        <v>0.09</v>
+      </c>
+      <c r="H348">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="349" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C349" t="s">
+        <v>276</v>
+      </c>
+      <c r="D349">
+        <v>-0.999</v>
+      </c>
+      <c r="E349">
+        <v>8</v>
+      </c>
+      <c r="F349">
+        <f>D349+E349*0.01</f>
+        <v>-0.91900000000000004</v>
+      </c>
+      <c r="G349">
+        <v>0.27</v>
+      </c>
+      <c r="H349">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="350" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C350" t="s">
+        <v>436</v>
+      </c>
+      <c r="D350">
+        <v>-0.999</v>
+      </c>
+      <c r="E350">
+        <v>12</v>
+      </c>
+      <c r="F350">
+        <f t="shared" ref="F350:F353" si="23">D350+E350*0.01</f>
+        <v>-0.879</v>
+      </c>
+      <c r="G350">
+        <v>0.13</v>
+      </c>
+      <c r="H350">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="351" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C351" t="s">
+        <v>437</v>
+      </c>
+      <c r="D351">
+        <v>-0.90900000000000003</v>
+      </c>
+      <c r="E351">
+        <v>4</v>
+      </c>
+      <c r="F351">
+        <f t="shared" si="23"/>
+        <v>-0.86899999999999999</v>
+      </c>
+      <c r="G351">
+        <v>0.02</v>
+      </c>
+      <c r="H351">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C352" t="s">
+        <v>438</v>
+      </c>
+      <c r="D352">
+        <v>-0.90900000000000003</v>
+      </c>
+      <c r="E352">
+        <v>4</v>
+      </c>
+      <c r="F352">
+        <f t="shared" si="23"/>
+        <v>-0.86899999999999999</v>
+      </c>
+      <c r="G352">
+        <v>0.04</v>
+      </c>
+      <c r="H352">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C353" t="s">
+        <v>439</v>
+      </c>
+      <c r="D353">
+        <v>-0.76500000000000001</v>
+      </c>
+      <c r="E353">
+        <v>6</v>
+      </c>
+      <c r="F353">
+        <f t="shared" si="23"/>
+        <v>-0.70500000000000007</v>
+      </c>
+      <c r="G353">
+        <v>0.01</v>
+      </c>
+      <c r="H353">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="355" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C355" t="s">
+        <v>435</v>
+      </c>
+      <c r="D355">
+        <v>-3.9969999999999999</v>
+      </c>
+      <c r="E355">
+        <v>6</v>
+      </c>
+      <c r="F355">
+        <f>D355+E355*0.01</f>
+        <v>-3.9369999999999998</v>
+      </c>
+      <c r="G355">
+        <v>0.15</v>
+      </c>
+      <c r="H355">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="356" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C356" t="s">
+        <v>276</v>
+      </c>
+      <c r="D356">
+        <v>-3.9990000000000001</v>
+      </c>
+      <c r="E356">
+        <v>14</v>
+      </c>
+      <c r="F356">
+        <f>D356+E356*0.01</f>
+        <v>-3.859</v>
+      </c>
+      <c r="G356" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="H356" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="357" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C357" t="s">
+        <v>436</v>
+      </c>
+      <c r="D357">
+        <v>-3.9969999999999999</v>
+      </c>
+      <c r="E357">
+        <v>6</v>
+      </c>
+      <c r="F357">
+        <f t="shared" ref="F357:G377" si="24">D357+E357*0.01</f>
+        <v>-3.9369999999999998</v>
+      </c>
+      <c r="G357">
+        <v>0.16</v>
+      </c>
+      <c r="H357" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
+        <v>437</v>
+      </c>
+      <c r="D358">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E358">
+        <v>6</v>
+      </c>
+      <c r="F358">
+        <f t="shared" si="24"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G358">
+        <v>0.04</v>
+      </c>
+      <c r="H358" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C359" t="s">
+        <v>438</v>
+      </c>
+      <c r="D359">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E359">
+        <v>6</v>
+      </c>
+      <c r="F359">
+        <f t="shared" si="24"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G359">
+        <v>0.03</v>
+      </c>
+      <c r="H359" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C360" t="s">
+        <v>439</v>
+      </c>
+      <c r="D360">
+        <v>-3.8839999999999999</v>
+      </c>
+      <c r="E360">
+        <v>6</v>
+      </c>
+      <c r="F360">
+        <f t="shared" si="24"/>
+        <v>-3.8239999999999998</v>
+      </c>
+      <c r="G360">
+        <v>0.03</v>
+      </c>
+      <c r="H360" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="362" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C362" t="s">
+        <v>435</v>
+      </c>
+      <c r="D362">
+        <v>-2.8780000000000001</v>
+      </c>
+      <c r="E362">
+        <v>14</v>
+      </c>
+      <c r="F362">
+        <f t="shared" si="24"/>
+        <v>-2.738</v>
+      </c>
+      <c r="G362">
+        <v>4.03</v>
+      </c>
+      <c r="H362">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="363" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C363" t="s">
+        <v>276</v>
+      </c>
+      <c r="D363">
+        <v>-2.883</v>
+      </c>
+      <c r="E363">
+        <v>22</v>
+      </c>
+      <c r="F363">
+        <f t="shared" si="24"/>
+        <v>-2.6629999999999998</v>
+      </c>
+      <c r="G363">
+        <v>22.19</v>
+      </c>
+      <c r="H363">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="364" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
+        <v>436</v>
+      </c>
+      <c r="D364">
+        <v>-2.8780000000000001</v>
+      </c>
+      <c r="E364">
+        <v>14</v>
+      </c>
+      <c r="F364">
+        <f t="shared" si="24"/>
+        <v>-2.738</v>
+      </c>
+      <c r="G364">
+        <v>3.4</v>
+      </c>
+      <c r="H364">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="365" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C365" t="s">
+        <v>437</v>
+      </c>
+      <c r="D365">
+        <v>-2.2130000000000001</v>
+      </c>
+      <c r="E365">
+        <v>6</v>
+      </c>
+      <c r="F365">
+        <f t="shared" si="24"/>
+        <v>-2.153</v>
+      </c>
+      <c r="G365">
+        <v>0.49</v>
+      </c>
+      <c r="H365">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="366" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C366" t="s">
+        <v>438</v>
+      </c>
+      <c r="D366">
+        <v>-2.2130000000000001</v>
+      </c>
+      <c r="E366">
+        <v>6</v>
+      </c>
+      <c r="F366">
+        <f t="shared" si="24"/>
+        <v>-2.153</v>
+      </c>
+      <c r="G366">
+        <v>0.42</v>
+      </c>
+      <c r="H366">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="367" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C367" t="s">
+        <v>439</v>
+      </c>
+      <c r="D367">
+        <v>-2.2130000000000001</v>
+      </c>
+      <c r="E367">
+        <v>6</v>
+      </c>
+      <c r="F367">
+        <f t="shared" si="24"/>
+        <v>-2.153</v>
+      </c>
+      <c r="G367">
+        <v>0.4</v>
+      </c>
+      <c r="H367">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="369" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C369" t="s">
+        <v>435</v>
+      </c>
+      <c r="D369">
+        <v>-5.3120000000000003</v>
+      </c>
+      <c r="E369">
+        <v>22</v>
+      </c>
+      <c r="F369">
+        <f t="shared" si="24"/>
+        <v>-5.0920000000000005</v>
+      </c>
+      <c r="G369">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="H369">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="370" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C370" t="s">
+        <v>276</v>
+      </c>
+      <c r="D370">
+        <v>-5.3049999999999997</v>
+      </c>
+      <c r="E370">
+        <v>18</v>
+      </c>
+      <c r="F370">
+        <f t="shared" si="24"/>
+        <v>-5.125</v>
+      </c>
+      <c r="G370">
+        <v>14.34</v>
+      </c>
+      <c r="H370">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="371" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C371" t="s">
+        <v>436</v>
+      </c>
+      <c r="D371">
+        <v>-5.3159999999999998</v>
+      </c>
+      <c r="E371">
+        <v>26</v>
+      </c>
+      <c r="F371">
+        <f t="shared" si="24"/>
+        <v>-5.056</v>
+      </c>
+      <c r="G371">
+        <v>21.83</v>
+      </c>
+      <c r="H371">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="372" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C372" t="s">
+        <v>437</v>
+      </c>
+      <c r="D372">
+        <v>-2.1</v>
+      </c>
+      <c r="E372">
+        <v>6</v>
+      </c>
+      <c r="F372">
+        <f t="shared" si="24"/>
+        <v>-2.04</v>
+      </c>
+      <c r="G372">
+        <v>0.11</v>
+      </c>
+      <c r="H372">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="373" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C373" t="s">
+        <v>438</v>
+      </c>
+      <c r="D373">
+        <v>-3.6659999999999999</v>
+      </c>
+      <c r="E373">
+        <v>6</v>
+      </c>
+      <c r="F373">
+        <f t="shared" si="24"/>
+        <v>-3.6059999999999999</v>
+      </c>
+      <c r="G373">
+        <v>0.37</v>
+      </c>
+      <c r="H373">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="374" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
+        <v>439</v>
+      </c>
+      <c r="D374">
+        <v>-2.1</v>
+      </c>
+      <c r="E374">
+        <v>6</v>
+      </c>
+      <c r="F374">
+        <f t="shared" si="24"/>
+        <v>-2.04</v>
+      </c>
+      <c r="G374">
+        <v>0.11</v>
+      </c>
+      <c r="H374">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="376" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C376" t="s">
+        <v>435</v>
+      </c>
+      <c r="D376">
+        <v>-3.7309999999999999</v>
+      </c>
+      <c r="E376">
+        <v>26</v>
+      </c>
+      <c r="F376">
+        <f t="shared" si="24"/>
+        <v>-3.4710000000000001</v>
+      </c>
+      <c r="G376">
+        <v>20.29</v>
+      </c>
+      <c r="H376">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="377" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C377" t="s">
+        <v>276</v>
+      </c>
+      <c r="D377">
+        <v>-3.7280000000000002</v>
+      </c>
+      <c r="E377">
+        <v>22</v>
+      </c>
+      <c r="F377">
+        <f t="shared" si="24"/>
+        <v>-3.508</v>
+      </c>
+      <c r="G377">
+        <v>21.52</v>
+      </c>
+      <c r="H377">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="378" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C378" t="s">
+        <v>436</v>
+      </c>
+      <c r="D378">
+        <v>-3.7280000000000002</v>
+      </c>
+      <c r="E378">
+        <v>22</v>
+      </c>
+      <c r="F378">
+        <f t="shared" ref="F378:H395" si="25">D378+E378*0.01</f>
+        <v>-3.508</v>
+      </c>
+      <c r="G378">
+        <v>14.01</v>
+      </c>
+      <c r="H378">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="379" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C379" t="s">
+        <v>437</v>
+      </c>
+      <c r="D379">
+        <v>-2.9649999999999999</v>
+      </c>
+      <c r="E379">
+        <v>6</v>
+      </c>
+      <c r="F379">
+        <f t="shared" si="25"/>
+        <v>-2.9049999999999998</v>
+      </c>
+      <c r="G379">
+        <v>0.51</v>
+      </c>
+      <c r="H379">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C380" t="s">
+        <v>438</v>
+      </c>
+      <c r="D380">
+        <v>-2.9649999999999999</v>
+      </c>
+      <c r="E380">
+        <v>6</v>
+      </c>
+      <c r="F380">
+        <f t="shared" si="25"/>
+        <v>-2.9049999999999998</v>
+      </c>
+      <c r="G380">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H380">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="381" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C381" t="s">
+        <v>439</v>
+      </c>
+      <c r="D381">
+        <v>-2.9649999999999999</v>
+      </c>
+      <c r="E381">
+        <v>6</v>
+      </c>
+      <c r="F381">
+        <f t="shared" si="25"/>
+        <v>-2.9049999999999998</v>
+      </c>
+      <c r="G381">
+        <v>0.77</v>
+      </c>
+      <c r="H381">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="383" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C383" t="s">
+        <v>435</v>
+      </c>
+      <c r="D383">
+        <v>-4.0730000000000004</v>
+      </c>
+      <c r="E383">
+        <v>14</v>
+      </c>
+      <c r="F383">
+        <f t="shared" si="25"/>
+        <v>-3.9330000000000003</v>
+      </c>
+      <c r="G383">
+        <v>6.87</v>
+      </c>
+      <c r="H383">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="384" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C384" t="s">
+        <v>276</v>
+      </c>
+      <c r="D384">
+        <v>-4.0730000000000004</v>
+      </c>
+      <c r="E384">
+        <v>14</v>
+      </c>
+      <c r="F384">
+        <f t="shared" si="25"/>
+        <v>-3.9330000000000003</v>
+      </c>
+      <c r="G384">
+        <v>7.84</v>
+      </c>
+      <c r="H384">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="385" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C385" t="s">
+        <v>436</v>
+      </c>
+      <c r="D385">
+        <v>-4.0449999999999999</v>
+      </c>
+      <c r="E385">
+        <v>10</v>
+      </c>
+      <c r="F385">
+        <f t="shared" si="25"/>
+        <v>-3.9449999999999998</v>
+      </c>
+      <c r="G385">
+        <v>1.75</v>
+      </c>
+      <c r="H385">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="386" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C386" t="s">
+        <v>437</v>
+      </c>
+      <c r="D386">
+        <v>-2.681</v>
+      </c>
+      <c r="E386">
+        <v>4</v>
+      </c>
+      <c r="F386">
+        <f t="shared" si="25"/>
+        <v>-2.641</v>
+      </c>
+      <c r="G386">
+        <v>0.3</v>
+      </c>
+      <c r="H386">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="387" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C387" t="s">
+        <v>438</v>
+      </c>
+      <c r="D387">
+        <v>-3.371</v>
+      </c>
+      <c r="E387">
+        <v>6</v>
+      </c>
+      <c r="F387">
+        <f t="shared" si="25"/>
+        <v>-3.3109999999999999</v>
+      </c>
+      <c r="G387">
+        <v>0.54</v>
+      </c>
+      <c r="H387">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="388" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C388" t="s">
+        <v>439</v>
+      </c>
+      <c r="D388">
+        <v>-3.371</v>
+      </c>
+      <c r="E388">
+        <v>6</v>
+      </c>
+      <c r="F388">
+        <f t="shared" si="25"/>
+        <v>-3.3109999999999999</v>
+      </c>
+      <c r="G388">
+        <v>0.62</v>
+      </c>
+      <c r="H388">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="390" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C390" t="s">
+        <v>435</v>
+      </c>
+      <c r="D390">
+        <v>-3.2879999999999998</v>
+      </c>
+      <c r="E390">
+        <v>22</v>
+      </c>
+      <c r="F390">
+        <f t="shared" si="25"/>
+        <v>-3.0679999999999996</v>
+      </c>
+      <c r="G390">
+        <v>29.41</v>
+      </c>
+      <c r="H390">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="391" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C391" t="s">
+        <v>276</v>
+      </c>
+      <c r="D391">
+        <v>-3.286</v>
+      </c>
+      <c r="E391">
+        <v>18</v>
+      </c>
+      <c r="F391">
+        <f t="shared" si="25"/>
+        <v>-3.1059999999999999</v>
+      </c>
+      <c r="G391">
+        <v>16.72</v>
+      </c>
+      <c r="H391">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="392" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C392" t="s">
+        <v>436</v>
+      </c>
+      <c r="D392">
+        <v>-3.282</v>
+      </c>
+      <c r="E392">
+        <v>14</v>
+      </c>
+      <c r="F392">
+        <f t="shared" si="25"/>
+        <v>-3.1419999999999999</v>
+      </c>
+      <c r="G392">
+        <v>6.15</v>
+      </c>
+      <c r="H392">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="393" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C393" t="s">
+        <v>437</v>
+      </c>
+      <c r="D393">
+        <v>-2.9340000000000002</v>
+      </c>
+      <c r="E393">
+        <v>6</v>
+      </c>
+      <c r="F393">
+        <f t="shared" si="25"/>
+        <v>-2.8740000000000001</v>
+      </c>
+      <c r="G393">
+        <v>0.67</v>
+      </c>
+      <c r="H393">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="394" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C394" t="s">
+        <v>438</v>
+      </c>
+      <c r="D394">
+        <v>-2.9340000000000002</v>
+      </c>
+      <c r="E394">
+        <v>6</v>
+      </c>
+      <c r="F394">
+        <f t="shared" si="25"/>
+        <v>-2.8740000000000001</v>
+      </c>
+      <c r="G394">
+        <v>0.61</v>
+      </c>
+      <c r="H394">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="395" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C395" t="s">
+        <v>439</v>
+      </c>
+      <c r="D395">
+        <v>-2.9340000000000002</v>
+      </c>
+      <c r="E395">
+        <v>6</v>
+      </c>
+      <c r="F395">
+        <f t="shared" si="25"/>
+        <v>-2.8740000000000001</v>
+      </c>
+      <c r="G395">
+        <v>0.66</v>
+      </c>
+      <c r="H395">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="397" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C397" t="s">
+        <v>435</v>
+      </c>
+      <c r="D397" s="1">
+        <f>AVERAGE(D362,D369,D376,D383,D390)</f>
+        <v>-3.8563999999999998</v>
+      </c>
+      <c r="E397">
+        <f>AVERAGE(E362,E369,E376,E383,E390)</f>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="F397" s="1">
+        <f>AVERAGE(F362,F369,F376,F383,F390)</f>
+        <v>-3.6604000000000001</v>
+      </c>
+      <c r="G397" s="3">
+        <f>AVERAGE(G362,G369,G376,G383,G390)</f>
+        <v>15.408000000000001</v>
+      </c>
+      <c r="H397">
+        <f>AVERAGE(H362,H369,H376,H383,H390)</f>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="398" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C398" t="s">
+        <v>276</v>
+      </c>
+      <c r="D398" s="1">
+        <f t="shared" ref="D398:H398" si="26">AVERAGE(D363,D370,D377,D384,D391)</f>
+        <v>-3.8549999999999995</v>
+      </c>
+      <c r="E398">
+        <f t="shared" si="26"/>
+        <v>18.8</v>
+      </c>
+      <c r="F398" s="1">
+        <f t="shared" si="26"/>
+        <v>-3.6670000000000003</v>
+      </c>
+      <c r="G398" s="3">
+        <f t="shared" si="26"/>
+        <v>16.521999999999998</v>
+      </c>
+      <c r="H398">
+        <f t="shared" si="26"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="399" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C399" t="s">
+        <v>436</v>
+      </c>
+      <c r="D399" s="1">
+        <f t="shared" ref="D399:H399" si="27">AVERAGE(D364,D371,D378,D385,D392)</f>
+        <v>-3.8497999999999997</v>
+      </c>
+      <c r="E399">
+        <f t="shared" si="27"/>
+        <v>17.2</v>
+      </c>
+      <c r="F399" s="1">
+        <f t="shared" si="27"/>
+        <v>-3.6778</v>
+      </c>
+      <c r="G399" s="3">
+        <f t="shared" si="27"/>
+        <v>9.427999999999999</v>
+      </c>
+      <c r="H399">
+        <f t="shared" si="27"/>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="400" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C400" t="s">
+        <v>437</v>
+      </c>
+      <c r="D400" s="1">
+        <f t="shared" ref="D400:H400" si="28">AVERAGE(D365,D372,D379,D386,D393)</f>
+        <v>-2.5786000000000002</v>
+      </c>
+      <c r="E400">
+        <f t="shared" si="28"/>
+        <v>5.6</v>
+      </c>
+      <c r="F400" s="1">
+        <f t="shared" si="28"/>
+        <v>-2.5225999999999997</v>
+      </c>
+      <c r="G400" s="3">
+        <f t="shared" si="28"/>
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="H400">
+        <f t="shared" si="28"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="401" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C401" t="s">
+        <v>438</v>
+      </c>
+      <c r="D401" s="1">
+        <f t="shared" ref="D401:H401" si="29">AVERAGE(D366,D373,D380,D387,D394)</f>
+        <v>-3.0298000000000003</v>
+      </c>
+      <c r="E401">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="F401" s="1">
+        <f t="shared" si="29"/>
+        <v>-2.9698000000000002</v>
+      </c>
+      <c r="G401" s="3">
+        <f t="shared" si="29"/>
+        <v>0.5</v>
+      </c>
+      <c r="H401">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="402" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C402" t="s">
+        <v>439</v>
+      </c>
+      <c r="D402" s="1">
+        <f t="shared" ref="D402:H402" si="30">AVERAGE(D367,D374,D381,D388,D395)</f>
+        <v>-2.7166000000000006</v>
+      </c>
+      <c r="E402">
+        <f t="shared" si="30"/>
+        <v>6</v>
+      </c>
+      <c r="F402" s="1">
+        <f t="shared" si="30"/>
+        <v>-2.6566000000000001</v>
+      </c>
+      <c r="G402" s="3">
+        <f t="shared" si="30"/>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H402">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="404" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C404" t="s">
+        <v>435</v>
+      </c>
+      <c r="D404">
+        <f>STDEV(D362,D369,D376,D383,D390)</f>
+        <v>0.93028990105235587</v>
+      </c>
+      <c r="E404">
+        <f t="shared" ref="E404:H404" si="31">STDEV(E362,E369,E376,E383,E390)</f>
+        <v>5.3665631459994962</v>
+      </c>
+      <c r="F404">
+        <f t="shared" si="31"/>
+        <v>0.91670895053992052</v>
+      </c>
+      <c r="G404">
+        <f t="shared" si="31"/>
+        <v>10.287264942636595</v>
+      </c>
+      <c r="H404">
+        <f t="shared" si="31"/>
+        <v>2.6832815729997481</v>
+      </c>
+    </row>
+    <row r="405" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C405" t="s">
+        <v>276</v>
+      </c>
+      <c r="D405">
+        <f t="shared" ref="D405:D409" si="32">STDEV(D363,D370,D377,D384,D391)</f>
+        <v>0.92664691225946627</v>
+      </c>
+      <c r="E405">
+        <f t="shared" ref="E405:H405" si="33">STDEV(E363,E370,E377,E384,E391)</f>
+        <v>3.3466401061363005</v>
+      </c>
+      <c r="F405">
+        <f t="shared" si="33"/>
+        <v>0.94134717293886883</v>
+      </c>
+      <c r="G405">
+        <f t="shared" si="33"/>
+        <v>5.8584059265298443</v>
+      </c>
+      <c r="H405">
+        <f t="shared" si="33"/>
+        <v>2.2803508501982734</v>
+      </c>
+    </row>
+    <row r="406" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C406" t="s">
+        <v>436</v>
+      </c>
+      <c r="D406">
+        <f t="shared" si="32"/>
+        <v>0.93132604387507867</v>
+      </c>
+      <c r="E406">
+        <f t="shared" ref="E406:H406" si="34">STDEV(E364,E371,E378,E385,E392)</f>
+        <v>6.5726706900619929</v>
+      </c>
+      <c r="F406">
+        <f t="shared" si="34"/>
+        <v>0.89022030981100497</v>
+      </c>
+      <c r="G406">
+        <f t="shared" si="34"/>
+        <v>8.3791121248017681</v>
+      </c>
+      <c r="H406">
+        <f t="shared" si="34"/>
+        <v>3.2863353450309964</v>
+      </c>
+    </row>
+    <row r="407" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C407" t="s">
+        <v>437</v>
+      </c>
+      <c r="D407">
+        <f t="shared" si="32"/>
+        <v>0.4027471911758046</v>
+      </c>
+      <c r="E407">
+        <f t="shared" ref="E407:H407" si="35">STDEV(E365,E372,E379,E386,E393)</f>
+        <v>0.8944271909999143</v>
+      </c>
+      <c r="F407">
+        <f t="shared" si="35"/>
+        <v>0.40411545380002578</v>
+      </c>
+      <c r="G407">
+        <f t="shared" si="35"/>
+        <v>0.21559220765138989</v>
+      </c>
+      <c r="H407">
+        <f t="shared" si="35"/>
+        <v>0.44721359549995715</v>
+      </c>
+    </row>
+    <row r="408" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C408" t="s">
+        <v>438</v>
+      </c>
+      <c r="D408">
+        <f t="shared" si="32"/>
+        <v>0.54811194112151873</v>
+      </c>
+      <c r="E408">
+        <f t="shared" ref="E408:H408" si="36">STDEV(E366,E373,E380,E387,E394)</f>
+        <v>0</v>
+      </c>
+      <c r="F408">
+        <f t="shared" si="36"/>
+        <v>0.54811194112151873</v>
+      </c>
+      <c r="G408">
+        <f t="shared" si="36"/>
+        <v>0.10074720839804939</v>
+      </c>
+      <c r="H408">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C409" t="s">
+        <v>439</v>
+      </c>
+      <c r="D409">
+        <f t="shared" si="32"/>
+        <v>0.54106681657628719</v>
+      </c>
+      <c r="E409">
+        <f t="shared" ref="E409:H409" si="37">STDEV(E367,E374,E381,E388,E395)</f>
+        <v>0</v>
+      </c>
+      <c r="F409">
+        <f t="shared" si="37"/>
+        <v>0.54106681657628874</v>
+      </c>
+      <c r="G409">
+        <f t="shared" si="37"/>
+        <v>0.26185874054535579</v>
+      </c>
+      <c r="H409">
+        <f t="shared" si="37"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8130,7 +9333,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>264</v>
       </c>
       <c r="B2" t="s">
@@ -8154,7 +9357,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="20"/>
       <c r="B3" t="s">
         <v>113</v>
       </c>
@@ -8179,7 +9382,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>114</v>
       </c>
@@ -8204,7 +9407,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
         <v>115</v>
       </c>
@@ -8229,7 +9432,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" t="s">
         <v>116</v>
       </c>
@@ -8254,7 +9457,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" t="s">
         <v>117</v>
       </c>
@@ -8279,7 +9482,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" t="s">
         <v>118</v>
       </c>
@@ -8304,7 +9507,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
         <v>119</v>
       </c>
@@ -8327,7 +9530,7 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
         <v>120</v>
       </c>
@@ -8350,7 +9553,7 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="2" t="s">
         <v>121</v>
       </c>
@@ -8375,7 +9578,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
         <v>122</v>
       </c>
@@ -8398,7 +9601,7 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>123</v>
       </c>
@@ -8421,7 +9624,7 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
         <v>178</v>
       </c>
@@ -8446,7 +9649,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="2" t="s">
         <v>125</v>
       </c>
@@ -8471,7 +9674,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="2" t="s">
         <v>124</v>
       </c>
@@ -8496,7 +9699,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2" t="s">
         <v>128</v>
       </c>
@@ -8518,7 +9721,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2" t="s">
         <v>127</v>
       </c>
@@ -8540,7 +9743,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2" t="s">
         <v>126</v>
       </c>
@@ -8562,7 +9765,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="2" t="s">
         <v>255</v>
       </c>
@@ -8584,7 +9787,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="2" t="s">
         <v>256</v>
       </c>
@@ -8606,7 +9809,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="2" t="s">
         <v>257</v>
       </c>
@@ -8629,7 +9832,7 @@
     </row>
     <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="20" t="s">
         <v>265</v>
       </c>
       <c r="B25" t="s">
@@ -8653,7 +9856,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>173</v>
       </c>
@@ -8678,7 +9881,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="2" t="s">
         <v>174</v>
       </c>
@@ -8700,7 +9903,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+      <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>175</v>
       </c>
@@ -8722,7 +9925,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
+      <c r="A29" s="20"/>
       <c r="B29" t="s">
         <v>176</v>
       </c>
@@ -8744,7 +9947,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
+      <c r="A30" s="20"/>
       <c r="B30" t="s">
         <v>177</v>
       </c>
@@ -8766,7 +9969,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
+      <c r="A31" s="20"/>
       <c r="B31" t="s">
         <v>180</v>
       </c>
@@ -8788,7 +9991,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>181</v>
       </c>
@@ -8810,7 +10013,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>182</v>
       </c>
@@ -8832,7 +10035,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="2" t="s">
         <v>183</v>
       </c>
@@ -8854,7 +10057,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
+      <c r="A35" s="20"/>
       <c r="B35" t="s">
         <v>184</v>
       </c>
@@ -8876,7 +10079,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
+      <c r="A36" s="20"/>
       <c r="B36" t="s">
         <v>185</v>
       </c>
@@ -8898,7 +10101,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
+      <c r="A37" s="20"/>
       <c r="B37" t="s">
         <v>179</v>
       </c>
@@ -8920,7 +10123,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
         <v>186</v>
       </c>
@@ -8942,7 +10145,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="2" t="s">
         <v>187</v>
       </c>
@@ -8964,7 +10167,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="2" t="s">
         <v>188</v>
       </c>
@@ -8986,7 +10189,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="2" t="s">
         <v>189</v>
       </c>
@@ -9008,7 +10211,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="2" t="s">
         <v>190</v>
       </c>
@@ -9030,7 +10233,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="2" t="s">
         <v>258</v>
       </c>
@@ -9052,7 +10255,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="2" t="s">
         <v>259</v>
       </c>
@@ -9074,7 +10277,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="2" t="s">
         <v>260</v>
       </c>
@@ -9097,7 +10300,7 @@
     </row>
     <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="21" t="s">
         <v>266</v>
       </c>
       <c r="B48" t="s">
@@ -9121,7 +10324,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
+      <c r="A49" s="21"/>
       <c r="B49" t="s">
         <v>200</v>
       </c>
@@ -9146,7 +10349,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="2" t="s">
         <v>201</v>
       </c>
@@ -9168,7 +10371,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
+      <c r="A51" s="21"/>
       <c r="B51" t="s">
         <v>192</v>
       </c>
@@ -9190,7 +10393,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
+      <c r="A52" s="21"/>
       <c r="B52" t="s">
         <v>193</v>
       </c>
@@ -9212,7 +10415,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
+      <c r="A53" s="21"/>
       <c r="B53" t="s">
         <v>194</v>
       </c>
@@ -9234,7 +10437,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
+      <c r="A54" s="21"/>
       <c r="B54" t="s">
         <v>202</v>
       </c>
@@ -9256,7 +10459,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
+      <c r="A55" s="21"/>
       <c r="B55" t="s">
         <v>203</v>
       </c>
@@ -9278,7 +10481,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
+      <c r="A56" s="21"/>
       <c r="B56" t="s">
         <v>204</v>
       </c>
@@ -9300,7 +10503,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="2" t="s">
         <v>205</v>
       </c>
@@ -9322,7 +10525,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
+      <c r="A58" s="21"/>
       <c r="B58" t="s">
         <v>206</v>
       </c>
@@ -9344,7 +10547,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
+      <c r="A59" s="21"/>
       <c r="B59" t="s">
         <v>207</v>
       </c>
@@ -9366,7 +10569,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
+      <c r="A60" s="21"/>
       <c r="B60" t="s">
         <v>208</v>
       </c>
@@ -9388,7 +10591,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="2" t="s">
         <v>195</v>
       </c>
@@ -9410,7 +10613,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="2" t="s">
         <v>196</v>
       </c>
@@ -9432,7 +10635,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="2" t="s">
         <v>198</v>
       </c>
@@ -9454,7 +10657,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="2" t="s">
         <v>197</v>
       </c>
@@ -9476,7 +10679,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="2" t="s">
         <v>199</v>
       </c>
@@ -9498,7 +10701,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="2" t="s">
         <v>252</v>
       </c>
@@ -9520,7 +10723,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="2" t="s">
         <v>253</v>
       </c>
@@ -9542,7 +10745,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="2" t="s">
         <v>254</v>
       </c>
@@ -9565,7 +10768,7 @@
     </row>
     <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B71" t="s">
@@ -9589,7 +10792,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
+      <c r="A72" s="21"/>
       <c r="B72" t="s">
         <v>215</v>
       </c>
@@ -9614,7 +10817,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="2" t="s">
         <v>216</v>
       </c>
@@ -9636,7 +10839,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
+      <c r="A74" s="21"/>
       <c r="B74" t="s">
         <v>212</v>
       </c>
@@ -9658,7 +10861,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
+      <c r="A75" s="21"/>
       <c r="B75" t="s">
         <v>213</v>
       </c>
@@ -9680,7 +10883,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="18"/>
+      <c r="A76" s="21"/>
       <c r="B76" t="s">
         <v>214</v>
       </c>
@@ -9702,7 +10905,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
+      <c r="A77" s="21"/>
       <c r="B77" t="s">
         <v>217</v>
       </c>
@@ -9724,7 +10927,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
+      <c r="A78" s="21"/>
       <c r="B78" t="s">
         <v>218</v>
       </c>
@@ -9746,7 +10949,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
+      <c r="A79" s="21"/>
       <c r="B79" t="s">
         <v>219</v>
       </c>
@@ -9768,7 +10971,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="2" t="s">
         <v>220</v>
       </c>
@@ -9790,7 +10993,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
+      <c r="A81" s="21"/>
       <c r="B81" t="s">
         <v>221</v>
       </c>
@@ -9812,7 +11015,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
+      <c r="A82" s="21"/>
       <c r="B82" t="s">
         <v>222</v>
       </c>
@@ -9834,7 +11037,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
+      <c r="A83" s="21"/>
       <c r="B83" t="s">
         <v>223</v>
       </c>
@@ -9856,7 +11059,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="2" t="s">
         <v>209</v>
       </c>
@@ -9878,7 +11081,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="2" t="s">
         <v>210</v>
       </c>
@@ -9900,7 +11103,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
+      <c r="A86" s="21"/>
       <c r="B86" s="2" t="s">
         <v>225</v>
       </c>
@@ -9922,7 +11125,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" s="18"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="2" t="s">
         <v>224</v>
       </c>
@@ -9944,7 +11147,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="2" t="s">
         <v>226</v>
       </c>
@@ -9966,7 +11169,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="2" t="s">
         <v>261</v>
       </c>
@@ -9988,7 +11191,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="2" t="s">
         <v>262</v>
       </c>
@@ -10010,7 +11213,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="2" t="s">
         <v>263</v>
       </c>
@@ -11636,10 +12839,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
-  <dimension ref="B1:I105"/>
+  <dimension ref="B1:I122"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105:H105"/>
+    <sheetView tabSelected="1" topLeftCell="B104" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12436,7 +13639,7 @@
         <v>278</v>
       </c>
       <c r="D33" s="9">
-        <v>0.70599999999999996</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E33">
         <v>8</v>
@@ -12446,7 +13649,7 @@
       </c>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>0.71399999999999997</v>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="H33" s="9">
         <v>0.01</v>
@@ -13784,7 +14987,7 @@
         <v>9.0500000000000007</v>
       </c>
     </row>
-    <row r="97" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B97" s="2" t="s">
         <v>402</v>
       </c>
@@ -13808,7 +15011,7 @@
         <v>59.21</v>
       </c>
     </row>
-    <row r="98" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
         <v>403</v>
       </c>
@@ -13832,7 +15035,7 @@
         <v>39.78</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B99" s="2" t="s">
         <v>404</v>
       </c>
@@ -13856,7 +15059,7 @@
         <v>46.26</v>
       </c>
     </row>
-    <row r="100" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B100" s="2" t="s">
         <v>405</v>
       </c>
@@ -13880,7 +15083,7 @@
         <v>74.88</v>
       </c>
     </row>
-    <row r="101" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B101" s="2" t="s">
         <v>406</v>
       </c>
@@ -13904,7 +15107,7 @@
         <v>20.02</v>
       </c>
     </row>
-    <row r="102" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>412</v>
       </c>
@@ -13928,7 +15131,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="103" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>413</v>
       </c>
@@ -13952,7 +15155,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="104" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>414</v>
       </c>
@@ -13976,7 +15179,7 @@
         <v>12.47</v>
       </c>
     </row>
-    <row r="105" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>415</v>
       </c>
@@ -13984,7 +15187,7 @@
         <v>278</v>
       </c>
       <c r="D105" s="9">
-        <v>0.46200000000000002</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="E105">
         <v>64</v>
@@ -13994,10 +15197,184 @@
       </c>
       <c r="G105" s="1">
         <f t="shared" si="2"/>
-        <v>0.52600000000000002</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="H105" s="9">
-        <v>16.89</v>
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
+        <v>440</v>
+      </c>
+      <c r="D110" s="8">
+        <v>5.7800000000000001E-7</v>
+      </c>
+      <c r="E110">
+        <v>20</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110" s="9">
+        <f>D110+E110*0.001</f>
+        <v>2.0000578000000001E-2</v>
+      </c>
+      <c r="H110">
+        <v>0.72</v>
+      </c>
+      <c r="I110">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
+        <v>276</v>
+      </c>
+      <c r="D111" s="8">
+        <v>1.4000000000000001E-7</v>
+      </c>
+      <c r="E111">
+        <v>8</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111" s="9">
+        <f t="shared" ref="G111:G115" si="4">D111+E111*0.001</f>
+        <v>8.0001399999999993E-3</v>
+      </c>
+      <c r="H111">
+        <v>0.16</v>
+      </c>
+      <c r="I111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C112" t="s">
+        <v>436</v>
+      </c>
+      <c r="D112">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E112">
+        <v>16</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112" s="9">
+        <f t="shared" si="4"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H112">
+        <v>0.17</v>
+      </c>
+      <c r="I112">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
+        <v>441</v>
+      </c>
+      <c r="D113">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E113">
+        <v>14</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113" s="9">
+        <f t="shared" si="4"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H113">
+        <v>0.26</v>
+      </c>
+      <c r="I113">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C114" t="s">
+        <v>438</v>
+      </c>
+      <c r="D114">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E114">
+        <v>6</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114" s="9">
+        <f t="shared" si="4"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H114">
+        <v>0.06</v>
+      </c>
+      <c r="I114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
+        <v>439</v>
+      </c>
+      <c r="D115">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E115">
+        <v>8</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115" s="9">
+        <f t="shared" si="4"/>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="H115">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I115">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="118" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="120" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C120" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="121" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="122" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CPU/Iterations-problem scale figures
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8917BD-F8F9-C445-AA13-D91015769277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CCE4F-8B82-5246-AD20-4823A5E12787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="28800" windowHeight="15800" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="35200" yWindow="900" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="546">
   <si>
     <t>Name</t>
   </si>
@@ -1692,6 +1693,27 @@
   </si>
   <si>
     <t>ADMM+STGMT</t>
+  </si>
+  <si>
+    <t>pGRPAE+MT</t>
+  </si>
+  <si>
+    <t>pGRAPE+MS</t>
+  </si>
+  <si>
+    <t>TR+MT</t>
+  </si>
+  <si>
+    <t>TR+MS</t>
+  </si>
+  <si>
+    <t>ADMM+MT</t>
+  </si>
+  <si>
+    <t>ADMM+MS</t>
+  </si>
+  <si>
+    <t>Root relaxation, IP, LP, gap</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:Q770"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B158" workbookViewId="0">
+    <sheetView topLeftCell="B158" workbookViewId="0">
       <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
@@ -17564,6 +17586,547 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE872A85-4DE9-F745-9374-575870CFA036}">
+  <dimension ref="A1:Y10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="B1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F1" t="s">
+        <v>540</v>
+      </c>
+      <c r="J1" t="s">
+        <v>541</v>
+      </c>
+      <c r="N1" t="s">
+        <v>542</v>
+      </c>
+      <c r="R1" t="s">
+        <v>543</v>
+      </c>
+      <c r="V1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.24188419999999999</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.24188416159439999</v>
+      </c>
+      <c r="D2" s="8">
+        <v>6.8181818180000006E-2</v>
+      </c>
+      <c r="E2" s="8">
+        <f>(C2-D2)/C2</f>
+        <v>0.71812202282872206</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2.430428520409E-2</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <f>(G2-H2)/G2</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.46668749999999998</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.48902466287239998</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.46668749209999999</v>
+      </c>
+      <c r="M2" s="8">
+        <f>(K2-L2)/K2</f>
+        <v>4.5676982099834049E-2</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0.46668749999999998</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.48902466287239998</v>
+      </c>
+      <c r="P2" s="8">
+        <v>0.46668749209999999</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>(O2-P2)/O2</f>
+        <v>4.5676982099834049E-2</v>
+      </c>
+      <c r="R2" s="8">
+        <v>0.23373150000000001</v>
+      </c>
+      <c r="S2" s="8">
+        <v>0.23373153902810001</v>
+      </c>
+      <c r="T2" s="8">
+        <v>5.788940435E-2</v>
+      </c>
+      <c r="U2" s="8">
+        <f>(S2-T2)/S2</f>
+        <v>0.75232523351056901</v>
+      </c>
+      <c r="V2" s="8">
+        <v>1.550431E-2</v>
+      </c>
+      <c r="W2" s="8">
+        <v>2.4750957841570002E-2</v>
+      </c>
+      <c r="X2" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>(W2-X2)/W2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>518</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.1401789</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.150339327813</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5.1496119129999997E-2</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E7" si="0">(C3-D3)/C3</f>
+        <v>0.65746741136122688</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.8934099999999999E-2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>6.0051314675590002E-2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" ref="I3:I7" si="1">(G3-H3)/G3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.1470931</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.161856852789</v>
+      </c>
+      <c r="L3" s="8">
+        <v>6.0145330349999998E-2</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M7" si="2">(K3-L3)/K3</f>
+        <v>0.62840417743444743</v>
+      </c>
+      <c r="N3" s="8">
+        <v>1.9132980000000001E-2</v>
+      </c>
+      <c r="O3" s="8">
+        <v>7.3222690283929998E-2</v>
+      </c>
+      <c r="P3" s="8">
+        <v>4.1661404980000002E-3</v>
+      </c>
+      <c r="Q3" s="8">
+        <f t="shared" ref="Q3:Q7" si="3">(O3-P3)/O3</f>
+        <v>0.94310314901234471</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0.13594419999999999</v>
+      </c>
+      <c r="S3" s="8">
+        <v>0.15169893830379999</v>
+      </c>
+      <c r="T3" s="8">
+        <v>4.5919320850000001E-2</v>
+      </c>
+      <c r="U3" s="8">
+        <f t="shared" ref="U3:U7" si="4">(S3-T3)/S3</f>
+        <v>0.6972996557296951</v>
+      </c>
+      <c r="V3" s="8">
+        <v>2.4577870000000002E-2</v>
+      </c>
+      <c r="W3" s="8">
+        <v>6.033009478806E-2</v>
+      </c>
+      <c r="X3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="8">
+        <f t="shared" ref="Y3:Y7" si="5">(W3-X3)/W3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.14010049999999999</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.21236115600809999</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1.8942617209999998E-2</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.91079999013907487</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2.05579E-2</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.1716302489722</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.14588110000000001</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.20572817840089999</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.878555153E-2</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" si="2"/>
+        <v>0.90868751341688925</v>
+      </c>
+      <c r="N4" s="8">
+        <v>2.3683800000000001E-2</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0.1590419513976</v>
+      </c>
+      <c r="P4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.10539569999999999</v>
+      </c>
+      <c r="S4" s="8">
+        <v>0.2003655848376</v>
+      </c>
+      <c r="T4" s="8">
+        <v>1.4713807230000001E-2</v>
+      </c>
+      <c r="U4" s="8">
+        <f t="shared" si="4"/>
+        <v>0.92656519710245733</v>
+      </c>
+      <c r="V4" s="8">
+        <v>2.3311709999999999E-2</v>
+      </c>
+      <c r="W4" s="8">
+        <v>0.12831494594660001</v>
+      </c>
+      <c r="X4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>520</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.12637470000000001</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.18079961653000001</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2.6135558069999999E-2</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.85544461558266993</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2.109801E-2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.32201949271769997</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.11582770000000001</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.18358220638780001</v>
+      </c>
+      <c r="L5" s="8">
+        <v>2.0650868879999999E-2</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="2"/>
+        <v>0.8875115988290444</v>
+      </c>
+      <c r="N5" s="8">
+        <v>2.479286E-2</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.2679285668459</v>
+      </c>
+      <c r="P5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R5" s="8">
+        <v>2.492221E-2</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0.2056017509561</v>
+      </c>
+      <c r="T5" s="8">
+        <v>2.7707433000000001E-3</v>
+      </c>
+      <c r="U5" s="8">
+        <f t="shared" si="4"/>
+        <v>0.98652373684992789</v>
+      </c>
+      <c r="V5" s="8">
+        <v>2.479286E-2</v>
+      </c>
+      <c r="W5" s="8">
+        <v>0.2679285668459</v>
+      </c>
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.1754299</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.17542990905459999</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4.35449142E-2</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.75178169768960379</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2.246223E-2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3.8006175272120003E-2</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.17443600000000001</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.1744360232671</v>
+      </c>
+      <c r="L6" s="8">
+        <v>4.1238028650000001E-2</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="2"/>
+        <v>0.76359224500976219</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2.4639029999999999E-2</v>
+      </c>
+      <c r="O6" s="8">
+        <v>3.206316663264E-2</v>
+      </c>
+      <c r="P6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R6" s="8">
+        <v>8.3261940000000007E-2</v>
+      </c>
+      <c r="S6" s="8">
+        <v>0.20879240267079999</v>
+      </c>
+      <c r="T6" s="8">
+        <v>6.016928554E-6</v>
+      </c>
+      <c r="U6" s="8">
+        <f t="shared" si="4"/>
+        <v>0.99997118224381232</v>
+      </c>
+      <c r="V6" s="8">
+        <v>2.4965480000000002E-2</v>
+      </c>
+      <c r="W6" s="8">
+        <v>8.3253018705480006E-2</v>
+      </c>
+      <c r="X6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.22373599999999999</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.25376387545930001</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3.3256842449999997E-2</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.86894571818070343</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4.8890919999999997E-2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.1199351176453</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.22373599999999999</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.27055884505689998</v>
+      </c>
+      <c r="L7" s="8">
+        <v>3.3256842449999997E-2</v>
+      </c>
+      <c r="M7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.87708092691256911</v>
+      </c>
+      <c r="N7" s="8">
+        <v>4.8813080000000002E-2</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.13277450015559999</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0.1214258</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0.2426227125124</v>
+      </c>
+      <c r="T7" s="8">
+        <v>1.324438497E-6</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" si="4"/>
+        <v>0.99999454116029252</v>
+      </c>
+      <c r="V7" s="8">
+        <v>4.9806219999999998E-2</v>
+      </c>
+      <c r="W7" s="8">
+        <v>0.16415733146719999</v>
+      </c>
+      <c r="X7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741D4DFB-7C75-0E41-A642-F95FBB75CB0A}">
   <dimension ref="A1:L109"/>
   <sheetViews>
@@ -20213,7 +20776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA6C1F7-3E09-4E4E-BA36-8FCB329B50FE}">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -20566,7 +21129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5EC59C-826A-9946-B4D2-773A781998E3}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -20794,7 +21357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C1058-6CFA-6948-AB8A-BD491AFAAAD5}">
   <dimension ref="A1:N91"/>
   <sheetViews>
@@ -23584,7 +24147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0842C86B-7D36-B04D-B09B-8D3C95D38C2E}">
   <dimension ref="B1:L70"/>
   <sheetViews>
@@ -25272,7 +25835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
   <dimension ref="B1:N159"/>
   <sheetViews>
@@ -29250,7 +29813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B1B372-4CC2-8848-A040-A5C43187FDD8}">
   <dimension ref="A1:C10"/>
   <sheetViews>

</xml_diff>

<commit_message>
update results and readme file, add citation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyuf/Documents/Michigan/phd_topic/qc_opt/Quantum-Control-qutip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846CCE4F-8B82-5246-AD20-4823A5E12787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7AA7E7-93E6-354E-9BFD-CB0B0702352D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="900" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="9" xr2:uid="{393AB6DC-0C1A-A74B-BEEF-2523904083F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId8"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId9"/>
+    <sheet name="NOT" sheetId="10" r:id="rId10"/>
+    <sheet name="NOT-new" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="553">
   <si>
     <t>Name</t>
   </si>
@@ -1714,6 +1716,27 @@
   </si>
   <si>
     <t>Root relaxation, IP, LP, gap</t>
+  </si>
+  <si>
+    <t>pGRAPE</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>pGRAPE+SUR</t>
+  </si>
+  <si>
+    <t>TR+SUR</t>
+  </si>
+  <si>
+    <t>pGRAPE+MT</t>
+  </si>
+  <si>
+    <t>pGRAPE+SUR+ALB</t>
+  </si>
+  <si>
+    <t>TR+SUR+ALB</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1749,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1780,6 +1803,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6897BB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1838,7 +1867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1888,6 +1917,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2205,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB70BE8-B604-B445-AA09-F9BD1573AC49}">
   <dimension ref="A1:Q770"/>
   <sheetViews>
-    <sheetView topLeftCell="B158" workbookViewId="0">
-      <selection activeCell="E177" sqref="E177"/>
+    <sheetView topLeftCell="A756" workbookViewId="0">
+      <selection activeCell="G162" sqref="G162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6099,6 +6130,10 @@
         <f>D163/D187</f>
         <v>0.84172090808064759</v>
       </c>
+      <c r="J163">
+        <f>1-I162</f>
+        <v>0.15462771868550562</v>
+      </c>
     </row>
     <row r="164" spans="3:10" ht="17">
       <c r="C164" s="2" t="s">
@@ -9853,6 +9888,10 @@
       <c r="G325">
         <v>1.32</v>
       </c>
+      <c r="I325">
+        <f>1-D325/D332</f>
+        <v>0.371</v>
+      </c>
     </row>
     <row r="326" spans="3:9" ht="17">
       <c r="C326" s="2" t="s">
@@ -17580,6 +17619,3038 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F960E117-0067-9F40-978D-4F06FC858D5C}">
+  <dimension ref="A1:S36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>546</v>
+      </c>
+      <c r="L1" t="s">
+        <v>547</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1">
+        <v>0.1627915417861</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.163004864866027</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.163397238895157</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.22647190568743</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.1875279744466101</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.90802992516876502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="8">
+        <v>4.2777181796793601E-10</v>
+      </c>
+      <c r="B3" s="8">
+        <v>6.5489364865944894E-5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.0668355438247999E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3.2510050806212401</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.65236551144146704</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.57809733973746502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="8">
+        <v>6.5504712765118698E-11</v>
+      </c>
+      <c r="B4" s="8">
+        <v>5.138848784203E-5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4.7887368864185599E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.7395401577687202</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.53025580755296</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.0051845518137399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>550</v>
+      </c>
+      <c r="E6" t="s">
+        <v>541</v>
+      </c>
+      <c r="F6" t="s">
+        <v>543</v>
+      </c>
+      <c r="G6" t="s">
+        <v>540</v>
+      </c>
+      <c r="H6" t="s">
+        <v>542</v>
+      </c>
+      <c r="I6" t="s">
+        <v>544</v>
+      </c>
+      <c r="K6" t="s">
+        <v>548</v>
+      </c>
+      <c r="L6" t="s">
+        <v>549</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>550</v>
+      </c>
+      <c r="O6" t="s">
+        <v>541</v>
+      </c>
+      <c r="P6" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>540</v>
+      </c>
+      <c r="R6" t="s">
+        <v>542</v>
+      </c>
+      <c r="S6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1">
+        <v>0.16433567494509899</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="K7" s="35">
+        <v>3</v>
+      </c>
+      <c r="L7" s="35">
+        <v>1</v>
+      </c>
+      <c r="M7" s="35">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="8">
+        <v>2.3757225945439898E-3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3.0976997160051499E-3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.5480209484370899E-3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.32271951015683E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.8306499557828602E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.7412570846754201E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <v>6.8071527126928502E-2</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.20404667937588E-2</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.9302345445700999E-2</v>
+      </c>
+      <c r="K8" s="35">
+        <v>40</v>
+      </c>
+      <c r="L8" s="35">
+        <v>46</v>
+      </c>
+      <c r="M8" s="35">
+        <v>52</v>
+      </c>
+      <c r="N8">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>23</v>
+      </c>
+      <c r="P8">
+        <v>26</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="8">
+        <v>4.7331475979300796E-3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3.9061170530529899E-4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>9.2249337445582304E-3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.15129113675343001</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.163455337405219</v>
+      </c>
+      <c r="F9" s="8">
+        <v>9.3943820904024405E-3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.109886658558011</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.102341799900144</v>
+      </c>
+      <c r="I9" s="8">
+        <v>5.07975385197068E-3</v>
+      </c>
+      <c r="K9" s="35">
+        <v>126</v>
+      </c>
+      <c r="L9" s="35">
+        <v>126</v>
+      </c>
+      <c r="M9" s="35">
+        <v>21</v>
+      </c>
+      <c r="N9">
+        <v>62</v>
+      </c>
+      <c r="O9">
+        <v>60</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>19</v>
+      </c>
+      <c r="R9">
+        <v>20</v>
+      </c>
+      <c r="S9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B11" t="s">
+        <v>552</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>550</v>
+      </c>
+      <c r="E11" t="s">
+        <v>541</v>
+      </c>
+      <c r="F11" t="s">
+        <v>543</v>
+      </c>
+      <c r="G11" t="s">
+        <v>540</v>
+      </c>
+      <c r="H11" t="s">
+        <v>542</v>
+      </c>
+      <c r="I11" t="s">
+        <v>544</v>
+      </c>
+      <c r="K11" t="s">
+        <v>551</v>
+      </c>
+      <c r="L11" t="s">
+        <v>552</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" t="s">
+        <v>550</v>
+      </c>
+      <c r="O11" t="s">
+        <v>541</v>
+      </c>
+      <c r="P11" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>540</v>
+      </c>
+      <c r="R11" t="s">
+        <v>542</v>
+      </c>
+      <c r="S11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="K12" s="35">
+        <v>1</v>
+      </c>
+      <c r="L12" s="35">
+        <v>1</v>
+      </c>
+      <c r="M12" s="35">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="8">
+        <v>1.4197286180969099E-3</v>
+      </c>
+      <c r="B13" s="8">
+        <v>7.3287569574531598E-4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>7.2370991824921495E-4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>9.5783468942822704E-4</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8.4021001032963296E-4</v>
+      </c>
+      <c r="F13" s="8">
+        <v>7.8802477326822497E-4</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1.7878595396783E-3</v>
+      </c>
+      <c r="H13" s="8">
+        <v>5.5138462056070203E-4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.2563070577620199E-3</v>
+      </c>
+      <c r="K13" s="35">
+        <v>6</v>
+      </c>
+      <c r="L13" s="35">
+        <v>6</v>
+      </c>
+      <c r="M13" s="35">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>19</v>
+      </c>
+      <c r="O13">
+        <v>23</v>
+      </c>
+      <c r="P13">
+        <v>26</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="S13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="8">
+        <v>5.5032683831412999E-4</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1.65868576629446E-3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6.1599207400919698E-4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.2237493045387201E-3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1.03518773611466E-3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>9.8219722142567291E-4</v>
+      </c>
+      <c r="G14" s="8">
+        <v>5.4321302183346599E-4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>9.9085545725019399E-4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>9.0459487803606897E-4</v>
+      </c>
+      <c r="K14" s="35">
+        <v>32</v>
+      </c>
+      <c r="L14" s="35">
+        <v>10</v>
+      </c>
+      <c r="M14" s="35">
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>57</v>
+      </c>
+      <c r="O14">
+        <v>54</v>
+      </c>
+      <c r="P14">
+        <v>14</v>
+      </c>
+      <c r="Q14">
+        <v>20</v>
+      </c>
+      <c r="R14">
+        <v>20</v>
+      </c>
+      <c r="S14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="25">
+        <f>(A7-A12)/A7</f>
+        <v>4.5632663669316334E-3</v>
+      </c>
+      <c r="B15" s="25">
+        <f t="shared" ref="B15:I15" si="0">(B7-B12)/B7</f>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="C15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="D15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="E15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="G15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="H15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="I15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="K15" s="25">
+        <f>(K7-K12)/K7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L15" s="25">
+        <f t="shared" ref="L15:S15" si="1">(L7-L12)/L7</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="25">
+        <f t="shared" ref="A16:I16" si="2">(A8-A13)/A8</f>
+        <v>0.40240134881176187</v>
+      </c>
+      <c r="B16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.76341293122806431</v>
+      </c>
+      <c r="C16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.53249345948458537</v>
+      </c>
+      <c r="D16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.77841849623190651</v>
+      </c>
+      <c r="E16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.78066124025213324</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.54743915748941974</v>
+      </c>
+      <c r="G16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.97373557469418015</v>
+      </c>
+      <c r="H16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.95420571062522985</v>
+      </c>
+      <c r="I16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.93491427965082752</v>
+      </c>
+      <c r="K16" s="25">
+        <f t="shared" ref="K16:S16" si="3">(K8-K13)/K8</f>
+        <v>0.85</v>
+      </c>
+      <c r="L16" s="25">
+        <f t="shared" si="3"/>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="M16" s="25">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="N16" s="25">
+        <f t="shared" si="3"/>
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="O16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.375</v>
+      </c>
+      <c r="R16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="S16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="25">
+        <f t="shared" ref="A17:I17" si="4">(A9-A14)/A9</f>
+        <v>0.88372920410198041</v>
+      </c>
+      <c r="B17" s="25">
+        <f>(B9-B14)/B14</f>
+        <v>-0.76450530097817493</v>
+      </c>
+      <c r="C17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.93322531184870894</v>
+      </c>
+      <c r="D17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.99191129546119305</v>
+      </c>
+      <c r="E17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.99366684653711645</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.89544844866070405</v>
+      </c>
+      <c r="G17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.99505660624354419</v>
+      </c>
+      <c r="H17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.99031817440950831</v>
+      </c>
+      <c r="I17" s="25">
+        <f t="shared" si="4"/>
+        <v>0.82192151344397657</v>
+      </c>
+      <c r="K17" s="25">
+        <f t="shared" ref="K17:S17" si="5">(K9-K14)/K9</f>
+        <v>0.74603174603174605</v>
+      </c>
+      <c r="L17" s="25">
+        <f t="shared" si="5"/>
+        <v>0.92063492063492058</v>
+      </c>
+      <c r="M17" s="25">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N17" s="25">
+        <f t="shared" si="5"/>
+        <v>8.0645161290322578E-2</v>
+      </c>
+      <c r="O17" s="25">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="P17" s="25">
+        <f t="shared" si="5"/>
+        <v>-0.4</v>
+      </c>
+      <c r="Q17" s="25">
+        <f t="shared" si="5"/>
+        <v>-5.2631578947368418E-2</v>
+      </c>
+      <c r="R17" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>546</v>
+      </c>
+      <c r="B20" t="s">
+        <v>547</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>546</v>
+      </c>
+      <c r="L20" t="s">
+        <v>547</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="1">
+        <v>0.1627915417861</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.163004864866027</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.163397238895157</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2.22647190568743</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1.1875279744466101</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.90802992516876502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="8">
+        <v>4.2777181796793601E-10</v>
+      </c>
+      <c r="B22" s="8">
+        <v>6.5489364865944894E-5</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1.0668355438247999E-4</v>
+      </c>
+      <c r="K22" s="1">
+        <v>3.2510050806212401</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.65236551144146704</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.57809733973746502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="8">
+        <v>6.5504712765118698E-11</v>
+      </c>
+      <c r="B23" s="8">
+        <v>5.138848784203E-5</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.7887368864185599E-5</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2.7395401577687202</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1.53025580755296</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1.0051845518137399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>548</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>550</v>
+      </c>
+      <c r="E25" t="s">
+        <v>541</v>
+      </c>
+      <c r="F25" t="s">
+        <v>543</v>
+      </c>
+      <c r="G25" t="s">
+        <v>540</v>
+      </c>
+      <c r="H25" t="s">
+        <v>542</v>
+      </c>
+      <c r="I25" t="s">
+        <v>544</v>
+      </c>
+      <c r="K25" t="s">
+        <v>548</v>
+      </c>
+      <c r="L25" t="s">
+        <v>549</v>
+      </c>
+      <c r="M25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N25" t="s">
+        <v>550</v>
+      </c>
+      <c r="O25" t="s">
+        <v>541</v>
+      </c>
+      <c r="P25" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>540</v>
+      </c>
+      <c r="R25" t="s">
+        <v>542</v>
+      </c>
+      <c r="S25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="1">
+        <v>0.16433567494509899</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.16433567494509899</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="K26" s="35">
+        <v>3</v>
+      </c>
+      <c r="L26" s="35">
+        <v>1</v>
+      </c>
+      <c r="M26" s="35">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>3</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="8">
+        <v>2.3757225945439898E-3</v>
+      </c>
+      <c r="B27" s="8">
+        <v>3.0976997160051499E-3</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.5480209484370899E-3</v>
+      </c>
+      <c r="D27" s="8">
+        <v>4.0541169326405203E-2</v>
+      </c>
+      <c r="E27" s="8">
+        <v>3.64952930012582E-2</v>
+      </c>
+      <c r="F27" s="8">
+        <v>7.5639736076547504E-2</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1.37921697000562E-2</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0.157913865967091</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.15372727824114801</v>
+      </c>
+      <c r="K27" s="35">
+        <v>40</v>
+      </c>
+      <c r="L27" s="35">
+        <v>46</v>
+      </c>
+      <c r="M27" s="35">
+        <v>52</v>
+      </c>
+      <c r="N27">
+        <v>8</v>
+      </c>
+      <c r="O27">
+        <v>9</v>
+      </c>
+      <c r="P27">
+        <v>10</v>
+      </c>
+      <c r="Q27">
+        <v>19</v>
+      </c>
+      <c r="R27">
+        <v>14</v>
+      </c>
+      <c r="S27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="8">
+        <v>4.7331475979300796E-3</v>
+      </c>
+      <c r="B28" s="8">
+        <v>3.9061170530529899E-4</v>
+      </c>
+      <c r="C28" s="8">
+        <v>9.2249337445582304E-3</v>
+      </c>
+      <c r="D28" s="8">
+        <v>2.78249395116992E-2</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.13362841537704501</v>
+      </c>
+      <c r="F28" s="8">
+        <v>6.3799358138828796E-2</v>
+      </c>
+      <c r="G28" s="8">
+        <v>6.1584116344166002E-2</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.28429134467709499</v>
+      </c>
+      <c r="I28" s="8">
+        <v>9.2249337445582304E-3</v>
+      </c>
+      <c r="K28" s="35">
+        <v>126</v>
+      </c>
+      <c r="L28" s="35">
+        <v>126</v>
+      </c>
+      <c r="M28" s="35">
+        <v>21</v>
+      </c>
+      <c r="N28">
+        <v>24</v>
+      </c>
+      <c r="O28">
+        <v>25</v>
+      </c>
+      <c r="P28">
+        <v>6</v>
+      </c>
+      <c r="Q28">
+        <v>40</v>
+      </c>
+      <c r="R28">
+        <v>40</v>
+      </c>
+      <c r="S28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>551</v>
+      </c>
+      <c r="B30" t="s">
+        <v>552</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>550</v>
+      </c>
+      <c r="E30" t="s">
+        <v>541</v>
+      </c>
+      <c r="F30" t="s">
+        <v>543</v>
+      </c>
+      <c r="G30" t="s">
+        <v>540</v>
+      </c>
+      <c r="H30" t="s">
+        <v>542</v>
+      </c>
+      <c r="I30" t="s">
+        <v>544</v>
+      </c>
+      <c r="K30" t="s">
+        <v>551</v>
+      </c>
+      <c r="L30" t="s">
+        <v>552</v>
+      </c>
+      <c r="M30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" t="s">
+        <v>550</v>
+      </c>
+      <c r="O30" t="s">
+        <v>541</v>
+      </c>
+      <c r="P30" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>540</v>
+      </c>
+      <c r="R30" t="s">
+        <v>542</v>
+      </c>
+      <c r="S30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.16332089384798201</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.16332089384798201</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.16332089384798201</v>
+      </c>
+      <c r="K31" s="35">
+        <v>1</v>
+      </c>
+      <c r="L31" s="35">
+        <v>1</v>
+      </c>
+      <c r="M31" s="35">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31">
+        <v>3</v>
+      </c>
+      <c r="S31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="8">
+        <v>1.4197286180969099E-3</v>
+      </c>
+      <c r="B32" s="8">
+        <v>7.3287569574531598E-4</v>
+      </c>
+      <c r="C32" s="8">
+        <v>7.2370991824921495E-4</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1.45487745103001E-3</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1.26964341440075E-2</v>
+      </c>
+      <c r="F32" s="8">
+        <v>3.38975597917934E-3</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1.0580051379641599E-3</v>
+      </c>
+      <c r="H32" s="8">
+        <v>8.9040596257472504E-4</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1.7390531314218599E-3</v>
+      </c>
+      <c r="K32" s="35">
+        <v>6</v>
+      </c>
+      <c r="L32" s="35">
+        <v>10</v>
+      </c>
+      <c r="M32" s="35">
+        <v>13</v>
+      </c>
+      <c r="N32">
+        <v>9</v>
+      </c>
+      <c r="O32">
+        <v>11</v>
+      </c>
+      <c r="P32">
+        <v>12</v>
+      </c>
+      <c r="Q32">
+        <v>22</v>
+      </c>
+      <c r="R32">
+        <v>18</v>
+      </c>
+      <c r="S32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="8">
+        <v>5.5032683831412999E-4</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1.65868576629446E-3</v>
+      </c>
+      <c r="C33" s="8">
+        <v>6.1599207400919698E-4</v>
+      </c>
+      <c r="D33" s="8">
+        <v>7.3686880993517601E-4</v>
+      </c>
+      <c r="E33" s="8">
+        <v>9.0865804021844599E-4</v>
+      </c>
+      <c r="F33" s="8">
+        <v>8.9017992988627004E-4</v>
+      </c>
+      <c r="G33" s="8">
+        <v>5.44075382333031E-4</v>
+      </c>
+      <c r="H33" s="8">
+        <v>7.5665498239863005E-4</v>
+      </c>
+      <c r="I33" s="8">
+        <v>8.9017992988627004E-4</v>
+      </c>
+      <c r="K33" s="35">
+        <v>32</v>
+      </c>
+      <c r="L33" s="35">
+        <v>6</v>
+      </c>
+      <c r="M33" s="35">
+        <v>7</v>
+      </c>
+      <c r="N33">
+        <v>24</v>
+      </c>
+      <c r="O33">
+        <v>20</v>
+      </c>
+      <c r="P33">
+        <v>8</v>
+      </c>
+      <c r="Q33">
+        <v>38</v>
+      </c>
+      <c r="R33">
+        <v>39</v>
+      </c>
+      <c r="S33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="25">
+        <f>(A26-A31)/A26</f>
+        <v>4.5632663669316334E-3</v>
+      </c>
+      <c r="B34" s="25">
+        <f t="shared" ref="B34:I34" si="6">(B26-B31)/B26</f>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="C34" s="25">
+        <f t="shared" si="6"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="D34" s="25">
+        <f t="shared" si="6"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="E34" s="25">
+        <f t="shared" si="6"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="F34" s="25">
+        <f t="shared" si="6"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="G34" s="25">
+        <f t="shared" si="6"/>
+        <v>6.1750505327342348E-3</v>
+      </c>
+      <c r="H34" s="25">
+        <f t="shared" si="6"/>
+        <v>5.2245649758014033E-3</v>
+      </c>
+      <c r="I34" s="25">
+        <f t="shared" si="6"/>
+        <v>5.2245649758014033E-3</v>
+      </c>
+      <c r="K34" s="25">
+        <f>(K26-K31)/K26</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L34" s="25">
+        <f t="shared" ref="L34:S34" si="7">(L26-L31)/L26</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="25">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="S34" s="25">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="25">
+        <f t="shared" ref="A35:I35" si="8">(A27-A32)/A27</f>
+        <v>0.40240134881176187</v>
+      </c>
+      <c r="B35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.76341293122806431</v>
+      </c>
+      <c r="C35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.53249345948458537</v>
+      </c>
+      <c r="D35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.96411357947481735</v>
+      </c>
+      <c r="E35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.65210762539788947</v>
+      </c>
+      <c r="F35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.95518551286655862</v>
+      </c>
+      <c r="G35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.92328943444193201</v>
+      </c>
+      <c r="H35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.99436144535426496</v>
+      </c>
+      <c r="I35" s="25">
+        <f t="shared" si="8"/>
+        <v>0.98868741350709499</v>
+      </c>
+      <c r="K35" s="25">
+        <f t="shared" ref="K35:S35" si="9">(K27-K32)/K27</f>
+        <v>0.85</v>
+      </c>
+      <c r="L35" s="25">
+        <f t="shared" si="9"/>
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="M35" s="25">
+        <f t="shared" si="9"/>
+        <v>0.75</v>
+      </c>
+      <c r="N35" s="25">
+        <f t="shared" si="9"/>
+        <v>-0.125</v>
+      </c>
+      <c r="O35" s="25">
+        <f t="shared" si="9"/>
+        <v>-0.22222222222222221</v>
+      </c>
+      <c r="P35" s="25">
+        <f>(P27-P32)/P27</f>
+        <v>-0.2</v>
+      </c>
+      <c r="Q35" s="25">
+        <f t="shared" si="9"/>
+        <v>-0.15789473684210525</v>
+      </c>
+      <c r="R35" s="25">
+        <f t="shared" si="9"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="S35" s="25">
+        <f t="shared" si="9"/>
+        <v>-0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="25">
+        <f t="shared" ref="A36:I36" si="10">(A28-A33)/A28</f>
+        <v>0.88372920410198041</v>
+      </c>
+      <c r="B36" s="25">
+        <f>(B28-B33)/B33</f>
+        <v>-0.76450530097817493</v>
+      </c>
+      <c r="C36" s="25">
+        <f t="shared" ref="C36:K36" si="11">(C28-C33)/C28</f>
+        <v>0.93322531184870894</v>
+      </c>
+      <c r="D36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.97351768511031789</v>
+      </c>
+      <c r="E36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.99320011363111216</v>
+      </c>
+      <c r="F36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.9860471961496976</v>
+      </c>
+      <c r="G36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.9911653293960988</v>
+      </c>
+      <c r="H36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.99733845227241069</v>
+      </c>
+      <c r="I36" s="25">
+        <f t="shared" si="11"/>
+        <v>0.90350283757740968</v>
+      </c>
+      <c r="K36" s="25">
+        <f t="shared" ref="K36:S36" si="12">(K28-K33)/K28</f>
+        <v>0.74603174603174605</v>
+      </c>
+      <c r="L36" s="25">
+        <f t="shared" si="12"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="M36" s="25">
+        <f t="shared" si="12"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N36" s="25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="25">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="P36" s="25">
+        <f t="shared" si="12"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="Q36" s="25">
+        <f t="shared" si="12"/>
+        <v>0.05</v>
+      </c>
+      <c r="R36" s="25">
+        <f t="shared" si="12"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S36" s="25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752C16C5-5FD2-094D-95FC-116C7455A54D}">
+  <dimension ref="A1:S36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>546</v>
+      </c>
+      <c r="L1" t="s">
+        <v>547</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1">
+        <v>0.1627915417861</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.163004864866027</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.163397238895157</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.22647190568743</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.1875279744466101</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.90802992516876502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="8">
+        <v>4.2777181796793601E-10</v>
+      </c>
+      <c r="B3" s="8">
+        <v>6.5489364865944894E-5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.0668355438247999E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3.2510050806212401</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.65236551144146704</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.57809733973746502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="8">
+        <v>4.8105963657008003E-13</v>
+      </c>
+      <c r="B4" s="8">
+        <v>4.8940391298990499E-5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4.8244618306214599E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.7395401577687202</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.53025580755296</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.0051845518137399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>550</v>
+      </c>
+      <c r="E6" t="s">
+        <v>541</v>
+      </c>
+      <c r="F6" t="s">
+        <v>543</v>
+      </c>
+      <c r="G6" t="s">
+        <v>540</v>
+      </c>
+      <c r="H6" t="s">
+        <v>542</v>
+      </c>
+      <c r="I6" t="s">
+        <v>544</v>
+      </c>
+      <c r="K6" t="s">
+        <v>548</v>
+      </c>
+      <c r="L6" t="s">
+        <v>549</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>550</v>
+      </c>
+      <c r="O6" t="s">
+        <v>541</v>
+      </c>
+      <c r="P6" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>540</v>
+      </c>
+      <c r="R6" t="s">
+        <v>542</v>
+      </c>
+      <c r="S6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1">
+        <v>0.16433567494509899</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="K7" s="35">
+        <v>3</v>
+      </c>
+      <c r="L7" s="35">
+        <v>1</v>
+      </c>
+      <c r="M7" s="35">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="8">
+        <v>2.3757225945439898E-3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3.0976997160051499E-3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.5480209484370899E-3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.32271951015683E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.8306499557828602E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.7412570846754201E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <v>6.8071527126928502E-2</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.20404667937588E-2</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.9302345445700999E-2</v>
+      </c>
+      <c r="K8" s="35">
+        <v>40</v>
+      </c>
+      <c r="L8" s="35">
+        <v>46</v>
+      </c>
+      <c r="M8" s="35">
+        <v>52</v>
+      </c>
+      <c r="N8">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>23</v>
+      </c>
+      <c r="P8">
+        <v>26</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="8">
+        <v>4.7331475979300796E-3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2.9309881882513202E-3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.21175623547081E-2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.15129113675343001</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.163455337405219</v>
+      </c>
+      <c r="F9" s="8">
+        <v>9.3943820904024405E-3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.109886658558011</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.102341799900144</v>
+      </c>
+      <c r="I9" s="8">
+        <v>5.07975385197068E-3</v>
+      </c>
+      <c r="K9" s="35">
+        <v>126</v>
+      </c>
+      <c r="L9" s="35">
+        <v>122</v>
+      </c>
+      <c r="M9" s="35">
+        <v>21</v>
+      </c>
+      <c r="N9">
+        <v>62</v>
+      </c>
+      <c r="O9">
+        <v>60</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>19</v>
+      </c>
+      <c r="R9">
+        <v>20</v>
+      </c>
+      <c r="S9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B11" t="s">
+        <v>552</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>550</v>
+      </c>
+      <c r="E11" t="s">
+        <v>541</v>
+      </c>
+      <c r="F11" t="s">
+        <v>543</v>
+      </c>
+      <c r="G11" t="s">
+        <v>540</v>
+      </c>
+      <c r="H11" t="s">
+        <v>542</v>
+      </c>
+      <c r="I11" t="s">
+        <v>544</v>
+      </c>
+      <c r="K11" t="s">
+        <v>551</v>
+      </c>
+      <c r="L11" t="s">
+        <v>552</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" t="s">
+        <v>550</v>
+      </c>
+      <c r="O11" t="s">
+        <v>541</v>
+      </c>
+      <c r="P11" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>540</v>
+      </c>
+      <c r="R11" t="s">
+        <v>542</v>
+      </c>
+      <c r="S11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="K12" s="35">
+        <v>1</v>
+      </c>
+      <c r="L12" s="35">
+        <v>1</v>
+      </c>
+      <c r="M12" s="35">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="8">
+        <v>1.4197286180969099E-3</v>
+      </c>
+      <c r="B13" s="8">
+        <v>7.3287569574531598E-4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>7.2370991824921495E-4</v>
+      </c>
+      <c r="D13" s="8">
+        <v>9.5783468942822704E-4</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8.4021001032963296E-4</v>
+      </c>
+      <c r="F13" s="8">
+        <v>7.8802477326822497E-4</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1.7878595396783E-3</v>
+      </c>
+      <c r="H13" s="8">
+        <v>5.5138462056070203E-4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.2563070577620199E-3</v>
+      </c>
+      <c r="K13" s="35">
+        <v>6</v>
+      </c>
+      <c r="L13" s="35">
+        <v>6</v>
+      </c>
+      <c r="M13" s="35">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>19</v>
+      </c>
+      <c r="O13">
+        <v>23</v>
+      </c>
+      <c r="P13">
+        <v>26</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="S13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="8">
+        <v>5.5032683831412999E-4</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1.65868576629446E-3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6.1599207400919698E-4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.2237493045387201E-3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1.03518773611466E-3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>9.8219722142567291E-4</v>
+      </c>
+      <c r="G14" s="8">
+        <v>5.4321302183346599E-4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>9.9085545725019399E-4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>9.0459487803606897E-4</v>
+      </c>
+      <c r="K14" s="35">
+        <v>32</v>
+      </c>
+      <c r="L14" s="35">
+        <v>10</v>
+      </c>
+      <c r="M14" s="35">
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>57</v>
+      </c>
+      <c r="O14">
+        <v>54</v>
+      </c>
+      <c r="P14">
+        <v>14</v>
+      </c>
+      <c r="Q14">
+        <v>20</v>
+      </c>
+      <c r="R14">
+        <v>20</v>
+      </c>
+      <c r="S14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="25">
+        <f>(A7-A12)/A7</f>
+        <v>4.5632663669316334E-3</v>
+      </c>
+      <c r="B15" s="25">
+        <f t="shared" ref="B15:I15" si="0">(B7-B12)/B7</f>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="C15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="D15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="E15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="G15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="H15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="I15" s="25">
+        <f t="shared" si="0"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="K15" s="25">
+        <f>(K7-K12)/K7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L15" s="25">
+        <f t="shared" ref="L15:S15" si="1">(L7-L12)/L7</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="25">
+        <f t="shared" ref="A16:I17" si="2">(A8-A13)/A8</f>
+        <v>0.40240134881176187</v>
+      </c>
+      <c r="B16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.76341293122806431</v>
+      </c>
+      <c r="C16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.53249345948458537</v>
+      </c>
+      <c r="D16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.77841849623190651</v>
+      </c>
+      <c r="E16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.78066124025213324</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.54743915748941974</v>
+      </c>
+      <c r="G16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.97373557469418015</v>
+      </c>
+      <c r="H16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.95420571062522985</v>
+      </c>
+      <c r="I16" s="25">
+        <f t="shared" si="2"/>
+        <v>0.93491427965082752</v>
+      </c>
+      <c r="K16" s="25">
+        <f t="shared" ref="K16:S17" si="3">(K8-K13)/K8</f>
+        <v>0.85</v>
+      </c>
+      <c r="L16" s="25">
+        <f t="shared" si="3"/>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="M16" s="25">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="N16" s="25">
+        <f t="shared" si="3"/>
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="O16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.375</v>
+      </c>
+      <c r="R16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="S16" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.88372920410198041</v>
+      </c>
+      <c r="B17" s="25">
+        <f>(B9-B14)/B14</f>
+        <v>0.76705452461873558</v>
+      </c>
+      <c r="C17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.94916534728869273</v>
+      </c>
+      <c r="D17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.99191129546119305</v>
+      </c>
+      <c r="E17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.99366684653711645</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.89544844866070405</v>
+      </c>
+      <c r="G17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.99505660624354419</v>
+      </c>
+      <c r="H17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.99031817440950831</v>
+      </c>
+      <c r="I17" s="25">
+        <f t="shared" si="2"/>
+        <v>0.82192151344397657</v>
+      </c>
+      <c r="K17" s="25">
+        <f t="shared" si="3"/>
+        <v>0.74603174603174605</v>
+      </c>
+      <c r="L17" s="25">
+        <f t="shared" si="3"/>
+        <v>0.91803278688524592</v>
+      </c>
+      <c r="M17" s="25">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N17" s="25">
+        <f t="shared" si="3"/>
+        <v>8.0645161290322578E-2</v>
+      </c>
+      <c r="O17" s="25">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="P17" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.4</v>
+      </c>
+      <c r="Q17" s="25">
+        <f t="shared" si="3"/>
+        <v>-5.2631578947368418E-2</v>
+      </c>
+      <c r="R17" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>546</v>
+      </c>
+      <c r="B20" t="s">
+        <v>547</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>546</v>
+      </c>
+      <c r="L20" t="s">
+        <v>547</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="36">
+        <v>0.05</v>
+      </c>
+      <c r="B21" s="36">
+        <v>4.93</v>
+      </c>
+      <c r="C21" s="36">
+        <v>2.63</v>
+      </c>
+      <c r="K21" s="36">
+        <v>15</v>
+      </c>
+      <c r="L21" s="36">
+        <v>1268</v>
+      </c>
+      <c r="M21" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="B22" s="36">
+        <v>48.81</v>
+      </c>
+      <c r="C22" s="36">
+        <v>10.93</v>
+      </c>
+      <c r="K22" s="36">
+        <v>24</v>
+      </c>
+      <c r="L22" s="36">
+        <v>3563</v>
+      </c>
+      <c r="M22" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23">
+        <v>0.11</v>
+      </c>
+      <c r="B23" s="8">
+        <v>94.54</v>
+      </c>
+      <c r="C23">
+        <v>34.71</v>
+      </c>
+      <c r="K23" s="35">
+        <v>8</v>
+      </c>
+      <c r="L23" s="35">
+        <v>3793</v>
+      </c>
+      <c r="M23" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>548</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>550</v>
+      </c>
+      <c r="E25" t="s">
+        <v>541</v>
+      </c>
+      <c r="F25" t="s">
+        <v>543</v>
+      </c>
+      <c r="G25" t="s">
+        <v>540</v>
+      </c>
+      <c r="H25" t="s">
+        <v>542</v>
+      </c>
+      <c r="I25" t="s">
+        <v>544</v>
+      </c>
+      <c r="K25" t="s">
+        <v>548</v>
+      </c>
+      <c r="L25" t="s">
+        <v>549</v>
+      </c>
+      <c r="M25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N25" t="s">
+        <v>550</v>
+      </c>
+      <c r="O25" t="s">
+        <v>541</v>
+      </c>
+      <c r="P25" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>540</v>
+      </c>
+      <c r="R25" t="s">
+        <v>542</v>
+      </c>
+      <c r="S25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="1">
+        <v>0.16433567494509899</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.16417865590338901</v>
+      </c>
+      <c r="K26" s="35">
+        <v>3</v>
+      </c>
+      <c r="L26" s="35">
+        <v>1</v>
+      </c>
+      <c r="M26" s="35">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="8">
+        <v>2.3757225945439898E-3</v>
+      </c>
+      <c r="B27" s="8">
+        <v>3.0976997160051499E-3</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.5480209484370899E-3</v>
+      </c>
+      <c r="D27" s="8">
+        <v>4.32271951015683E-3</v>
+      </c>
+      <c r="E27" s="8">
+        <v>3.8306499557828602E-3</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1.7412570846754201E-3</v>
+      </c>
+      <c r="G27" s="8">
+        <v>6.8071527126928502E-2</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1.20404667937588E-2</v>
+      </c>
+      <c r="I27" s="8">
+        <v>1.9302345445700999E-2</v>
+      </c>
+      <c r="K27" s="35">
+        <v>40</v>
+      </c>
+      <c r="L27" s="35">
+        <v>46</v>
+      </c>
+      <c r="M27" s="35">
+        <v>52</v>
+      </c>
+      <c r="N27">
+        <v>21</v>
+      </c>
+      <c r="O27">
+        <v>23</v>
+      </c>
+      <c r="P27">
+        <v>26</v>
+      </c>
+      <c r="Q27">
+        <v>8</v>
+      </c>
+      <c r="R27">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="8">
+        <v>4.7331475979300796E-3</v>
+      </c>
+      <c r="B28" s="8">
+        <v>3.9061170530529899E-4</v>
+      </c>
+      <c r="C28" s="8">
+        <v>9.2249337445582304E-3</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.15129113675343001</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.163455337405219</v>
+      </c>
+      <c r="F28" s="8">
+        <v>9.3943820904024405E-3</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0.109886658558011</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.102341799900144</v>
+      </c>
+      <c r="I28" s="8">
+        <v>5.07975385197068E-3</v>
+      </c>
+      <c r="K28" s="35">
+        <v>126</v>
+      </c>
+      <c r="L28" s="35">
+        <v>126</v>
+      </c>
+      <c r="M28" s="35">
+        <v>21</v>
+      </c>
+      <c r="N28">
+        <v>62</v>
+      </c>
+      <c r="O28">
+        <v>60</v>
+      </c>
+      <c r="P28">
+        <v>10</v>
+      </c>
+      <c r="Q28">
+        <v>19</v>
+      </c>
+      <c r="R28">
+        <v>20</v>
+      </c>
+      <c r="S28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>551</v>
+      </c>
+      <c r="B30" t="s">
+        <v>552</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>550</v>
+      </c>
+      <c r="E30" t="s">
+        <v>541</v>
+      </c>
+      <c r="F30" t="s">
+        <v>543</v>
+      </c>
+      <c r="G30" t="s">
+        <v>540</v>
+      </c>
+      <c r="H30" t="s">
+        <v>542</v>
+      </c>
+      <c r="I30" t="s">
+        <v>544</v>
+      </c>
+      <c r="K30" t="s">
+        <v>551</v>
+      </c>
+      <c r="L30" t="s">
+        <v>552</v>
+      </c>
+      <c r="M30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" t="s">
+        <v>550</v>
+      </c>
+      <c r="O30" t="s">
+        <v>541</v>
+      </c>
+      <c r="P30" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>540</v>
+      </c>
+      <c r="R30" t="s">
+        <v>542</v>
+      </c>
+      <c r="S30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.16358576748673501</v>
+      </c>
+      <c r="K31" s="35">
+        <v>1</v>
+      </c>
+      <c r="L31" s="35">
+        <v>1</v>
+      </c>
+      <c r="M31" s="35">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="8">
+        <v>1.4197286180969099E-3</v>
+      </c>
+      <c r="B32" s="8">
+        <v>7.3287569574531598E-4</v>
+      </c>
+      <c r="C32" s="8">
+        <v>7.2370991824921495E-4</v>
+      </c>
+      <c r="D32" s="8">
+        <v>9.5783468942822704E-4</v>
+      </c>
+      <c r="E32" s="8">
+        <v>8.4021001032963296E-4</v>
+      </c>
+      <c r="F32" s="8">
+        <v>7.8802477326822497E-4</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1.7878595396783E-3</v>
+      </c>
+      <c r="H32" s="8">
+        <v>5.5138462056070203E-4</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1.2563070577620199E-3</v>
+      </c>
+      <c r="K32" s="35">
+        <v>6</v>
+      </c>
+      <c r="L32" s="35">
+        <v>6</v>
+      </c>
+      <c r="M32" s="35">
+        <v>13</v>
+      </c>
+      <c r="N32">
+        <v>19</v>
+      </c>
+      <c r="O32">
+        <v>23</v>
+      </c>
+      <c r="P32">
+        <v>26</v>
+      </c>
+      <c r="Q32">
+        <v>11</v>
+      </c>
+      <c r="R32">
+        <v>8</v>
+      </c>
+      <c r="S32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="8">
+        <v>5.5032683831412999E-4</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1.65868576629446E-3</v>
+      </c>
+      <c r="C33" s="8">
+        <v>6.1599207400919698E-4</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1.2237493045387201E-3</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1.03518773611466E-3</v>
+      </c>
+      <c r="F33" s="8">
+        <v>9.8219722142567291E-4</v>
+      </c>
+      <c r="G33" s="8">
+        <v>5.4321302183346599E-4</v>
+      </c>
+      <c r="H33" s="8">
+        <v>9.9085545725019399E-4</v>
+      </c>
+      <c r="I33" s="8">
+        <v>9.0459487803606897E-4</v>
+      </c>
+      <c r="K33" s="35">
+        <v>32</v>
+      </c>
+      <c r="L33" s="35">
+        <v>10</v>
+      </c>
+      <c r="M33" s="35">
+        <v>7</v>
+      </c>
+      <c r="N33">
+        <v>57</v>
+      </c>
+      <c r="O33">
+        <v>54</v>
+      </c>
+      <c r="P33">
+        <v>14</v>
+      </c>
+      <c r="Q33">
+        <v>20</v>
+      </c>
+      <c r="R33">
+        <v>20</v>
+      </c>
+      <c r="S33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="25">
+        <f>(A26-A31)/A26</f>
+        <v>4.5632663669316334E-3</v>
+      </c>
+      <c r="B34" s="25">
+        <f t="shared" ref="B34:I34" si="4">(B26-B31)/B26</f>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="C34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="D34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="E34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="F34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="G34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="H34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="I34" s="25">
+        <f t="shared" si="4"/>
+        <v>3.6112393136102181E-3</v>
+      </c>
+      <c r="K34" s="25">
+        <f>(K26-K31)/K26</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L34" s="25">
+        <f t="shared" ref="L34:S34" si="5">(L26-L31)/L26</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="25">
+        <f t="shared" ref="A35:I36" si="6">(A27-A32)/A27</f>
+        <v>0.40240134881176187</v>
+      </c>
+      <c r="B35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.76341293122806431</v>
+      </c>
+      <c r="C35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.53249345948458537</v>
+      </c>
+      <c r="D35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.77841849623190651</v>
+      </c>
+      <c r="E35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.78066124025213324</v>
+      </c>
+      <c r="F35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.54743915748941974</v>
+      </c>
+      <c r="G35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.97373557469418015</v>
+      </c>
+      <c r="H35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.95420571062522985</v>
+      </c>
+      <c r="I35" s="25">
+        <f t="shared" si="6"/>
+        <v>0.93491427965082752</v>
+      </c>
+      <c r="K35" s="25">
+        <f t="shared" ref="K35:S36" si="7">(K27-K32)/K27</f>
+        <v>0.85</v>
+      </c>
+      <c r="L35" s="25">
+        <f t="shared" si="7"/>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="M35" s="25">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="N35" s="25">
+        <f t="shared" si="7"/>
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="O35" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="25">
+        <f t="shared" si="7"/>
+        <v>-0.375</v>
+      </c>
+      <c r="R35" s="25">
+        <f t="shared" si="7"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="S35" s="25">
+        <f t="shared" si="7"/>
+        <v>-0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.88372920410198041</v>
+      </c>
+      <c r="B36" s="25">
+        <f>(B28-B33)/B33</f>
+        <v>-0.76450530097817493</v>
+      </c>
+      <c r="C36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.93322531184870894</v>
+      </c>
+      <c r="D36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.99191129546119305</v>
+      </c>
+      <c r="E36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.99366684653711645</v>
+      </c>
+      <c r="F36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.89544844866070405</v>
+      </c>
+      <c r="G36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.99505660624354419</v>
+      </c>
+      <c r="H36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.99031817440950831</v>
+      </c>
+      <c r="I36" s="25">
+        <f t="shared" si="6"/>
+        <v>0.82192151344397657</v>
+      </c>
+      <c r="K36" s="25">
+        <f t="shared" si="7"/>
+        <v>0.74603174603174605</v>
+      </c>
+      <c r="L36" s="25">
+        <f t="shared" si="7"/>
+        <v>0.92063492063492058</v>
+      </c>
+      <c r="M36" s="25">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N36" s="25">
+        <f t="shared" si="7"/>
+        <v>8.0645161290322578E-2</v>
+      </c>
+      <c r="O36" s="25">
+        <f t="shared" si="7"/>
+        <v>0.1</v>
+      </c>
+      <c r="P36" s="25">
+        <f t="shared" si="7"/>
+        <v>-0.4</v>
+      </c>
+      <c r="Q36" s="25">
+        <f t="shared" si="7"/>
+        <v>-5.2631578947368418E-2</v>
+      </c>
+      <c r="R36" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -17589,7 +20660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE872A85-4DE9-F745-9374-575870CFA036}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -25839,7 +28910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13319D89-0C0E-B74C-8733-68AAE68AA77A}">
   <dimension ref="B1:N159"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
+    <sheetView topLeftCell="A146" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>